<commit_message>
change the serial numbers
last time we deleted some lines but forgot to change the serial numbers
</commit_message>
<xml_diff>
--- a/testing/testcases.xlsx
+++ b/testing/testcases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\project-g5t4\testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chen yibing\Documents\GitHub\project-g5t4\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{290671AE-F523-4F50-923A-C4F4BF99F98E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CCB2A1B-ACB1-4BC2-9837-66995B5A6E4B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F747292D-6CBE-43A0-AF24-F2F7C25CEB64}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="14400" windowHeight="7374" xr2:uid="{F747292D-6CBE-43A0-AF24-F2F7C25CEB64}"/>
   </bookViews>
   <sheets>
     <sheet name="Manual Testing" sheetId="1" r:id="rId1"/>
@@ -1124,20 +1124,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E23735C8-ED28-4D29-AF91-DF94B0DE9482}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="60" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7890625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="3" width="15.6328125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18.36328125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="21.81640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="26.81640625" style="2" customWidth="1"/>
-    <col min="7" max="9" width="15.6328125" style="2" customWidth="1"/>
+    <col min="1" max="3" width="15.62890625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.3671875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="21.7890625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="26.7890625" style="2" customWidth="1"/>
+    <col min="7" max="9" width="15.62890625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1166,7 +1166,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="36.9" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1195,7 +1195,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1224,7 +1224,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1253,7 +1253,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="50" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1311,7 +1311,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1340,7 +1340,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="36.9" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1369,7 +1369,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1398,7 +1398,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="145" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1427,9 +1427,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="145" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="3">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>20</v>
@@ -1456,9 +1456,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="145" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="3">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>21</v>
@@ -1485,9 +1485,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="145" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="3">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>22</v>
@@ -1514,9 +1514,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="174" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="3">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>23</v>
@@ -1543,9 +1543,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="145" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="3">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>24</v>
@@ -1572,9 +1572,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="145" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="3">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>25</v>
@@ -1601,9 +1601,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="145" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="3">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>26</v>
@@ -1630,9 +1630,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="145" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="3">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>27</v>
@@ -1659,9 +1659,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="145" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="3">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>28</v>
@@ -1688,9 +1688,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="145" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="3">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>29</v>
@@ -1717,9 +1717,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="145" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="3">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>30</v>
@@ -1746,9 +1746,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="145" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="3">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>31</v>
@@ -1775,9 +1775,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="145" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="3">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>32</v>
@@ -1804,9 +1804,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="3">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>33</v>
@@ -1833,9 +1833,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="145" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="3">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>34</v>
@@ -1862,9 +1862,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="145" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="3">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>35</v>
@@ -1891,9 +1891,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="145" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="3">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>36</v>
@@ -1920,9 +1920,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="3">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>37</v>
@@ -1949,9 +1949,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="3">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>38</v>
@@ -1978,9 +1978,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="3">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>39</v>
@@ -2007,9 +2007,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="3">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>40</v>
@@ -2036,9 +2036,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="3">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>41</v>
@@ -2065,9 +2065,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="3">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>42</v>
@@ -2094,9 +2094,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" ht="36.9" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="3">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>43</v>
@@ -2120,9 +2120,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="145" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="3">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>44</v>
@@ -2149,9 +2149,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="145" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="3">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>45</v>
@@ -2178,9 +2178,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A37" s="2">
-        <v>39</v>
+    <row r="37" spans="1:9" ht="144" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="3">
+        <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>114</v>

</xml_diff>

<commit_message>
Updated Testcases with Clearing test cases
Updated Testcases with Clearing test cases
</commit_message>
<xml_diff>
--- a/testing/testcases.xlsx
+++ b/testing/testcases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Serene\Documents\GitHub\project-g5t4\testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lai See Hoe\Documents\GitHub\project-g5t4\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88EFF09-6F43-44EA-BF56-C7763930D2B1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65505E83-1FC2-4A04-8D51-9E14D710B397}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F747292D-6CBE-43A0-AF24-F2F7C25CEB64}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="200">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -779,6 +779,24 @@
   </si>
   <si>
     <t>Bid placed successfully! Amount left: $190</t>
+  </si>
+  <si>
+    <t>Clearing of Bid by student who placed $10</t>
+  </si>
+  <si>
+    <t>Admin logged in and presses Clear Round 1</t>
+  </si>
+  <si>
+    <t>Student bids for IS100 with $10 and admin clears it after</t>
+  </si>
+  <si>
+    <t>Student: amy.ng.2009
+Course: IS100
+Section: S1
+Amount: $10</t>
+  </si>
+  <si>
+    <t>amy.ng.2009 in student table will have $190 instead of $200</t>
   </si>
 </sst>
 </file>
@@ -1168,10 +1186,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E23735C8-ED28-4D29-AF91-DF94B0DE9482}">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="60" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="60" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42:F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2340,6 +2358,35 @@
         <v>9</v>
       </c>
     </row>
+    <row r="41" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="A41" s="2">
+        <v>40</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated Testcases to reflect testing for round 1 and 2 clearing
Updated Testcases to reflect testing for round 1 and 2 clearing

Co-Authored-By: tohjaslyn <tohjaslyn@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/testing/testcases.xlsx
+++ b/testing/testcases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Serene\Documents\GitHub\project-g5t4\testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lai See Hoe\Documents\GitHub\project-g5t4\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A569D957-DB17-41BF-929B-30D876195514}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ECB38CD-51A9-4F2E-B611-D0954366B152}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F747292D-6CBE-43A0-AF24-F2F7C25CEB64}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="280">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -1014,6 +1014,48 @@
   </si>
   <si>
     <t>Fail</t>
+  </si>
+  <si>
+    <t>Only maggie.ng.2009 and nielson.ng.2019 added to section student table</t>
+  </si>
+  <si>
+    <t>Admin clears round 1</t>
+  </si>
+  <si>
+    <t>Validate clearing logic</t>
+  </si>
+  <si>
+    <t>bidding table must have bids</t>
+  </si>
+  <si>
+    <t>Admin presses clear round 1 button on admin_homepage.php</t>
+  </si>
+  <si>
+    <t>Admin clears round 2</t>
+  </si>
+  <si>
+    <t>Admin presses clear round 2 button on admin_homepage.php</t>
+  </si>
+  <si>
+    <t>Sampledata.zip</t>
+  </si>
+  <si>
+    <t>R1 clearing test cases.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">only calvin.ng.2009
+dawn.ng.2009
+eddy.ng.2009
+fred.ng.2009
+harry.ng.2009
+ian.ng.2009
+larry.ng.2009
+maggie.ng.2009
+neilson.ng.2009
+olivia.ng.2009 in Section student table </t>
+  </si>
+  <si>
+    <t xml:space="preserve">maggie.ng.2009 and nielson.ng.2019 have the wrong bid values in the bid table resulting in them not appearing in section student table </t>
   </si>
 </sst>
 </file>
@@ -1419,10 +1461,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E23735C8-ED28-4D29-AF91-DF94B0DE9482}">
-  <dimension ref="A1:I59"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="67" workbookViewId="0">
-      <selection activeCell="I60" sqref="I60"/>
+    <sheetView tabSelected="1" zoomScale="67" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I61" sqref="I61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3142,6 +3185,64 @@
         <v>9</v>
       </c>
     </row>
+    <row r="60" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+      <c r="A60" s="2">
+        <v>59</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="188.5" x14ac:dyDescent="0.35">
+      <c r="A61" s="2">
+        <v>60</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="I61" s="2" t="s">
+        <v>268</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated testcases.xlsx to contain more testcases for drop section, round 2 bidding and view bidding status
Updated testcases.xlsx to contain more testcases for drop section, round 2 bidding and view bidding status
</commit_message>
<xml_diff>
--- a/testing/testcases.xlsx
+++ b/testing/testcases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lai See Hoe\Downloads\Telegram Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lai See Hoe\Documents\GitHub\project-g5t4\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA7521C-1ADA-46DD-B2B9-6D1062EC9697}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D3B289A-5223-4F0D-A460-D841A41B14BC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{F747292D-6CBE-43A0-AF24-F2F7C25CEB64}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="844" firstSheet="1" activeTab="1" xr2:uid="{F747292D-6CBE-43A0-AF24-F2F7C25CEB64}"/>
   </bookViews>
   <sheets>
     <sheet name="JSON testing" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1300" uniqueCount="754">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1420" uniqueCount="794">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -6387,6 +6387,152 @@
 Section: S1
 Bid Amount: 11.00
 Status: Fail</t>
+  </si>
+  <si>
+    <t>View bidding status during round 1 active</t>
+  </si>
+  <si>
+    <t>Bidded for IS003</t>
+  </si>
+  <si>
+    <t>Userid: amy
+Course: IS003
+Section: S1
+Bid Amount: 10.00</t>
+  </si>
+  <si>
+    <t>View bidding status during round 1 inactive</t>
+  </si>
+  <si>
+    <t>Error: Unable to drop any section now</t>
+  </si>
+  <si>
+    <t>Clear round 1</t>
+  </si>
+  <si>
+    <t>Drop section in Round 1 inactive</t>
+  </si>
+  <si>
+    <t>Drop section</t>
+  </si>
+  <si>
+    <t>View bidding status during round 2 active</t>
+  </si>
+  <si>
+    <t>Course: IS003
+Section: 2</t>
+  </si>
+  <si>
+    <t>Student checks vacancy and min bid in round 2</t>
+  </si>
+  <si>
+    <t>Vacancy = 4</t>
+  </si>
+  <si>
+    <t>Userid: amy
+Course: IS003
+Section: S2
+Bid Amount: 10.00</t>
+  </si>
+  <si>
+    <t>Course: IS003
+Section: S2
+Bid Amount: 10.00
+Status: Pending</t>
+  </si>
+  <si>
+    <t>Course: IS003
+Section: S2
+Bid Amount: 10.00
+Status: Success</t>
+  </si>
+  <si>
+    <t>Drop Section in round 2 Active</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>Student bids for a course already enrolled into</t>
+  </si>
+  <si>
+    <t>Student selects IS003</t>
+  </si>
+  <si>
+    <t>Student bids on IS003 section 1</t>
+  </si>
+  <si>
+    <t>Course: IS003
+Section: 1</t>
+  </si>
+  <si>
+    <t>Student bids on IS003 section 1 while he is enrolled in section 2</t>
+  </si>
+  <si>
+    <t>Course Enrolled</t>
+  </si>
+  <si>
+    <t>Vacancy = 3
+min bid = 10.00</t>
+  </si>
+  <si>
+    <t>Student selects a course to check for vacancy while enrolled in IS003 section 2</t>
+  </si>
+  <si>
+    <t>Student attempts to bid without enough money and with 5 mods enrolled already</t>
+  </si>
+  <si>
+    <t>user: benny
+Course: IS003
+Section: 1
+Amount: 10.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insufficient e$
+section limit reached
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Student Bids with enough money </t>
+  </si>
+  <si>
+    <t>Success! Amount left: 14.97</t>
+  </si>
+  <si>
+    <t>View bidding status for round 2</t>
+  </si>
+  <si>
+    <t>Student bids for IS003 section 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3rd Student bids for IS003 section 1 where 2 students have bidded $10.00 </t>
+  </si>
+  <si>
+    <t>Course: IS003
+Section: S2
+Bid Amount: 10.00
+Status: Fail</t>
+  </si>
+  <si>
+    <t>Student checks vacancy in round 2 after someone drops the section from that section</t>
+  </si>
+  <si>
+    <t>View bidding status during round 2 inactive</t>
+  </si>
+  <si>
+    <t>View Bid status for a failed bid</t>
+  </si>
+  <si>
+    <t>View Bid status for a Successful bid</t>
+  </si>
+  <si>
+    <t>Userid: Charlie
+Course: IS003
+Section: S1
+Bid Amount: 11.00</t>
+  </si>
+  <si>
+    <t>Drop Section in round 2 inactive</t>
   </si>
 </sst>
 </file>
@@ -10115,8 +10261,8 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10166,127 +10312,241 @@
       </c>
     </row>
     <row r="2" spans="1:11" s="6" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A2" s="6">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="2" t="s">
         <v>734</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="2" t="s">
         <v>733</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="2" t="s">
         <v>724</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="2" t="s">
         <v>736</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="2" t="s">
         <v>726</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="2" t="s">
         <v>735</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="2" t="s">
         <v>735</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="6" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A3" s="6">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="2" t="s">
         <v>737</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="2" t="s">
         <v>733</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="2" t="s">
         <v>724</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="2" t="s">
         <v>736</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="2" t="s">
         <v>726</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="2" t="s">
         <v>735</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="2" t="s">
         <v>735</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="6" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="6">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="2" t="s">
         <v>739</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="2" t="s">
         <v>733</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="2" t="s">
         <v>727</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="2" t="s">
         <v>736</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="2" t="s">
         <v>726</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="2" t="s">
         <v>738</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="2" t="s">
         <v>738</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="6" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A5" s="6">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="2" t="s">
         <v>740</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="2" t="s">
         <v>733</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="2" t="s">
         <v>727</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="2" t="s">
         <v>736</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="2" t="s">
         <v>741</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="2" t="s">
         <v>735</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="2" t="s">
         <v>735</v>
       </c>
-      <c r="I5" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35"/>
+      <c r="I5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="6" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>760</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>761</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>736</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>758</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>758</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="6" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>769</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>761</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>736</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>770</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>770</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="6" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>793</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>761</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>736</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>792</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>758</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>758</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+    </row>
     <row r="12" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="13" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="14" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35"/>
@@ -10302,7 +10562,7 @@
   <sheetViews>
     <sheetView zoomScale="77" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10484,11 +10744,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{038D9871-6BF2-4210-AB19-5595569BDB87}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView zoomScale="84" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I7" sqref="I7"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10754,6 +11014,209 @@
       <c r="J8" s="11"/>
       <c r="K8" s="11"/>
     </row>
+    <row r="9" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="11">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>754</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>723</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>755</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>725</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>756</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>767</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>767</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="11">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>757</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>723</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>759</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>725</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>756</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>767</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>767</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>762</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>723</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>479</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>725</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>756</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>768</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>768</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="11">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>762</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>784</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>785</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>725</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>756</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>768</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>768</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="11">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>762</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>784</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>786</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>725</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>756</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>787</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>768</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="11">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>784</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>790</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>725</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>756</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>787</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>787</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="11">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>784</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>791</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>725</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>792</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>768</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>768</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -10765,8 +11228,8 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView zoomScale="72" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10986,11 +11449,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D48F8994-0480-456C-9C73-8DEBC1CF05E8}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView zoomScale="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11684,6 +12147,151 @@
       </c>
       <c r="J21" s="2"/>
       <c r="K21" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="2">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>778</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>763</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>777</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>777</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="2">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>771</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>772</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>775</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>774</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>776</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>776</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>772</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>763</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>765</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>765</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="2">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>772</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>773</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>781</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>781</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A26" s="2">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>782</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>772</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>773</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>783</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>783</v>
+      </c>
+      <c r="I26" s="2" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated testcase. xslx regarding bootstrap validation
Updated testcase. xslx regarding bootstrap validation
</commit_message>
<xml_diff>
--- a/testing/testcases.xlsx
+++ b/testing/testcases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lai See Hoe\Documents\GitHub\project-g5t4\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D3B289A-5223-4F0D-A460-D841A41B14BC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B896A8-DF46-429E-8462-D510ACDD6E10}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="844" firstSheet="1" activeTab="1" xr2:uid="{F747292D-6CBE-43A0-AF24-F2F7C25CEB64}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="844" firstSheet="4" activeTab="7" xr2:uid="{F747292D-6CBE-43A0-AF24-F2F7C25CEB64}"/>
   </bookViews>
   <sheets>
     <sheet name="JSON testing" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1420" uniqueCount="794">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1428" uniqueCount="800">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -6533,6 +6533,49 @@
   </si>
   <si>
     <t>Drop Section in round 2 inactive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administrator uploads edollartest.zip </t>
+  </si>
+  <si>
+    <t>Validate e dollars for student and Bid</t>
+  </si>
+  <si>
+    <t>student and bid csv with 1 d.p. values instead of 2 d.p.</t>
+  </si>
+  <si>
+    <t>testedollars.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Bootstrap Results
+Status	error
+bid.csv	9
+course.csv	24
+course_completed.csv	3
+prerequisite.csv	8
+section.csv	35
+student.csv	14
+bid.csv	Line: 2	invalid amount
+bid.csv	Line: 5	course completed
+bid.csv	Line: 13	incomplete prerequisites
+course_completed.csv	Line: 2	invalid userid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Bootstrap Results
+Status	error
+bid.csv	9
+course.csv	24
+course_completed.csv	3
+prerequisite.csv	8
+section.csv	35
+student.csv	14
+bid.csv	Line: 2	invalid amount
+bid.csv	Line: 5	course completed
+bid.csv	Line: 13	incomplete prerequisites
+course_completed.csv	Line: 2	invalid userid
+student.csv	Line: 2	invalid e-dollar</t>
   </si>
 </sst>
 </file>
@@ -6982,9 +7025,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E622AFF1-7BAD-40A3-9A13-C74C8BBD0E61}">
   <dimension ref="A1:K165"/>
   <sheetViews>
-    <sheetView zoomScale="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+    <sheetView topLeftCell="B1" zoomScale="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10260,7 +10303,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A3F21E7-F613-4F5C-A232-03BE67008ACA}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I9" sqref="I9"/>
     </sheetView>
@@ -12617,10 +12660,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77076042-100F-4228-9C99-338194152E9B}">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView zoomScale="71" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13563,7 +13606,37 @@
         <v>8</v>
       </c>
     </row>
+    <row r="30" spans="1:11" ht="348" x14ac:dyDescent="0.35">
+      <c r="A30" s="3">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>794</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>795</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>796</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>797</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>798</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>799</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated testcases for Iter1 Json authenticate
Updated testcases for Iter1 Json authenticate
</commit_message>
<xml_diff>
--- a/testing/testcases.xlsx
+++ b/testing/testcases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lai See Hoe\Documents\GitHub\project-g5t4\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA89F565-EB1E-45A7-9202-73BD1A1E4AD4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E378ABBE-D14D-4631-8165-4D607CB2B059}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="844" firstSheet="14" activeTab="17" xr2:uid="{F747292D-6CBE-43A0-AF24-F2F7C25CEB64}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="844" firstSheet="6" activeTab="9" xr2:uid="{F747292D-6CBE-43A0-AF24-F2F7C25CEB64}"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 3 - JSON - BidDump" sheetId="20" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2677" uniqueCount="841">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2677" uniqueCount="844">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -6704,6 +6704,31 @@
   </si>
   <si>
     <t xml:space="preserve">Pass/Fail 13/11/19 </t>
+  </si>
+  <si>
+    <t>{ 
+"status": "error", 
+"messages": [ 
+"blank username" 
+] 
+}</t>
+  </si>
+  <si>
+    <t>{ 
+"status": "error", 
+"messages": [ 
+"blank password" 
+] 
+}</t>
+  </si>
+  <si>
+    <t>{ 
+"status": "error", 
+"messages": [ 
+"blank username", 
+"blank password" 
+] 
+}</t>
   </si>
 </sst>
 </file>
@@ -6845,7 +6870,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -6977,6 +7002,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7501,11 +7529,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01360F1A-846B-44B4-BA3B-EAE40848B114}">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="6" max="6" width="8.7265625" customWidth="1"/>
+    <col min="7" max="7" width="17.81640625" customWidth="1"/>
+    <col min="8" max="8" width="22.08984375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" s="28" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
@@ -7542,7 +7575,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="338.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="176" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -7571,7 +7604,7 @@
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
     </row>
-    <row r="3" spans="1:11" ht="138.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="101" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -7600,7 +7633,7 @@
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
     </row>
-    <row r="4" spans="1:11" ht="138.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="88.5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -7620,7 +7653,7 @@
         <v>294</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>295</v>
+        <v>842</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>295</v>
@@ -7629,7 +7662,7 @@
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="1:11" ht="138.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="88.5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -7649,7 +7682,7 @@
         <v>298</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>299</v>
+        <v>841</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>299</v>
@@ -7658,7 +7691,7 @@
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
     </row>
-    <row r="6" spans="1:11" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -7678,7 +7711,7 @@
         <v>302</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>303</v>
+        <v>843</v>
       </c>
       <c r="H6" s="6" t="s">
         <v>303</v>
@@ -7687,7 +7720,7 @@
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
     </row>
-    <row r="7" spans="1:11" ht="138.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="101" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -7745,7 +7778,7 @@
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
     </row>
-    <row r="9" spans="1:11" ht="338.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" ht="176" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -12525,7 +12558,7 @@
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView zoomScale="72" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="N1" sqref="N1:O1"/>
     </sheetView>
   </sheetViews>
@@ -12881,7 +12914,7 @@
   <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="N1" sqref="N1:O1"/>
     </sheetView>
   </sheetViews>
@@ -14582,9 +14615,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77076042-100F-4228-9C99-338194152E9B}">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="55" zoomScaleNormal="40" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P2" sqref="P2:Q29"/>
+    <sheetView topLeftCell="C1" zoomScale="55" zoomScaleNormal="40" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16182,7 +16215,7 @@
   <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView zoomScale="87" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
@@ -17106,8 +17139,8 @@
   <dimension ref="A1:Z30"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1:M1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6328125" defaultRowHeight="50" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -18260,11 +18293,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB7AA43-4AE1-4D26-A97B-9F9B33DC61B2}">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="10.36328125" customWidth="1"/>
+    <col min="7" max="7" width="18.6328125" customWidth="1"/>
+    <col min="8" max="8" width="17.54296875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -18301,208 +18339,208 @@
         <v>274</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="409.6" x14ac:dyDescent="0.35">
-      <c r="A2" s="6">
+    <row r="2" spans="1:11" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="48">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="48" t="s">
         <v>320</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="48" t="s">
         <v>321</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="48" t="s">
         <v>322</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="48" t="s">
         <v>323</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="48" t="s">
         <v>324</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="48" t="s">
         <v>656</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="48" t="s">
         <v>656</v>
       </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-    </row>
-    <row r="3" spans="1:11" ht="409.6" x14ac:dyDescent="0.35">
-      <c r="A3" s="6">
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+    </row>
+    <row r="3" spans="1:11" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="48">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="48" t="s">
         <v>320</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="48" t="s">
         <v>326</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="48" t="s">
         <v>322</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="48" t="s">
         <v>327</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="48" t="s">
         <v>328</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="48" t="s">
         <v>657</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="48" t="s">
         <v>657</v>
       </c>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-    </row>
-    <row r="4" spans="1:11" ht="409.6" x14ac:dyDescent="0.35">
-      <c r="A4">
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
+    </row>
+    <row r="4" spans="1:11" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="8">
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="48" t="s">
         <v>320</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="48" t="s">
         <v>330</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="48" t="s">
         <v>322</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="48" t="s">
         <v>331</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="48" t="s">
         <v>332</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="48" t="s">
         <v>658</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="48" t="s">
         <v>658</v>
       </c>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-    </row>
-    <row r="5" spans="1:11" ht="409.6" x14ac:dyDescent="0.35">
-      <c r="A5">
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+    </row>
+    <row r="5" spans="1:11" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="8">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="48" t="s">
         <v>320</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="48" t="s">
         <v>334</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="48" t="s">
         <v>322</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="48" t="s">
         <v>335</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="48" t="s">
         <v>336</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="48" t="s">
         <v>659</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="48" t="s">
         <v>659</v>
       </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-    </row>
-    <row r="6" spans="1:11" ht="409.6" x14ac:dyDescent="0.35">
-      <c r="A6">
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="48"/>
+    </row>
+    <row r="6" spans="1:11" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="8">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="48" t="s">
         <v>320</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="48" t="s">
         <v>338</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="48" t="s">
         <v>322</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="48" t="s">
         <v>339</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="48" t="s">
         <v>340</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="48" t="s">
         <v>659</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="48" t="s">
         <v>660</v>
       </c>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-    </row>
-    <row r="7" spans="1:11" ht="409.6" x14ac:dyDescent="0.35">
-      <c r="A7">
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="48"/>
+    </row>
+    <row r="7" spans="1:11" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="8">
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="48" t="s">
         <v>320</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="48" t="s">
         <v>342</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="48" t="s">
         <v>322</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="48" t="s">
         <v>343</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="48" t="s">
         <v>344</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="48" t="s">
         <v>661</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="48" t="s">
         <v>661</v>
       </c>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-    </row>
-    <row r="8" spans="1:11" ht="409.6" x14ac:dyDescent="0.35">
-      <c r="A8">
+      <c r="I7" s="48"/>
+      <c r="J7" s="48"/>
+      <c r="K7" s="48"/>
+    </row>
+    <row r="8" spans="1:11" ht="325" x14ac:dyDescent="0.35">
+      <c r="A8" s="8">
         <v>7</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="48" t="s">
         <v>320</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="48" t="s">
         <v>346</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="48" t="s">
         <v>322</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="48" t="s">
         <v>347</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="48" t="s">
         <v>348</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="48" t="s">
         <v>662</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="48" t="s">
         <v>663</v>
       </c>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
+      <c r="I8" s="48"/>
+      <c r="J8" s="48"/>
+      <c r="K8" s="48"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update TestCases for Json Authenticate
update TestCases for Json Authenticate
</commit_message>
<xml_diff>
--- a/testing/testcases.xlsx
+++ b/testing/testcases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lai See Hoe\Documents\GitHub\project-g5t4\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E378ABBE-D14D-4631-8165-4D607CB2B059}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03517EE4-2488-43D1-B714-DA0ADA95623E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="844" firstSheet="6" activeTab="9" xr2:uid="{F747292D-6CBE-43A0-AF24-F2F7C25CEB64}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2677" uniqueCount="844">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2701" uniqueCount="848">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -6729,6 +6729,18 @@
 "blank password" 
 ] 
 }</t>
+  </si>
+  <si>
+    <t>Fal</t>
+  </si>
+  <si>
+    <t>Result 1</t>
+  </si>
+  <si>
+    <t>Pass/ Fail</t>
+  </si>
+  <si>
+    <t>Pass/Fail</t>
   </si>
 </sst>
 </file>
@@ -7529,8 +7541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01360F1A-846B-44B4-BA3B-EAE40848B114}">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7538,6 +7550,8 @@
     <col min="6" max="6" width="8.7265625" customWidth="1"/>
     <col min="7" max="7" width="17.81640625" customWidth="1"/>
     <col min="8" max="8" width="22.08984375" customWidth="1"/>
+    <col min="9" max="9" width="11.81640625" customWidth="1"/>
+    <col min="10" max="10" width="16.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="28" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7563,16 +7577,16 @@
         <v>6</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>7</v>
+        <v>845</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>272</v>
+        <v>846</v>
       </c>
       <c r="J1" s="15" t="s">
         <v>273</v>
       </c>
       <c r="K1" s="15" t="s">
-        <v>274</v>
+        <v>847</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="176" x14ac:dyDescent="0.35">
@@ -7600,9 +7614,15 @@
       <c r="H2" s="6" t="s">
         <v>655</v>
       </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
+      <c r="I2" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="K2" s="48" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" spans="1:11" ht="101" x14ac:dyDescent="0.35">
       <c r="A3">
@@ -7629,9 +7649,15 @@
       <c r="H3" s="6" t="s">
         <v>291</v>
       </c>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
+      <c r="I3" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="K3" s="48" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="1:11" ht="88.5" x14ac:dyDescent="0.35">
       <c r="A4">
@@ -7658,9 +7684,15 @@
       <c r="H4" s="6" t="s">
         <v>295</v>
       </c>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
+      <c r="I4" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>842</v>
+      </c>
+      <c r="K4" s="48" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="1:11" ht="88.5" x14ac:dyDescent="0.35">
       <c r="A5">
@@ -7687,9 +7719,15 @@
       <c r="H5" s="6" t="s">
         <v>299</v>
       </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
+      <c r="I5" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>841</v>
+      </c>
+      <c r="K5" s="48" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="6" spans="1:11" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A6">
@@ -7716,9 +7754,15 @@
       <c r="H6" s="6" t="s">
         <v>303</v>
       </c>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
+      <c r="I6" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>843</v>
+      </c>
+      <c r="K6" s="48" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" spans="1:11" ht="101" x14ac:dyDescent="0.35">
       <c r="A7">
@@ -7745,11 +7789,17 @@
       <c r="H7" s="6" t="s">
         <v>291</v>
       </c>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-    </row>
-    <row r="8" spans="1:11" ht="138.5" x14ac:dyDescent="0.35">
+      <c r="I7" s="48" t="s">
+        <v>844</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="K7" s="48" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -7774,9 +7824,15 @@
       <c r="H8" s="6" t="s">
         <v>291</v>
       </c>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
+      <c r="I8" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="K8" s="48" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="9" spans="1:11" ht="176" x14ac:dyDescent="0.35">
       <c r="A9">
@@ -7803,9 +7859,15 @@
       <c r="H9" s="6" t="s">
         <v>318</v>
       </c>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
+      <c r="I9" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="K9" s="48" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated testcases.xlsx to reflect latest test cases on update bid for Json
Updated testcases.xlsx to reflect latest test cases on update bid for Json
</commit_message>
<xml_diff>
--- a/testing/testcases.xlsx
+++ b/testing/testcases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lai See Hoe\Documents\GitHub\project-g5t4\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03517EE4-2488-43D1-B714-DA0ADA95623E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B93868-E388-4DCE-AE5D-9317A2378B4A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="844" firstSheet="6" activeTab="9" xr2:uid="{F747292D-6CBE-43A0-AF24-F2F7C25CEB64}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="844" firstSheet="4" activeTab="5" xr2:uid="{F747292D-6CBE-43A0-AF24-F2F7C25CEB64}"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 3 - JSON - BidDump" sheetId="20" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2701" uniqueCount="848">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2769" uniqueCount="848">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -6882,7 +6882,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -7017,6 +7017,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7541,8 +7544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01360F1A-846B-44B4-BA3B-EAE40848B114}">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7582,10 +7585,10 @@
       <c r="I1" s="13" t="s">
         <v>846</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="J1" s="13" t="s">
         <v>273</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="K1" s="13" t="s">
         <v>847</v>
       </c>
     </row>
@@ -14678,8 +14681,8 @@
   <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="55" zoomScaleNormal="40" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J17" sqref="J17"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N1" sqref="N1:Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17200,9 +17203,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5170428E-8DD4-4128-8426-F6B56272B186}">
   <dimension ref="A1:Z30"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
+      <selection pane="bottomLeft" activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6328125" defaultRowHeight="50" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -17212,7 +17215,9 @@
     <col min="6" max="6" width="17" style="24" customWidth="1"/>
     <col min="7" max="7" width="18" style="24" customWidth="1"/>
     <col min="8" max="8" width="21.7265625" style="24" customWidth="1"/>
-    <col min="9" max="16384" width="10.6328125" style="24"/>
+    <col min="9" max="15" width="10.6328125" style="24"/>
+    <col min="16" max="16" width="16.1796875" style="24" customWidth="1"/>
+    <col min="17" max="16384" width="10.6328125" style="24"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="22" customFormat="1" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -17255,6 +17260,18 @@
       <c r="M1" s="25" t="s">
         <v>823</v>
       </c>
+      <c r="N1" s="27" t="s">
+        <v>837</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>838</v>
+      </c>
+      <c r="P1" s="27" t="s">
+        <v>839</v>
+      </c>
+      <c r="Q1" s="13" t="s">
+        <v>840</v>
+      </c>
     </row>
     <row r="2" spans="1:26" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="35" t="s">
@@ -17296,6 +17313,18 @@
       <c r="M2" s="34" t="s">
         <v>8</v>
       </c>
+      <c r="N2" s="35" t="s">
+        <v>355</v>
+      </c>
+      <c r="O2" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2" s="35" t="s">
+        <v>355</v>
+      </c>
+      <c r="Q2" s="34" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" spans="1:26" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="35" t="s">
@@ -17337,6 +17366,18 @@
       <c r="M3" s="34" t="s">
         <v>8</v>
       </c>
+      <c r="N3" s="35" t="s">
+        <v>362</v>
+      </c>
+      <c r="O3" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3" s="35" t="s">
+        <v>362</v>
+      </c>
+      <c r="Q3" s="34" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="1:26" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="35" t="s">
@@ -17378,6 +17419,18 @@
       <c r="M4" s="34" t="s">
         <v>8</v>
       </c>
+      <c r="N4" s="35" t="s">
+        <v>369</v>
+      </c>
+      <c r="O4" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="P4" s="35" t="s">
+        <v>369</v>
+      </c>
+      <c r="Q4" s="34" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="1:26" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="35" t="s">
@@ -17419,6 +17472,18 @@
       <c r="M5" s="34" t="s">
         <v>8</v>
       </c>
+      <c r="N5" s="35" t="s">
+        <v>664</v>
+      </c>
+      <c r="O5" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="P5" s="35" t="s">
+        <v>664</v>
+      </c>
+      <c r="Q5" s="34" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="6" spans="1:26" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="35" t="s">
@@ -17460,6 +17525,18 @@
       <c r="M6" s="34" t="s">
         <v>8</v>
       </c>
+      <c r="N6" s="35" t="s">
+        <v>665</v>
+      </c>
+      <c r="O6" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="P6" s="35" t="s">
+        <v>665</v>
+      </c>
+      <c r="Q6" s="34" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" spans="1:26" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="35" t="s">
@@ -17501,6 +17578,18 @@
       <c r="M7" s="34" t="s">
         <v>8</v>
       </c>
+      <c r="N7" s="35" t="s">
+        <v>385</v>
+      </c>
+      <c r="O7" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="P7" s="35" t="s">
+        <v>385</v>
+      </c>
+      <c r="Q7" s="34" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="8" spans="1:26" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="35" t="s">
@@ -17542,6 +17631,18 @@
       <c r="M8" s="34" t="s">
         <v>8</v>
       </c>
+      <c r="N8" s="35" t="s">
+        <v>390</v>
+      </c>
+      <c r="O8" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="P8" s="35" t="s">
+        <v>390</v>
+      </c>
+      <c r="Q8" s="34" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="9" spans="1:26" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="35" t="s">
@@ -17583,6 +17684,18 @@
       <c r="M9" s="34" t="s">
         <v>8</v>
       </c>
+      <c r="N9" s="35" t="s">
+        <v>666</v>
+      </c>
+      <c r="O9" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="P9" s="35" t="s">
+        <v>666</v>
+      </c>
+      <c r="Q9" s="34" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="10" spans="1:26" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="35" t="s">
@@ -17624,6 +17737,18 @@
       <c r="M10" s="34" t="s">
         <v>8</v>
       </c>
+      <c r="N10" s="49" t="s">
+        <v>675</v>
+      </c>
+      <c r="O10" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="P10" s="35" t="s">
+        <v>667</v>
+      </c>
+      <c r="Q10" s="8" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="11" spans="1:26" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="35" t="s">
@@ -17665,10 +17790,18 @@
       <c r="M11" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="N11" s="35"/>
-      <c r="O11" s="35"/>
-      <c r="P11" s="35"/>
-      <c r="Q11" s="35"/>
+      <c r="N11" s="35" t="s">
+        <v>675</v>
+      </c>
+      <c r="O11" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="P11" s="35" t="s">
+        <v>675</v>
+      </c>
+      <c r="Q11" s="34" t="s">
+        <v>8</v>
+      </c>
       <c r="R11" s="35"/>
       <c r="S11" s="35"/>
       <c r="T11" s="35"/>
@@ -17719,10 +17852,18 @@
       <c r="M12" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="N12" s="35"/>
-      <c r="O12" s="35"/>
-      <c r="P12" s="35"/>
-      <c r="Q12" s="35"/>
+      <c r="N12" s="35" t="s">
+        <v>679</v>
+      </c>
+      <c r="O12" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="P12" s="35" t="s">
+        <v>679</v>
+      </c>
+      <c r="Q12" s="34" t="s">
+        <v>8</v>
+      </c>
       <c r="R12" s="35"/>
       <c r="S12" s="35"/>
       <c r="T12" s="35"/>
@@ -17773,6 +17914,18 @@
       <c r="M13" s="34" t="s">
         <v>8</v>
       </c>
+      <c r="N13" s="35" t="s">
+        <v>689</v>
+      </c>
+      <c r="O13" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="P13" s="35" t="s">
+        <v>689</v>
+      </c>
+      <c r="Q13" s="34" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="14" spans="1:26" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="35" t="s">
@@ -17814,6 +17967,18 @@
       <c r="M14" s="34" t="s">
         <v>8</v>
       </c>
+      <c r="N14" s="35" t="s">
+        <v>690</v>
+      </c>
+      <c r="O14" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="P14" s="35" t="s">
+        <v>690</v>
+      </c>
+      <c r="Q14" s="34" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="15" spans="1:26" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="35" t="s">
@@ -17855,6 +18020,18 @@
       <c r="M15" s="34" t="s">
         <v>8</v>
       </c>
+      <c r="N15" s="35" t="s">
+        <v>675</v>
+      </c>
+      <c r="O15" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="P15" s="35" t="s">
+        <v>675</v>
+      </c>
+      <c r="Q15" s="34" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="16" spans="1:26" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="35" t="s">
@@ -17896,8 +18073,20 @@
       <c r="M16" s="34" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N16" s="35" t="s">
+        <v>675</v>
+      </c>
+      <c r="O16" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="P16" s="35" t="s">
+        <v>675</v>
+      </c>
+      <c r="Q16" s="34" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="35" t="s">
         <v>501</v>
       </c>
@@ -17937,8 +18126,20 @@
       <c r="M17" s="34" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N17" s="35" t="s">
+        <v>675</v>
+      </c>
+      <c r="O17" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="P17" s="35" t="s">
+        <v>675</v>
+      </c>
+      <c r="Q17" s="34" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="37"/>
       <c r="B18" s="37"/>
       <c r="C18" s="37"/>
@@ -17948,7 +18149,7 @@
       <c r="G18" s="37"/>
       <c r="H18" s="37"/>
     </row>
-    <row r="19" spans="1:13" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:17" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="37"/>
       <c r="B19" s="37"/>
       <c r="C19" s="37"/>
@@ -17958,7 +18159,7 @@
       <c r="G19" s="37"/>
       <c r="H19" s="37"/>
     </row>
-    <row r="20" spans="1:13" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:17" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="37"/>
       <c r="B20" s="37"/>
       <c r="C20" s="37"/>
@@ -17968,7 +18169,7 @@
       <c r="G20" s="37"/>
       <c r="H20" s="37"/>
     </row>
-    <row r="21" spans="1:13" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:17" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="37"/>
       <c r="B21" s="37"/>
       <c r="C21" s="37"/>
@@ -17978,7 +18179,7 @@
       <c r="G21" s="37"/>
       <c r="H21" s="37"/>
     </row>
-    <row r="22" spans="1:13" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:17" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="37"/>
       <c r="B22" s="37"/>
       <c r="C22" s="37"/>
@@ -17988,7 +18189,7 @@
       <c r="G22" s="37"/>
       <c r="H22" s="37"/>
     </row>
-    <row r="23" spans="1:13" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:17" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="37"/>
       <c r="B23" s="38"/>
       <c r="C23" s="37"/>
@@ -17998,7 +18199,7 @@
       <c r="G23" s="37"/>
       <c r="H23" s="37"/>
     </row>
-    <row r="24" spans="1:13" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:17" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="37"/>
       <c r="B24" s="37"/>
       <c r="C24" s="37"/>
@@ -18008,7 +18209,7 @@
       <c r="G24" s="37"/>
       <c r="H24" s="37"/>
     </row>
-    <row r="25" spans="1:13" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:17" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="37"/>
       <c r="B25" s="37"/>
       <c r="C25" s="37"/>
@@ -18018,7 +18219,7 @@
       <c r="G25" s="37"/>
       <c r="H25" s="37"/>
     </row>
-    <row r="26" spans="1:13" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:17" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="37"/>
       <c r="B26" s="37"/>
       <c r="C26" s="37"/>
@@ -18028,7 +18229,7 @@
       <c r="G26" s="37"/>
       <c r="H26" s="37"/>
     </row>
-    <row r="27" spans="1:13" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:17" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="37"/>
       <c r="B27" s="37"/>
       <c r="C27" s="37"/>
@@ -18038,7 +18239,7 @@
       <c r="G27" s="37"/>
       <c r="H27" s="37"/>
     </row>
-    <row r="28" spans="1:13" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:17" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="37"/>
       <c r="B28" s="37"/>
       <c r="C28" s="37"/>
@@ -18048,7 +18249,7 @@
       <c r="G28" s="37"/>
       <c r="H28" s="37"/>
     </row>
-    <row r="29" spans="1:13" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:17" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="37"/>
       <c r="B29" s="37"/>
       <c r="C29" s="37"/>
@@ -18058,7 +18259,7 @@
       <c r="G29" s="37"/>
       <c r="H29" s="37"/>
     </row>
-    <row r="30" spans="1:13" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:17" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="37"/>
       <c r="B30" s="37"/>
       <c r="C30" s="37"/>
@@ -18355,7 +18556,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB7AA43-4AE1-4D26-A97B-9F9B33DC61B2}">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated testcases for manual Bidding
Updated testcases for manual Bidding
</commit_message>
<xml_diff>
--- a/testing/testcases.xlsx
+++ b/testing/testcases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lai See Hoe\Documents\GitHub\project-g5t4\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF61A701-643A-4D79-B2ED-519564EC3155}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4A2DBAC-B7D7-4EFB-9B12-2D12660069E6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="844" firstSheet="14" activeTab="16" xr2:uid="{F747292D-6CBE-43A0-AF24-F2F7C25CEB64}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="844" firstSheet="14" activeTab="15" xr2:uid="{F747292D-6CBE-43A0-AF24-F2F7C25CEB64}"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 3 - JSON - BidDump" sheetId="20" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2862" uniqueCount="850">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3018" uniqueCount="849">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -6578,9 +6578,6 @@
   </si>
   <si>
     <t>Pass/Fail 9/10/19</t>
-  </si>
-  <si>
-    <t>Result 2 9/10/19</t>
   </si>
   <si>
     <t>Result 1 15/10/19</t>
@@ -7358,28 +7355,28 @@
         <v>6</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="I1" s="13" t="s">
         <v>793</v>
       </c>
       <c r="J1" s="13" t="s">
+        <v>800</v>
+      </c>
+      <c r="K1" s="13" t="s">
         <v>801</v>
       </c>
-      <c r="K1" s="13" t="s">
-        <v>802</v>
-      </c>
       <c r="L1" s="13" t="s">
+        <v>816</v>
+      </c>
+      <c r="M1" s="13" t="s">
         <v>817</v>
       </c>
-      <c r="M1" s="13" t="s">
-        <v>818</v>
-      </c>
       <c r="N1" s="22" t="s">
+        <v>829</v>
+      </c>
+      <c r="O1" s="22" t="s">
         <v>830</v>
-      </c>
-      <c r="O1" s="22" t="s">
-        <v>831</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -7393,7 +7390,7 @@
         <v>542</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E2" s="32" t="s">
         <v>543</v>
@@ -7440,7 +7437,7 @@
         <v>546</v>
       </c>
       <c r="D3" s="32" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>547</v>
@@ -7487,7 +7484,7 @@
         <v>550</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="E4" s="32" t="s">
         <v>551</v>
@@ -7568,16 +7565,16 @@
         <v>6</v>
       </c>
       <c r="H1" s="13" t="s">
+        <v>837</v>
+      </c>
+      <c r="I1" s="13" t="s">
         <v>838</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>839</v>
       </c>
       <c r="J1" s="13" t="s">
         <v>273</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="176" x14ac:dyDescent="0.35">
@@ -7670,7 +7667,7 @@
         <v>294</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>295</v>
@@ -7679,7 +7676,7 @@
         <v>260</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="K4" s="45" t="s">
         <v>8</v>
@@ -7705,7 +7702,7 @@
         <v>298</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>299</v>
@@ -7714,7 +7711,7 @@
         <v>260</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="K5" s="45" t="s">
         <v>8</v>
@@ -7740,7 +7737,7 @@
         <v>302</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="H6" s="6" t="s">
         <v>303</v>
@@ -7749,7 +7746,7 @@
         <v>260</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="K6" s="45" t="s">
         <v>8</v>
@@ -7781,7 +7778,7 @@
         <v>291</v>
       </c>
       <c r="I7" s="45" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="J7" s="6" t="s">
         <v>291</v>
@@ -7892,7 +7889,7 @@
   <sheetData>
     <row r="1" spans="1:13" s="30" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="29" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="B1" s="29" t="s">
         <v>1</v>
@@ -7916,19 +7913,19 @@
         <v>274</v>
       </c>
       <c r="I1" s="29" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="J1" s="29" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="K1" s="29" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="L1" s="29" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="M1" s="29" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="138.5" x14ac:dyDescent="0.35">
@@ -11205,28 +11202,28 @@
         <v>6</v>
       </c>
       <c r="H1" s="13" t="s">
+        <v>802</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>805</v>
+      </c>
+      <c r="J1" s="15" t="s">
         <v>803</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="K1" s="13" t="s">
+        <v>805</v>
+      </c>
+      <c r="L1" s="17" t="s">
         <v>806</v>
       </c>
-      <c r="J1" s="15" t="s">
-        <v>804</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>806</v>
-      </c>
-      <c r="L1" s="17" t="s">
+      <c r="M1" s="13" t="s">
         <v>807</v>
       </c>
-      <c r="M1" s="13" t="s">
-        <v>808</v>
-      </c>
       <c r="N1" s="24" t="s">
+        <v>826</v>
+      </c>
+      <c r="O1" s="13" t="s">
         <v>827</v>
-      </c>
-      <c r="O1" s="13" t="s">
-        <v>828</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="5" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
@@ -11646,28 +11643,28 @@
         <v>6</v>
       </c>
       <c r="H1" s="13" t="s">
+        <v>802</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>801</v>
+      </c>
+      <c r="J1" s="13" t="s">
         <v>803</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>802</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>804</v>
       </c>
       <c r="K1" s="13" t="s">
         <v>794</v>
       </c>
       <c r="L1" s="24" t="s">
+        <v>806</v>
+      </c>
+      <c r="M1" s="13" t="s">
         <v>807</v>
       </c>
-      <c r="M1" s="13" t="s">
-        <v>808</v>
-      </c>
       <c r="N1" s="24" t="s">
+        <v>826</v>
+      </c>
+      <c r="O1" s="13" t="s">
         <v>827</v>
-      </c>
-      <c r="O1" s="13" t="s">
-        <v>828</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="20" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -11678,7 +11675,7 @@
         <v>706</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="D2" s="20" t="s">
         <v>710</v>
@@ -11819,7 +11816,7 @@
         <v>706</v>
       </c>
       <c r="C5" s="43" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="D5" s="43" t="s">
         <v>711</v>
@@ -11918,28 +11915,28 @@
         <v>6</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="I1" s="13" t="s">
         <v>793</v>
       </c>
       <c r="J1" s="15" t="s">
+        <v>800</v>
+      </c>
+      <c r="K1" s="15" t="s">
         <v>801</v>
       </c>
-      <c r="K1" s="15" t="s">
-        <v>802</v>
-      </c>
       <c r="L1" s="24" t="s">
+        <v>806</v>
+      </c>
+      <c r="M1" s="13" t="s">
         <v>807</v>
       </c>
-      <c r="M1" s="13" t="s">
-        <v>808</v>
-      </c>
       <c r="N1" s="24" t="s">
+        <v>823</v>
+      </c>
+      <c r="O1" s="13" t="s">
         <v>824</v>
-      </c>
-      <c r="O1" s="13" t="s">
-        <v>825</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="130.5" x14ac:dyDescent="0.35">
@@ -12663,16 +12660,16 @@
         <v>798</v>
       </c>
       <c r="L1" s="24" t="s">
+        <v>806</v>
+      </c>
+      <c r="M1" s="13" t="s">
         <v>807</v>
       </c>
-      <c r="M1" s="13" t="s">
-        <v>808</v>
-      </c>
       <c r="N1" s="24" t="s">
+        <v>821</v>
+      </c>
+      <c r="O1" s="13" t="s">
         <v>822</v>
-      </c>
-      <c r="O1" s="13" t="s">
-        <v>823</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="116" x14ac:dyDescent="0.35">
@@ -12915,43 +12912,43 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>808</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>809</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>810</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>446</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>446</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="M7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="O7" s="2" t="s">
         <v>8</v>
@@ -12964,11 +12961,11 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D48F8994-0480-456C-9C73-8DEBC1CF05E8}">
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:U26"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N1" sqref="N1:O1"/>
+      <selection pane="bottomLeft" activeCell="T2" sqref="T2:U26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12982,7 +12979,7 @@
     <col min="11" max="11" width="15.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="26" customFormat="1" ht="24.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" s="26" customFormat="1" ht="24.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -12990,46 +12987,64 @@
         <v>1</v>
       </c>
       <c r="C1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="F1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="G1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="I1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="13" t="s">
-        <v>795</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>796</v>
-      </c>
       <c r="J1" s="13" t="s">
-        <v>799</v>
+        <v>845</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>798</v>
-      </c>
-      <c r="L1" s="24" t="s">
+        <v>792</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>846</v>
+      </c>
+      <c r="M1" s="15" t="s">
+        <v>793</v>
+      </c>
+      <c r="N1" s="24" t="s">
+        <v>847</v>
+      </c>
+      <c r="O1" s="13" t="s">
         <v>807</v>
       </c>
-      <c r="M1" s="13" t="s">
-        <v>808</v>
-      </c>
-      <c r="N1" s="24" t="s">
+      <c r="P1" s="24" t="s">
+        <v>848</v>
+      </c>
+      <c r="Q1" s="13" t="s">
         <v>822</v>
       </c>
-      <c r="O1" s="13" t="s">
-        <v>823</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="R1" s="24" t="s">
+        <v>843</v>
+      </c>
+      <c r="S1" s="13" t="s">
+        <v>831</v>
+      </c>
+      <c r="T1" s="24" t="s">
+        <v>844</v>
+      </c>
+      <c r="U1" s="13" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -13075,8 +13090,26 @@
       <c r="O2" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" ht="87" x14ac:dyDescent="0.35">
+      <c r="P2" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="87" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -13122,8 +13155,26 @@
       <c r="O3" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="P3" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -13169,8 +13220,26 @@
       <c r="O4" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="P4" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -13216,8 +13285,26 @@
       <c r="O5" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="P5" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -13263,8 +13350,26 @@
       <c r="O6" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+      <c r="P6" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="U6" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="58" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -13310,8 +13415,26 @@
       <c r="O7" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="P7" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T7" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="U7" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -13357,8 +13480,26 @@
       <c r="O8" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+      <c r="P8" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T8" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="U8" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -13404,8 +13545,26 @@
       <c r="O9" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="P9" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R9" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="S9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T9" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="U9" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -13451,8 +13610,26 @@
       <c r="O10" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+      <c r="P10" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="U10" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="58" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -13498,8 +13675,26 @@
       <c r="O11" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="P11" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T11" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="U11" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -13545,8 +13740,26 @@
       <c r="O12" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" ht="145" x14ac:dyDescent="0.35">
+      <c r="P12" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T12" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="U12" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="145" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -13592,8 +13805,26 @@
       <c r="O13" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" ht="145" x14ac:dyDescent="0.35">
+      <c r="P13" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R13" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="S13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T13" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="U13" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="145" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -13639,8 +13870,26 @@
       <c r="O14" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" ht="203" x14ac:dyDescent="0.35">
+      <c r="P14" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="Q14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R14" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="S14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T14" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="U14" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="203" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -13686,8 +13935,26 @@
       <c r="O15" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" ht="87" x14ac:dyDescent="0.35">
+      <c r="P15" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="Q15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R15" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="S15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T15" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="U15" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="87" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -13733,8 +14000,26 @@
       <c r="O16" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="P16" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="Q16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R16" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="S16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T16" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="U16" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -13780,8 +14065,26 @@
       <c r="O17" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" ht="87" x14ac:dyDescent="0.35">
+      <c r="P17" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="Q17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R17" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="S17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T17" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="U17" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="87" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -13827,8 +14130,26 @@
       <c r="O18" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" ht="87" x14ac:dyDescent="0.35">
+      <c r="P18" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="Q18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R18" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="S18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T18" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="U18" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" ht="87" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -13874,8 +14195,26 @@
       <c r="O19" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="P19" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="Q19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R19" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="S19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T19" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="U19" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -13921,8 +14260,26 @@
       <c r="O20" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="P20" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R20" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="S20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T20" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="U20" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -13968,8 +14325,26 @@
       <c r="O21" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="P21" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R21" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="S21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T21" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="U21" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -14015,8 +14390,26 @@
       <c r="O22" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="P22" s="2" t="s">
+        <v>769</v>
+      </c>
+      <c r="Q22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R22" s="2" t="s">
+        <v>769</v>
+      </c>
+      <c r="S22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T22" s="2" t="s">
+        <v>769</v>
+      </c>
+      <c r="U22" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -14062,8 +14455,26 @@
       <c r="O23" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="P23" s="2" t="s">
+        <v>768</v>
+      </c>
+      <c r="Q23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R23" s="2" t="s">
+        <v>768</v>
+      </c>
+      <c r="S23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T23" s="2" t="s">
+        <v>768</v>
+      </c>
+      <c r="U23" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -14109,8 +14520,26 @@
       <c r="O24" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" ht="87" x14ac:dyDescent="0.35">
+      <c r="P24" s="2" t="s">
+        <v>757</v>
+      </c>
+      <c r="Q24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R24" s="2" t="s">
+        <v>757</v>
+      </c>
+      <c r="S24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T24" s="2" t="s">
+        <v>757</v>
+      </c>
+      <c r="U24" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" ht="87" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -14156,8 +14585,26 @@
       <c r="O25" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+      <c r="P25" s="5" t="s">
+        <v>773</v>
+      </c>
+      <c r="Q25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R25" s="5" t="s">
+        <v>773</v>
+      </c>
+      <c r="S25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T25" s="5" t="s">
+        <v>773</v>
+      </c>
+      <c r="U25" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" ht="58" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -14201,6 +14648,24 @@
         <v>775</v>
       </c>
       <c r="O26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P26" s="2" t="s">
+        <v>775</v>
+      </c>
+      <c r="Q26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R26" s="2" t="s">
+        <v>775</v>
+      </c>
+      <c r="S26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T26" s="2" t="s">
+        <v>775</v>
+      </c>
+      <c r="U26" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -14213,7 +14678,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55C5E1F7-185F-4415-A762-CA1DF36823C6}">
   <dimension ref="A1:S9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="69" workbookViewId="0">
+    <sheetView zoomScale="69" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="R2" sqref="R2:S9"/>
     </sheetView>
@@ -14256,40 +14721,40 @@
         <v>6</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="I1" s="13" t="s">
         <v>792</v>
       </c>
       <c r="J1" s="15" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="K1" s="15" t="s">
         <v>793</v>
       </c>
       <c r="L1" s="24" t="s">
+        <v>847</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>807</v>
+      </c>
+      <c r="N1" s="24" t="s">
         <v>848</v>
       </c>
-      <c r="M1" s="13" t="s">
-        <v>808</v>
-      </c>
-      <c r="N1" s="24" t="s">
-        <v>849</v>
-      </c>
       <c r="O1" s="13" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="P1" s="24" t="s">
+        <v>843</v>
+      </c>
+      <c r="Q1" s="13" t="s">
+        <v>831</v>
+      </c>
+      <c r="R1" s="24" t="s">
         <v>844</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="S1" s="13" t="s">
         <v>832</v>
-      </c>
-      <c r="R1" s="24" t="s">
-        <v>845</v>
-      </c>
-      <c r="S1" s="13" t="s">
-        <v>833</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="87" x14ac:dyDescent="0.35">
@@ -14821,40 +15286,40 @@
         <v>6</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="I1" s="13" t="s">
         <v>792</v>
       </c>
       <c r="J1" s="15" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="K1" s="15" t="s">
         <v>793</v>
       </c>
       <c r="L1" s="24" t="s">
+        <v>847</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>807</v>
+      </c>
+      <c r="N1" s="24" t="s">
         <v>848</v>
       </c>
-      <c r="M1" s="13" t="s">
-        <v>808</v>
-      </c>
-      <c r="N1" s="24" t="s">
-        <v>849</v>
-      </c>
       <c r="O1" s="13" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="P1" s="24" t="s">
+        <v>843</v>
+      </c>
+      <c r="Q1" s="13" t="s">
+        <v>831</v>
+      </c>
+      <c r="R1" s="24" t="s">
         <v>844</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="S1" s="13" t="s">
         <v>832</v>
-      </c>
-      <c r="R1" s="24" t="s">
-        <v>845</v>
-      </c>
-      <c r="S1" s="13" t="s">
-        <v>833</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="145" x14ac:dyDescent="0.35">
@@ -16578,34 +17043,34 @@
         <v>6</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="I1" s="22" t="s">
         <v>793</v>
       </c>
       <c r="J1" s="22" t="s">
+        <v>800</v>
+      </c>
+      <c r="K1" s="22" t="s">
         <v>801</v>
       </c>
-      <c r="K1" s="22" t="s">
-        <v>802</v>
-      </c>
       <c r="L1" s="22" t="s">
+        <v>816</v>
+      </c>
+      <c r="M1" s="22" t="s">
         <v>817</v>
       </c>
-      <c r="M1" s="22" t="s">
-        <v>818</v>
-      </c>
       <c r="N1" s="22" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="O1" s="22" t="s">
+        <v>828</v>
+      </c>
+      <c r="P1" s="22" t="s">
         <v>829</v>
       </c>
-      <c r="P1" s="22" t="s">
+      <c r="Q1" s="22" t="s">
         <v>830</v>
-      </c>
-      <c r="Q1" s="22" t="s">
-        <v>831</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="126.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -16773,28 +17238,28 @@
         <v>6</v>
       </c>
       <c r="H1" s="29" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="I1" s="29" t="s">
         <v>793</v>
       </c>
       <c r="J1" s="29" t="s">
+        <v>800</v>
+      </c>
+      <c r="K1" s="29" t="s">
         <v>801</v>
       </c>
-      <c r="K1" s="29" t="s">
-        <v>802</v>
-      </c>
       <c r="L1" s="29" t="s">
+        <v>816</v>
+      </c>
+      <c r="M1" s="29" t="s">
         <v>817</v>
       </c>
-      <c r="M1" s="29" t="s">
-        <v>818</v>
-      </c>
       <c r="N1" s="22" t="s">
+        <v>829</v>
+      </c>
+      <c r="O1" s="22" t="s">
         <v>830</v>
-      </c>
-      <c r="O1" s="22" t="s">
-        <v>831</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="120.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -16907,28 +17372,28 @@
         <v>6</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="I1" s="22" t="s">
         <v>793</v>
       </c>
       <c r="J1" s="22" t="s">
+        <v>800</v>
+      </c>
+      <c r="K1" s="22" t="s">
         <v>801</v>
       </c>
-      <c r="K1" s="22" t="s">
-        <v>802</v>
-      </c>
       <c r="L1" s="22" t="s">
+        <v>816</v>
+      </c>
+      <c r="M1" s="22" t="s">
         <v>817</v>
       </c>
-      <c r="M1" s="22" t="s">
-        <v>818</v>
-      </c>
       <c r="N1" s="22" t="s">
+        <v>829</v>
+      </c>
+      <c r="O1" s="22" t="s">
         <v>830</v>
-      </c>
-      <c r="O1" s="22" t="s">
-        <v>831</v>
       </c>
     </row>
     <row r="2" spans="1:26" ht="115.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -17067,22 +17532,22 @@
         <v>6</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="I1" s="22" t="s">
         <v>793</v>
       </c>
       <c r="J1" s="22" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="K1" s="22" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="L1" s="22" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="M1" s="22" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="2" spans="1:26" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -17512,34 +17977,34 @@
         <v>6</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="I1" s="22" t="s">
         <v>793</v>
       </c>
       <c r="J1" s="22" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="K1" s="22" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="L1" s="22" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="M1" s="22" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="N1" s="24" t="s">
+        <v>843</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>831</v>
+      </c>
+      <c r="P1" s="24" t="s">
         <v>844</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="Q1" s="13" t="s">
         <v>832</v>
-      </c>
-      <c r="P1" s="24" t="s">
-        <v>845</v>
-      </c>
-      <c r="Q1" s="13" t="s">
-        <v>833</v>
       </c>
     </row>
     <row r="2" spans="1:26" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -18577,22 +19042,22 @@
         <v>6</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="I1" s="22" t="s">
         <v>793</v>
       </c>
       <c r="J1" s="22" t="s">
+        <v>800</v>
+      </c>
+      <c r="K1" s="22" t="s">
         <v>801</v>
       </c>
-      <c r="K1" s="22" t="s">
-        <v>802</v>
-      </c>
       <c r="L1" s="22" t="s">
+        <v>816</v>
+      </c>
+      <c r="M1" s="22" t="s">
         <v>817</v>
-      </c>
-      <c r="M1" s="22" t="s">
-        <v>818</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="76.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -18716,22 +19181,22 @@
         <v>6</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="I1" s="13" t="s">
         <v>793</v>
       </c>
       <c r="J1" s="13" t="s">
+        <v>800</v>
+      </c>
+      <c r="K1" s="13" t="s">
         <v>801</v>
       </c>
-      <c r="K1" s="13" t="s">
-        <v>802</v>
-      </c>
       <c r="L1" s="13" t="s">
+        <v>816</v>
+      </c>
+      <c r="M1" s="13" t="s">
         <v>817</v>
-      </c>
-      <c r="M1" s="13" t="s">
-        <v>818</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="76.5" thickBot="1" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
Updat testcases for sectiondump (JSON)
Co-Authored-By: seehoe <seehoe@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/testing/testcases.xlsx
+++ b/testing/testcases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lai See Hoe\Documents\GitHub\project-g5t4\testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\project-g5t4\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4A2DBAC-B7D7-4EFB-9B12-2D12660069E6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE0EC1EA-71A3-4C4A-BC44-B9A109B4E67C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="844" firstSheet="14" activeTab="15" xr2:uid="{F747292D-6CBE-43A0-AF24-F2F7C25CEB64}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="844" activeTab="4" xr2:uid="{F747292D-6CBE-43A0-AF24-F2F7C25CEB64}"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 3 - JSON - BidDump" sheetId="20" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3018" uniqueCount="849">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3086" uniqueCount="853">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -6745,6 +6745,62 @@
   <si>
     <t>Result 3/11/19</t>
   </si>
+  <si>
+    <t>Result  31/10/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pass/Fail 31/10/19 </t>
+  </si>
+  <si>
+    <t>{
+    "status": "success",
+    "students": [
+        {
+            "userid": "olivia.ng.2009",
+            "amount": "22.00"
+        },
+        {
+            "userid": "neilson.ng.2009",
+            "amount": "21.00"
+        },
+        {
+            "userid": "maggie.ng.2009",
+            "amount": "20.00"
+        },
+        {
+            "userid": "ian.ng.2009",
+            "amount": "18.00"
+        },
+        {
+            "userid": "harry.ng.2009",
+            "amount": "17.00"
+        },
+        {
+            "userid": "fred.ng.2009",
+            "amount": "15.00"
+        },
+        {
+            "userid": "eddy.ng.2009",
+            "amount": "14.00"
+        },
+        {
+            "userid": "dawn.ng.2009",
+            "amount": "13.00"
+        },
+        {
+            "userid": "calvin.ng.2009",
+            "amount": "12.00"
+        },
+        {
+            "userid": "ben.ng.2009",
+            "amount": "11.00"
+        }
+    ]
+}</t>
+  </si>
+  <si>
+    <t>r={"course": "IS100","section": "S11"}</t>
+  </si>
 </sst>
 </file>
 
@@ -6812,7 +6868,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -6872,11 +6928,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -7005,6 +7076,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7327,12 +7401,12 @@
       <selection pane="bottomLeft" activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.6328125" defaultRowHeight="50" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="14.08984375" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="37" customFormat="1" ht="38" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" s="37" customFormat="1" ht="38.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -7379,7 +7453,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
         <v>540</v>
       </c>
@@ -7426,7 +7500,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="32" t="s">
         <v>544</v>
       </c>
@@ -7473,7 +7547,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:15" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="32" t="s">
         <v>548</v>
       </c>
@@ -7533,16 +7607,16 @@
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="8.7265625" customWidth="1"/>
-    <col min="7" max="7" width="17.81640625" customWidth="1"/>
-    <col min="8" max="8" width="22.08984375" customWidth="1"/>
-    <col min="9" max="9" width="11.81640625" customWidth="1"/>
-    <col min="10" max="10" width="16.90625" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" customWidth="1"/>
+    <col min="8" max="8" width="22.140625" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="25" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="25" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -7577,7 +7651,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="176" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="192" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -7612,7 +7686,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="101" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="102.75" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -7647,7 +7721,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="88.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -7682,7 +7756,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="88.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -7717,7 +7791,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="113.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="115.5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -7752,7 +7826,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="101" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="102.75" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -7787,7 +7861,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="113.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="102.75" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -7822,7 +7896,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="176" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" ht="192" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -7871,23 +7945,23 @@
       <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.54296875" style="28" customWidth="1"/>
-    <col min="2" max="2" width="24.08984375" style="28" customWidth="1"/>
-    <col min="3" max="3" width="14.7265625" style="28" customWidth="1"/>
-    <col min="4" max="4" width="12.54296875" style="28" customWidth="1"/>
-    <col min="5" max="5" width="38.81640625" style="28" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.36328125" style="28" customWidth="1"/>
-    <col min="7" max="7" width="27.7265625" style="28" customWidth="1"/>
-    <col min="8" max="8" width="25.54296875" style="28" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" style="28" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" style="28" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" style="28" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" style="28" customWidth="1"/>
+    <col min="5" max="5" width="38.85546875" style="28" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" style="28" customWidth="1"/>
+    <col min="7" max="7" width="27.7109375" style="28" customWidth="1"/>
+    <col min="8" max="8" width="25.5703125" style="28" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" style="28" customWidth="1"/>
-    <col min="10" max="10" width="10.81640625" style="28" customWidth="1"/>
-    <col min="11" max="11" width="8.453125" style="28" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.7265625" style="28"/>
+    <col min="10" max="10" width="10.85546875" style="28" customWidth="1"/>
+    <col min="11" max="11" width="8.42578125" style="28" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.7109375" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="30" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="30" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
         <v>814</v>
       </c>
@@ -7928,7 +8002,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="138.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="141" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
         <v>282</v>
       </c>
@@ -7959,7 +8033,7 @@
       <c r="J2" s="27"/>
       <c r="K2" s="27"/>
     </row>
-    <row r="3" spans="1:13" ht="76" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
         <v>288</v>
       </c>
@@ -7990,7 +8064,7 @@
       <c r="J3" s="27"/>
       <c r="K3" s="27"/>
     </row>
-    <row r="4" spans="1:13" ht="76" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
         <v>292</v>
       </c>
@@ -8021,7 +8095,7 @@
       <c r="J4" s="27"/>
       <c r="K4" s="27"/>
     </row>
-    <row r="5" spans="1:13" ht="76" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A5" s="27" t="s">
         <v>296</v>
       </c>
@@ -8052,7 +8126,7 @@
       <c r="J5" s="27"/>
       <c r="K5" s="27"/>
     </row>
-    <row r="6" spans="1:13" ht="88.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" ht="102.75" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
         <v>300</v>
       </c>
@@ -8083,7 +8157,7 @@
       <c r="J6" s="27"/>
       <c r="K6" s="27"/>
     </row>
-    <row r="7" spans="1:13" ht="76" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
         <v>304</v>
       </c>
@@ -8114,7 +8188,7 @@
       <c r="J7" s="27"/>
       <c r="K7" s="27"/>
     </row>
-    <row r="8" spans="1:13" ht="76" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
         <v>309</v>
       </c>
@@ -8145,7 +8219,7 @@
       <c r="J8" s="27"/>
       <c r="K8" s="27"/>
     </row>
-    <row r="9" spans="1:13" ht="138.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" ht="141" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
         <v>313</v>
       </c>
@@ -8174,7 +8248,7 @@
       <c r="J9" s="27"/>
       <c r="K9" s="27"/>
     </row>
-    <row r="10" spans="1:13" ht="409.6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A10" s="27" t="s">
         <v>319</v>
       </c>
@@ -8203,7 +8277,7 @@
       <c r="J10" s="27"/>
       <c r="K10" s="27"/>
     </row>
-    <row r="11" spans="1:13" ht="409.6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A11" s="27" t="s">
         <v>325</v>
       </c>
@@ -8232,7 +8306,7 @@
       <c r="J11" s="27"/>
       <c r="K11" s="27"/>
     </row>
-    <row r="12" spans="1:13" ht="409.6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A12" s="27" t="s">
         <v>329</v>
       </c>
@@ -8261,7 +8335,7 @@
       <c r="J12" s="27"/>
       <c r="K12" s="27"/>
     </row>
-    <row r="13" spans="1:13" ht="409.6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="s">
         <v>333</v>
       </c>
@@ -8290,7 +8364,7 @@
       <c r="J13" s="27"/>
       <c r="K13" s="27"/>
     </row>
-    <row r="14" spans="1:13" ht="409.6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A14" s="27" t="s">
         <v>337</v>
       </c>
@@ -8319,7 +8393,7 @@
       <c r="J14" s="27"/>
       <c r="K14" s="27"/>
     </row>
-    <row r="15" spans="1:13" ht="409.6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
         <v>341</v>
       </c>
@@ -8348,7 +8422,7 @@
       <c r="J15" s="27"/>
       <c r="K15" s="27"/>
     </row>
-    <row r="16" spans="1:13" ht="301" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" ht="306.75" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
         <v>345</v>
       </c>
@@ -8377,7 +8451,7 @@
       <c r="J16" s="27"/>
       <c r="K16" s="27"/>
     </row>
-    <row r="17" spans="1:11" ht="101" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" ht="102.75" x14ac:dyDescent="0.25">
       <c r="A17" s="27" t="s">
         <v>349</v>
       </c>
@@ -8406,7 +8480,7 @@
       <c r="J17" s="27"/>
       <c r="K17" s="27"/>
     </row>
-    <row r="18" spans="1:11" ht="101" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" ht="102.75" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
         <v>356</v>
       </c>
@@ -8435,7 +8509,7 @@
       <c r="J18" s="27"/>
       <c r="K18" s="27"/>
     </row>
-    <row r="19" spans="1:11" ht="76" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
         <v>363</v>
       </c>
@@ -8464,7 +8538,7 @@
       <c r="J19" s="27"/>
       <c r="K19" s="27"/>
     </row>
-    <row r="20" spans="1:11" ht="76" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
         <v>370</v>
       </c>
@@ -8493,7 +8567,7 @@
       <c r="J20" s="27"/>
       <c r="K20" s="27"/>
     </row>
-    <row r="21" spans="1:11" ht="76" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A21" s="27" t="s">
         <v>375</v>
       </c>
@@ -8522,7 +8596,7 @@
       <c r="J21" s="27"/>
       <c r="K21" s="27"/>
     </row>
-    <row r="22" spans="1:11" ht="76" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A22" s="27" t="s">
         <v>380</v>
       </c>
@@ -8551,7 +8625,7 @@
       <c r="J22" s="27"/>
       <c r="K22" s="27"/>
     </row>
-    <row r="23" spans="1:11" ht="76" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A23" s="27" t="s">
         <v>386</v>
       </c>
@@ -8580,7 +8654,7 @@
       <c r="J23" s="27"/>
       <c r="K23" s="27"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="s">
         <v>391</v>
       </c>
@@ -8595,7 +8669,7 @@
       <c r="J24" s="27"/>
       <c r="K24" s="27"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="27" t="s">
         <v>392</v>
       </c>
@@ -8610,7 +8684,7 @@
       <c r="J25" s="27"/>
       <c r="K25" s="27"/>
     </row>
-    <row r="26" spans="1:11" ht="88.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A26" s="27" t="s">
         <v>393</v>
       </c>
@@ -8639,7 +8713,7 @@
       <c r="J26" s="27"/>
       <c r="K26" s="27"/>
     </row>
-    <row r="27" spans="1:11" ht="88.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" s="27" t="s">
         <v>399</v>
       </c>
@@ -8668,7 +8742,7 @@
       <c r="J27" s="27"/>
       <c r="K27" s="27"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="27" t="s">
         <v>405</v>
       </c>
@@ -8683,7 +8757,7 @@
       <c r="J28" s="27"/>
       <c r="K28" s="27"/>
     </row>
-    <row r="29" spans="1:11" ht="76" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A29" s="27" t="s">
         <v>406</v>
       </c>
@@ -8710,7 +8784,7 @@
       <c r="J29" s="27"/>
       <c r="K29" s="27"/>
     </row>
-    <row r="30" spans="1:11" ht="76" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A30" s="27" t="s">
         <v>411</v>
       </c>
@@ -8739,7 +8813,7 @@
       <c r="J30" s="27"/>
       <c r="K30" s="27"/>
     </row>
-    <row r="31" spans="1:11" ht="128.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" ht="128.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="27" t="s">
         <v>415</v>
       </c>
@@ -8768,7 +8842,7 @@
       <c r="J31" s="27"/>
       <c r="K31" s="27"/>
     </row>
-    <row r="32" spans="1:11" ht="51" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A32" s="27" t="s">
         <v>419</v>
       </c>
@@ -8797,7 +8871,7 @@
       <c r="J32" s="27"/>
       <c r="K32" s="27"/>
     </row>
-    <row r="33" spans="1:11" ht="63.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
       <c r="A33" s="27" t="s">
         <v>423</v>
       </c>
@@ -8826,7 +8900,7 @@
       <c r="J33" s="27"/>
       <c r="K33" s="27"/>
     </row>
-    <row r="34" spans="1:11" ht="409.6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A34" s="27" t="s">
         <v>429</v>
       </c>
@@ -8855,7 +8929,7 @@
       <c r="J34" s="27"/>
       <c r="K34" s="27"/>
     </row>
-    <row r="35" spans="1:11" ht="51" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A35" s="27" t="s">
         <v>434</v>
       </c>
@@ -8884,7 +8958,7 @@
       <c r="J35" s="27"/>
       <c r="K35" s="27"/>
     </row>
-    <row r="36" spans="1:11" ht="38.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" ht="39" x14ac:dyDescent="0.25">
       <c r="A36" s="27" t="s">
         <v>439</v>
       </c>
@@ -8913,7 +8987,7 @@
       <c r="J36" s="27"/>
       <c r="K36" s="27"/>
     </row>
-    <row r="37" spans="1:11" ht="88.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A37" s="27" t="s">
         <v>443</v>
       </c>
@@ -8942,7 +9016,7 @@
       <c r="J37" s="27"/>
       <c r="K37" s="27"/>
     </row>
-    <row r="38" spans="1:11" ht="76" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A38" s="27" t="s">
         <v>449</v>
       </c>
@@ -8971,7 +9045,7 @@
       <c r="J38" s="27"/>
       <c r="K38" s="27"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="27" t="s">
         <v>452</v>
       </c>
@@ -8986,7 +9060,7 @@
       <c r="J39" s="27"/>
       <c r="K39" s="27"/>
     </row>
-    <row r="40" spans="1:11" ht="409.6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A40" s="27" t="s">
         <v>453</v>
       </c>
@@ -9013,7 +9087,7 @@
       <c r="J40" s="27"/>
       <c r="K40" s="27"/>
     </row>
-    <row r="41" spans="1:11" ht="101" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" ht="102.75" x14ac:dyDescent="0.25">
       <c r="A41" s="27" t="s">
         <v>456</v>
       </c>
@@ -9042,7 +9116,7 @@
       <c r="J41" s="27"/>
       <c r="K41" s="27"/>
     </row>
-    <row r="42" spans="1:11" ht="409.6" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A42" s="27" t="s">
         <v>460</v>
       </c>
@@ -9071,7 +9145,7 @@
       <c r="J42" s="27"/>
       <c r="K42" s="27"/>
     </row>
-    <row r="43" spans="1:11" ht="76" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A43" s="27" t="s">
         <v>464</v>
       </c>
@@ -9100,7 +9174,7 @@
       <c r="J43" s="27"/>
       <c r="K43" s="27"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="27" t="s">
         <v>469</v>
       </c>
@@ -9115,7 +9189,7 @@
       <c r="J44" s="27"/>
       <c r="K44" s="27"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="27" t="s">
         <v>470</v>
       </c>
@@ -9130,7 +9204,7 @@
       <c r="J45" s="27"/>
       <c r="K45" s="27"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="27" t="s">
         <v>471</v>
       </c>
@@ -9145,7 +9219,7 @@
       <c r="J46" s="27"/>
       <c r="K46" s="27"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="27" t="s">
         <v>472</v>
       </c>
@@ -9160,7 +9234,7 @@
       <c r="J47" s="27"/>
       <c r="K47" s="27"/>
     </row>
-    <row r="48" spans="1:11" ht="51" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A48" s="27" t="s">
         <v>473</v>
       </c>
@@ -9189,7 +9263,7 @@
       <c r="J48" s="27"/>
       <c r="K48" s="27"/>
     </row>
-    <row r="49" spans="1:11" ht="76" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:11" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A49" s="27" t="s">
         <v>478</v>
       </c>
@@ -9218,7 +9292,7 @@
       <c r="J49" s="27"/>
       <c r="K49" s="27"/>
     </row>
-    <row r="50" spans="1:11" ht="88.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A50" s="27" t="s">
         <v>484</v>
       </c>
@@ -9247,7 +9321,7 @@
       <c r="J50" s="27"/>
       <c r="K50" s="27"/>
     </row>
-    <row r="51" spans="1:11" ht="76" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:11" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A51" s="27" t="s">
         <v>489</v>
       </c>
@@ -9276,7 +9350,7 @@
       <c r="J51" s="27"/>
       <c r="K51" s="27"/>
     </row>
-    <row r="52" spans="1:11" ht="76" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:11" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A52" s="27" t="s">
         <v>495</v>
       </c>
@@ -9305,7 +9379,7 @@
       <c r="J52" s="27"/>
       <c r="K52" s="27"/>
     </row>
-    <row r="53" spans="1:11" ht="76" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:11" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A53" s="27" t="s">
         <v>501</v>
       </c>
@@ -9334,7 +9408,7 @@
       <c r="J53" s="27"/>
       <c r="K53" s="27"/>
     </row>
-    <row r="54" spans="1:11" ht="76" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:11" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A54" s="27" t="s">
         <v>506</v>
       </c>
@@ -9363,7 +9437,7 @@
       <c r="J54" s="27"/>
       <c r="K54" s="27"/>
     </row>
-    <row r="55" spans="1:11" ht="409.6" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A55" s="27" t="s">
         <v>511</v>
       </c>
@@ -9392,7 +9466,7 @@
       <c r="J55" s="27"/>
       <c r="K55" s="27"/>
     </row>
-    <row r="56" spans="1:11" ht="76" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:11" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A56" s="27" t="s">
         <v>516</v>
       </c>
@@ -9421,7 +9495,7 @@
       <c r="J56" s="27"/>
       <c r="K56" s="27"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="27" t="s">
         <v>521</v>
       </c>
@@ -9436,7 +9510,7 @@
       <c r="J57" s="27"/>
       <c r="K57" s="27"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="27" t="s">
         <v>522</v>
       </c>
@@ -9451,7 +9525,7 @@
       <c r="J58" s="27"/>
       <c r="K58" s="27"/>
     </row>
-    <row r="59" spans="1:11" ht="409.6" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A59" s="27" t="s">
         <v>523</v>
       </c>
@@ -9480,7 +9554,7 @@
       <c r="J59" s="27"/>
       <c r="K59" s="27"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="27" t="s">
         <v>528</v>
       </c>
@@ -9495,7 +9569,7 @@
       <c r="J60" s="27"/>
       <c r="K60" s="27"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="27" t="s">
         <v>529</v>
       </c>
@@ -9510,7 +9584,7 @@
       <c r="J61" s="27"/>
       <c r="K61" s="27"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="27" t="s">
         <v>530</v>
       </c>
@@ -9525,7 +9599,7 @@
       <c r="J62" s="27"/>
       <c r="K62" s="27"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="27" t="s">
         <v>531</v>
       </c>
@@ -9540,7 +9614,7 @@
       <c r="J63" s="27"/>
       <c r="K63" s="27"/>
     </row>
-    <row r="64" spans="1:11" ht="38.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:11" ht="39" x14ac:dyDescent="0.25">
       <c r="A64" s="27" t="s">
         <v>532</v>
       </c>
@@ -9569,7 +9643,7 @@
       <c r="J64" s="27"/>
       <c r="K64" s="27"/>
     </row>
-    <row r="65" spans="1:11" ht="409.6" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A65" s="27" t="s">
         <v>537</v>
       </c>
@@ -9592,7 +9666,7 @@
       <c r="J65" s="27"/>
       <c r="K65" s="27"/>
     </row>
-    <row r="66" spans="1:11" ht="76" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:11" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A66" s="27" t="s">
         <v>540</v>
       </c>
@@ -9619,7 +9693,7 @@
       <c r="J66" s="27"/>
       <c r="K66" s="27"/>
     </row>
-    <row r="67" spans="1:11" ht="76" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:11" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A67" s="27" t="s">
         <v>544</v>
       </c>
@@ -9646,7 +9720,7 @@
       <c r="J67" s="27"/>
       <c r="K67" s="27"/>
     </row>
-    <row r="68" spans="1:11" ht="409.6" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A68" s="27" t="s">
         <v>548</v>
       </c>
@@ -9673,7 +9747,7 @@
       <c r="J68" s="27"/>
       <c r="K68" s="27"/>
     </row>
-    <row r="69" spans="1:11" ht="76" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:11" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A69" s="27" t="s">
         <v>552</v>
       </c>
@@ -9700,7 +9774,7 @@
       <c r="J69" s="27"/>
       <c r="K69" s="27"/>
     </row>
-    <row r="70" spans="1:11" ht="409.6" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A70" s="27" t="s">
         <v>556</v>
       </c>
@@ -9727,7 +9801,7 @@
       <c r="J70" s="27"/>
       <c r="K70" s="27"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="27" t="s">
         <v>560</v>
       </c>
@@ -9742,7 +9816,7 @@
       <c r="J71" s="27"/>
       <c r="K71" s="27"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="27" t="s">
         <v>561</v>
       </c>
@@ -9757,7 +9831,7 @@
       <c r="J72" s="27"/>
       <c r="K72" s="27"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="27" t="s">
         <v>562</v>
       </c>
@@ -9772,7 +9846,7 @@
       <c r="J73" s="27"/>
       <c r="K73" s="27"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="27" t="s">
         <v>563</v>
       </c>
@@ -9787,7 +9861,7 @@
       <c r="J74" s="27"/>
       <c r="K74" s="27"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="27" t="s">
         <v>564</v>
       </c>
@@ -9802,7 +9876,7 @@
       <c r="J75" s="27"/>
       <c r="K75" s="27"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="27" t="s">
         <v>565</v>
       </c>
@@ -9817,7 +9891,7 @@
       <c r="J76" s="27"/>
       <c r="K76" s="27"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="27" t="s">
         <v>566</v>
       </c>
@@ -9832,7 +9906,7 @@
       <c r="J77" s="27"/>
       <c r="K77" s="27"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="27" t="s">
         <v>567</v>
       </c>
@@ -9847,7 +9921,7 @@
       <c r="J78" s="27"/>
       <c r="K78" s="27"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="27" t="s">
         <v>568</v>
       </c>
@@ -9862,7 +9936,7 @@
       <c r="J79" s="27"/>
       <c r="K79" s="27"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="27" t="s">
         <v>569</v>
       </c>
@@ -9877,7 +9951,7 @@
       <c r="J80" s="27"/>
       <c r="K80" s="27"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="27" t="s">
         <v>570</v>
       </c>
@@ -9892,7 +9966,7 @@
       <c r="J81" s="27"/>
       <c r="K81" s="27"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="27" t="s">
         <v>571</v>
       </c>
@@ -9907,7 +9981,7 @@
       <c r="J82" s="27"/>
       <c r="K82" s="27"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="27" t="s">
         <v>572</v>
       </c>
@@ -9922,7 +9996,7 @@
       <c r="J83" s="27"/>
       <c r="K83" s="27"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="27" t="s">
         <v>573</v>
       </c>
@@ -9937,7 +10011,7 @@
       <c r="J84" s="27"/>
       <c r="K84" s="27"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="27" t="s">
         <v>574</v>
       </c>
@@ -9952,7 +10026,7 @@
       <c r="J85" s="27"/>
       <c r="K85" s="27"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="27" t="s">
         <v>575</v>
       </c>
@@ -9967,7 +10041,7 @@
       <c r="J86" s="27"/>
       <c r="K86" s="27"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="27" t="s">
         <v>576</v>
       </c>
@@ -9982,7 +10056,7 @@
       <c r="J87" s="27"/>
       <c r="K87" s="27"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="27" t="s">
         <v>577</v>
       </c>
@@ -9997,7 +10071,7 @@
       <c r="J88" s="27"/>
       <c r="K88" s="27"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="27" t="s">
         <v>578</v>
       </c>
@@ -10012,7 +10086,7 @@
       <c r="J89" s="27"/>
       <c r="K89" s="27"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="27" t="s">
         <v>579</v>
       </c>
@@ -10027,7 +10101,7 @@
       <c r="J90" s="27"/>
       <c r="K90" s="27"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="27" t="s">
         <v>580</v>
       </c>
@@ -10042,7 +10116,7 @@
       <c r="J91" s="27"/>
       <c r="K91" s="27"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="27" t="s">
         <v>581</v>
       </c>
@@ -10057,7 +10131,7 @@
       <c r="J92" s="27"/>
       <c r="K92" s="27"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="27" t="s">
         <v>582</v>
       </c>
@@ -10072,7 +10146,7 @@
       <c r="J93" s="27"/>
       <c r="K93" s="27"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="27" t="s">
         <v>583</v>
       </c>
@@ -10087,7 +10161,7 @@
       <c r="J94" s="27"/>
       <c r="K94" s="27"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="27" t="s">
         <v>584</v>
       </c>
@@ -10102,7 +10176,7 @@
       <c r="J95" s="27"/>
       <c r="K95" s="27"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="27" t="s">
         <v>585</v>
       </c>
@@ -10117,7 +10191,7 @@
       <c r="J96" s="27"/>
       <c r="K96" s="27"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="27" t="s">
         <v>586</v>
       </c>
@@ -10132,7 +10206,7 @@
       <c r="J97" s="27"/>
       <c r="K97" s="27"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="27" t="s">
         <v>587</v>
       </c>
@@ -10147,7 +10221,7 @@
       <c r="J98" s="27"/>
       <c r="K98" s="27"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="27" t="s">
         <v>588</v>
       </c>
@@ -10162,7 +10236,7 @@
       <c r="J99" s="27"/>
       <c r="K99" s="27"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="27" t="s">
         <v>589</v>
       </c>
@@ -10177,7 +10251,7 @@
       <c r="J100" s="27"/>
       <c r="K100" s="27"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="27" t="s">
         <v>590</v>
       </c>
@@ -10192,7 +10266,7 @@
       <c r="J101" s="27"/>
       <c r="K101" s="27"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="27" t="s">
         <v>591</v>
       </c>
@@ -10207,7 +10281,7 @@
       <c r="J102" s="27"/>
       <c r="K102" s="27"/>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="27" t="s">
         <v>592</v>
       </c>
@@ -10222,7 +10296,7 @@
       <c r="J103" s="27"/>
       <c r="K103" s="27"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="27" t="s">
         <v>593</v>
       </c>
@@ -10237,7 +10311,7 @@
       <c r="J104" s="27"/>
       <c r="K104" s="27"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="27" t="s">
         <v>594</v>
       </c>
@@ -10252,7 +10326,7 @@
       <c r="J105" s="27"/>
       <c r="K105" s="27"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="27" t="s">
         <v>595</v>
       </c>
@@ -10267,7 +10341,7 @@
       <c r="J106" s="27"/>
       <c r="K106" s="27"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="27" t="s">
         <v>596</v>
       </c>
@@ -10282,7 +10356,7 @@
       <c r="J107" s="27"/>
       <c r="K107" s="27"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="27" t="s">
         <v>597</v>
       </c>
@@ -10297,7 +10371,7 @@
       <c r="J108" s="27"/>
       <c r="K108" s="27"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="27" t="s">
         <v>598</v>
       </c>
@@ -10312,7 +10386,7 @@
       <c r="J109" s="27"/>
       <c r="K109" s="27"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="27" t="s">
         <v>599</v>
       </c>
@@ -10327,7 +10401,7 @@
       <c r="J110" s="27"/>
       <c r="K110" s="27"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="27" t="s">
         <v>600</v>
       </c>
@@ -10342,7 +10416,7 @@
       <c r="J111" s="27"/>
       <c r="K111" s="27"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="27" t="s">
         <v>601</v>
       </c>
@@ -10357,7 +10431,7 @@
       <c r="J112" s="27"/>
       <c r="K112" s="27"/>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="27" t="s">
         <v>602</v>
       </c>
@@ -10372,7 +10446,7 @@
       <c r="J113" s="27"/>
       <c r="K113" s="27"/>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="27" t="s">
         <v>603</v>
       </c>
@@ -10387,7 +10461,7 @@
       <c r="J114" s="27"/>
       <c r="K114" s="27"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="27" t="s">
         <v>604</v>
       </c>
@@ -10402,7 +10476,7 @@
       <c r="J115" s="27"/>
       <c r="K115" s="27"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="27" t="s">
         <v>605</v>
       </c>
@@ -10417,7 +10491,7 @@
       <c r="J116" s="27"/>
       <c r="K116" s="27"/>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="27" t="s">
         <v>606</v>
       </c>
@@ -10432,7 +10506,7 @@
       <c r="J117" s="27"/>
       <c r="K117" s="27"/>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="27" t="s">
         <v>607</v>
       </c>
@@ -10447,7 +10521,7 @@
       <c r="J118" s="27"/>
       <c r="K118" s="27"/>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="27" t="s">
         <v>608</v>
       </c>
@@ -10462,7 +10536,7 @@
       <c r="J119" s="27"/>
       <c r="K119" s="27"/>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="27" t="s">
         <v>609</v>
       </c>
@@ -10477,7 +10551,7 @@
       <c r="J120" s="27"/>
       <c r="K120" s="27"/>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="27" t="s">
         <v>610</v>
       </c>
@@ -10492,7 +10566,7 @@
       <c r="J121" s="27"/>
       <c r="K121" s="27"/>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="27" t="s">
         <v>611</v>
       </c>
@@ -10507,7 +10581,7 @@
       <c r="J122" s="27"/>
       <c r="K122" s="27"/>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="27" t="s">
         <v>612</v>
       </c>
@@ -10522,7 +10596,7 @@
       <c r="J123" s="27"/>
       <c r="K123" s="27"/>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="27" t="s">
         <v>613</v>
       </c>
@@ -10537,7 +10611,7 @@
       <c r="J124" s="27"/>
       <c r="K124" s="27"/>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="27" t="s">
         <v>614</v>
       </c>
@@ -10552,7 +10626,7 @@
       <c r="J125" s="27"/>
       <c r="K125" s="27"/>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="27" t="s">
         <v>615</v>
       </c>
@@ -10567,7 +10641,7 @@
       <c r="J126" s="27"/>
       <c r="K126" s="27"/>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" s="27" t="s">
         <v>616</v>
       </c>
@@ -10582,7 +10656,7 @@
       <c r="J127" s="27"/>
       <c r="K127" s="27"/>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" s="27" t="s">
         <v>617</v>
       </c>
@@ -10597,7 +10671,7 @@
       <c r="J128" s="27"/>
       <c r="K128" s="27"/>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" s="27" t="s">
         <v>618</v>
       </c>
@@ -10612,7 +10686,7 @@
       <c r="J129" s="27"/>
       <c r="K129" s="27"/>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="27" t="s">
         <v>619</v>
       </c>
@@ -10627,7 +10701,7 @@
       <c r="J130" s="27"/>
       <c r="K130" s="27"/>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="27" t="s">
         <v>620</v>
       </c>
@@ -10642,7 +10716,7 @@
       <c r="J131" s="27"/>
       <c r="K131" s="27"/>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="27" t="s">
         <v>621</v>
       </c>
@@ -10657,7 +10731,7 @@
       <c r="J132" s="27"/>
       <c r="K132" s="27"/>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" s="27" t="s">
         <v>622</v>
       </c>
@@ -10672,7 +10746,7 @@
       <c r="J133" s="27"/>
       <c r="K133" s="27"/>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" s="27" t="s">
         <v>623</v>
       </c>
@@ -10687,7 +10761,7 @@
       <c r="J134" s="27"/>
       <c r="K134" s="27"/>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" s="27" t="s">
         <v>624</v>
       </c>
@@ -10702,7 +10776,7 @@
       <c r="J135" s="27"/>
       <c r="K135" s="27"/>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" s="27" t="s">
         <v>625</v>
       </c>
@@ -10717,7 +10791,7 @@
       <c r="J136" s="27"/>
       <c r="K136" s="27"/>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" s="27" t="s">
         <v>626</v>
       </c>
@@ -10732,7 +10806,7 @@
       <c r="J137" s="27"/>
       <c r="K137" s="27"/>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" s="27" t="s">
         <v>627</v>
       </c>
@@ -10747,7 +10821,7 @@
       <c r="J138" s="27"/>
       <c r="K138" s="27"/>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" s="27" t="s">
         <v>628</v>
       </c>
@@ -10762,7 +10836,7 @@
       <c r="J139" s="27"/>
       <c r="K139" s="27"/>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" s="27" t="s">
         <v>629</v>
       </c>
@@ -10777,7 +10851,7 @@
       <c r="J140" s="27"/>
       <c r="K140" s="27"/>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" s="27" t="s">
         <v>630</v>
       </c>
@@ -10792,7 +10866,7 @@
       <c r="J141" s="27"/>
       <c r="K141" s="27"/>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" s="27" t="s">
         <v>631</v>
       </c>
@@ -10807,7 +10881,7 @@
       <c r="J142" s="27"/>
       <c r="K142" s="27"/>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" s="27" t="s">
         <v>632</v>
       </c>
@@ -10822,7 +10896,7 @@
       <c r="J143" s="27"/>
       <c r="K143" s="27"/>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" s="27" t="s">
         <v>633</v>
       </c>
@@ -10837,7 +10911,7 @@
       <c r="J144" s="27"/>
       <c r="K144" s="27"/>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" s="27" t="s">
         <v>634</v>
       </c>
@@ -10852,7 +10926,7 @@
       <c r="J145" s="27"/>
       <c r="K145" s="27"/>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" s="27" t="s">
         <v>635</v>
       </c>
@@ -10867,7 +10941,7 @@
       <c r="J146" s="27"/>
       <c r="K146" s="27"/>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" s="27" t="s">
         <v>636</v>
       </c>
@@ -10882,7 +10956,7 @@
       <c r="J147" s="27"/>
       <c r="K147" s="27"/>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" s="27" t="s">
         <v>637</v>
       </c>
@@ -10897,7 +10971,7 @@
       <c r="J148" s="27"/>
       <c r="K148" s="27"/>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" s="27" t="s">
         <v>638</v>
       </c>
@@ -10912,7 +10986,7 @@
       <c r="J149" s="27"/>
       <c r="K149" s="27"/>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" s="27" t="s">
         <v>639</v>
       </c>
@@ -10927,7 +11001,7 @@
       <c r="J150" s="27"/>
       <c r="K150" s="27"/>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" s="27" t="s">
         <v>640</v>
       </c>
@@ -10942,7 +11016,7 @@
       <c r="J151" s="27"/>
       <c r="K151" s="27"/>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" s="27" t="s">
         <v>641</v>
       </c>
@@ -10957,7 +11031,7 @@
       <c r="J152" s="27"/>
       <c r="K152" s="27"/>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" s="27" t="s">
         <v>642</v>
       </c>
@@ -10972,7 +11046,7 @@
       <c r="J153" s="27"/>
       <c r="K153" s="27"/>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" s="27" t="s">
         <v>643</v>
       </c>
@@ -10987,7 +11061,7 @@
       <c r="J154" s="27"/>
       <c r="K154" s="27"/>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" s="27" t="s">
         <v>644</v>
       </c>
@@ -11002,7 +11076,7 @@
       <c r="J155" s="27"/>
       <c r="K155" s="27"/>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" s="27" t="s">
         <v>645</v>
       </c>
@@ -11017,7 +11091,7 @@
       <c r="J156" s="27"/>
       <c r="K156" s="27"/>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" s="27" t="s">
         <v>646</v>
       </c>
@@ -11032,7 +11106,7 @@
       <c r="J157" s="27"/>
       <c r="K157" s="27"/>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158" s="27" t="s">
         <v>647</v>
       </c>
@@ -11047,7 +11121,7 @@
       <c r="J158" s="27"/>
       <c r="K158" s="27"/>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159" s="27" t="s">
         <v>648</v>
       </c>
@@ -11062,7 +11136,7 @@
       <c r="J159" s="27"/>
       <c r="K159" s="27"/>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160" s="27" t="s">
         <v>649</v>
       </c>
@@ -11077,7 +11151,7 @@
       <c r="J160" s="27"/>
       <c r="K160" s="27"/>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" s="27" t="s">
         <v>650</v>
       </c>
@@ -11092,7 +11166,7 @@
       <c r="J161" s="27"/>
       <c r="K161" s="27"/>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" s="27" t="s">
         <v>651</v>
       </c>
@@ -11107,7 +11181,7 @@
       <c r="J162" s="27"/>
       <c r="K162" s="27"/>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" s="27" t="s">
         <v>652</v>
       </c>
@@ -11122,7 +11196,7 @@
       <c r="J163" s="27"/>
       <c r="K163" s="27"/>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" s="27" t="s">
         <v>653</v>
       </c>
@@ -11137,7 +11211,7 @@
       <c r="J164" s="27"/>
       <c r="K164" s="27"/>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165" s="27" t="s">
         <v>654</v>
       </c>
@@ -11167,19 +11241,19 @@
       <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="15.54296875" customWidth="1"/>
-    <col min="4" max="4" width="18.453125" customWidth="1"/>
-    <col min="5" max="5" width="21.81640625" customWidth="1"/>
-    <col min="6" max="6" width="26.81640625" customWidth="1"/>
-    <col min="7" max="9" width="15.54296875" customWidth="1"/>
-    <col min="10" max="10" width="13.08984375" customWidth="1"/>
-    <col min="11" max="11" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.36328125" customWidth="1"/>
+    <col min="1" max="3" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" customWidth="1"/>
+    <col min="7" max="9" width="15.5703125" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="16" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -11226,7 +11300,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="5" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -11273,7 +11347,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="5" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -11320,7 +11394,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="5" customFormat="1" ht="145" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" s="5" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -11367,7 +11441,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="5" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -11414,7 +11488,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="5" customFormat="1" ht="87" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" s="5" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -11461,7 +11535,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="5" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -11508,7 +11582,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="5" customFormat="1" ht="87" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" s="5" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -11555,7 +11629,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -11566,7 +11640,7 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -11577,7 +11651,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -11588,9 +11662,9 @@
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -11606,21 +11680,21 @@
       <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="15.54296875" style="21" customWidth="1"/>
-    <col min="4" max="4" width="18.453125" style="21" customWidth="1"/>
-    <col min="5" max="5" width="14.1796875" style="21" customWidth="1"/>
-    <col min="6" max="6" width="14.54296875" style="21" customWidth="1"/>
-    <col min="7" max="9" width="15.54296875" style="21" customWidth="1"/>
-    <col min="10" max="10" width="14.26953125" style="21" customWidth="1"/>
-    <col min="11" max="11" width="11.26953125" style="21" customWidth="1"/>
-    <col min="12" max="12" width="11.6328125" style="21" customWidth="1"/>
-    <col min="13" max="13" width="12.36328125" style="21" customWidth="1"/>
-    <col min="14" max="16384" width="8.7265625" style="21"/>
+    <col min="1" max="3" width="15.5703125" style="21" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" style="21" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" style="21" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="21" customWidth="1"/>
+    <col min="7" max="9" width="15.5703125" style="21" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" style="21" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" style="21" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" style="21" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" style="21" customWidth="1"/>
+    <col min="14" max="16384" width="8.7109375" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="23" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" s="23" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -11667,7 +11741,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="20" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" s="20" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="20">
         <v>1</v>
       </c>
@@ -11714,7 +11788,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="20" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="20">
         <v>2</v>
       </c>
@@ -11761,7 +11835,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="20" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" s="20" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="20">
         <v>3</v>
       </c>
@@ -11808,7 +11882,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="43" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" s="43" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="43">
         <v>4</v>
       </c>
@@ -11855,16 +11929,16 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11879,20 +11953,20 @@
       <selection pane="bottomLeft" activeCell="N1" sqref="N1:O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="15.54296875" customWidth="1"/>
-    <col min="4" max="4" width="18.453125" customWidth="1"/>
-    <col min="5" max="5" width="21.81640625" customWidth="1"/>
-    <col min="6" max="6" width="26.81640625" customWidth="1"/>
-    <col min="7" max="9" width="15.54296875" customWidth="1"/>
-    <col min="10" max="10" width="16.7265625" customWidth="1"/>
-    <col min="11" max="11" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.90625" customWidth="1"/>
-    <col min="13" max="13" width="15.90625" customWidth="1"/>
+    <col min="1" max="3" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" customWidth="1"/>
+    <col min="7" max="9" width="15.5703125" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" customWidth="1"/>
+    <col min="13" max="13" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="14" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -11939,7 +12013,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" ht="135" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -11986,7 +12060,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -12033,7 +12107,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="5" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" s="5" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -12080,7 +12154,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="5" customFormat="1" ht="174" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" s="5" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -12127,7 +12201,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="124.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" ht="124.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -12174,7 +12248,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="124.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" ht="124.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>5</v>
       </c>
@@ -12221,7 +12295,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>6</v>
       </c>
@@ -12268,7 +12342,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" ht="135" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>7</v>
       </c>
@@ -12315,7 +12389,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>8</v>
       </c>
@@ -12362,7 +12436,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" ht="135" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>9</v>
       </c>
@@ -12409,7 +12483,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" ht="135" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>10</v>
       </c>
@@ -12456,7 +12530,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" ht="135" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>11</v>
       </c>
@@ -12503,7 +12577,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" ht="135" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>12</v>
       </c>
@@ -12550,7 +12624,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" ht="135" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>13</v>
       </c>
@@ -12612,20 +12686,20 @@
       <selection pane="bottomLeft" activeCell="N1" sqref="N1:O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="15.54296875" customWidth="1"/>
-    <col min="4" max="4" width="18.453125" customWidth="1"/>
-    <col min="5" max="5" width="21.81640625" customWidth="1"/>
-    <col min="6" max="6" width="26.81640625" customWidth="1"/>
-    <col min="7" max="7" width="15.54296875" customWidth="1"/>
-    <col min="8" max="8" width="11.7265625" customWidth="1"/>
-    <col min="9" max="10" width="11.90625" customWidth="1"/>
-    <col min="12" max="12" width="12.26953125" customWidth="1"/>
-    <col min="13" max="13" width="12.54296875" customWidth="1"/>
+    <col min="1" max="3" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+    <col min="9" max="10" width="11.85546875" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="14" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -12672,7 +12746,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="116" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" ht="120" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -12719,7 +12793,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -12766,7 +12840,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="145" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" ht="150" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -12813,7 +12887,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="348" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" ht="360" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -12860,7 +12934,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -12907,7 +12981,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="87" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -12963,23 +13037,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D48F8994-0480-456C-9C73-8DEBC1CF05E8}">
   <dimension ref="A1:U26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T2" sqref="T2:U26"/>
+      <selection pane="bottomLeft" activeCell="N1" sqref="N1:U1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="15.54296875" customWidth="1"/>
-    <col min="4" max="4" width="18.453125" customWidth="1"/>
-    <col min="5" max="5" width="21.81640625" customWidth="1"/>
-    <col min="6" max="6" width="26.81640625" customWidth="1"/>
-    <col min="7" max="9" width="15.54296875" customWidth="1"/>
-    <col min="10" max="10" width="16.7265625" customWidth="1"/>
-    <col min="11" max="11" width="15.90625" customWidth="1"/>
+    <col min="1" max="3" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" customWidth="1"/>
+    <col min="7" max="9" width="15.5703125" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="26" customFormat="1" ht="24.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" s="26" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -13044,7 +13118,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -13109,7 +13183,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="87" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -13174,7 +13248,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -13239,7 +13313,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -13304,7 +13378,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -13369,7 +13443,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="58" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -13434,7 +13508,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -13499,7 +13573,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="58" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -13564,7 +13638,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -13629,7 +13703,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="58" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -13694,7 +13768,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -13759,7 +13833,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="145" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" ht="150" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -13824,7 +13898,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="145" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:21" ht="150" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -13889,7 +13963,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="203" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" ht="210" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -13954,7 +14028,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="87" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -14019,7 +14093,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:21" ht="165" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -14084,7 +14158,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="87" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:21" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -14149,7 +14223,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="87" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:21" ht="90" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -14214,7 +14288,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -14279,7 +14353,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -14344,7 +14418,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -14409,7 +14483,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -14474,7 +14548,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:21" ht="105" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -14539,7 +14613,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="87" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:21" ht="90" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -14604,7 +14678,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="58" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -14683,22 +14757,22 @@
       <selection pane="bottomLeft" activeCell="R2" sqref="R2:S9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="15.54296875" customWidth="1"/>
-    <col min="4" max="4" width="18.453125" customWidth="1"/>
-    <col min="5" max="5" width="13.36328125" customWidth="1"/>
-    <col min="6" max="6" width="14.453125" customWidth="1"/>
-    <col min="7" max="8" width="15.54296875" customWidth="1"/>
-    <col min="9" max="9" width="8.453125" customWidth="1"/>
-    <col min="10" max="10" width="12.54296875" customWidth="1"/>
+    <col min="1" max="3" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="7" max="8" width="15.5703125" customWidth="1"/>
+    <col min="9" max="9" width="8.42578125" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" customWidth="1"/>
     <col min="12" max="12" width="13" customWidth="1"/>
-    <col min="13" max="13" width="12.81640625" customWidth="1"/>
-    <col min="14" max="14" width="12.1796875" customWidth="1"/>
-    <col min="15" max="15" width="14.36328125" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" customWidth="1"/>
+    <col min="15" max="15" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="18" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -14757,7 +14831,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="87" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -14816,7 +14890,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="87" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -14875,7 +14949,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -14934,7 +15008,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -14993,7 +15067,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="145" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" ht="165" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -15052,7 +15126,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="87" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -15111,7 +15185,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="87" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -15170,7 +15244,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="87" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -15244,26 +15318,25 @@
       <selection pane="bottomLeft" activeCell="S1" sqref="A1:S1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="15.54296875" customWidth="1"/>
-    <col min="4" max="4" width="18.453125" customWidth="1"/>
-    <col min="5" max="5" width="21.81640625" customWidth="1"/>
-    <col min="6" max="6" width="26.81640625" customWidth="1"/>
-    <col min="7" max="7" width="15.54296875" customWidth="1"/>
-    <col min="8" max="9" width="18.36328125" customWidth="1"/>
-    <col min="10" max="10" width="16.7265625" customWidth="1"/>
-    <col min="11" max="11" width="21.08984375" customWidth="1"/>
-    <col min="12" max="12" width="17.81640625" customWidth="1"/>
-    <col min="13" max="13" width="17.1796875" customWidth="1"/>
-    <col min="14" max="14" width="17.36328125" customWidth="1"/>
-    <col min="15" max="16" width="17.453125" customWidth="1"/>
-    <col min="17" max="17" width="13.08984375" customWidth="1"/>
-    <col min="18" max="18" width="17.453125" customWidth="1"/>
-    <col min="19" max="19" width="13.7265625" customWidth="1"/>
+    <col min="1" max="3" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1"/>
+    <col min="8" max="9" width="18.42578125" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" customWidth="1"/>
+    <col min="11" max="11" width="21.140625" customWidth="1"/>
+    <col min="12" max="12" width="17.85546875" customWidth="1"/>
+    <col min="13" max="13" width="17.140625" customWidth="1"/>
+    <col min="14" max="16" width="17.42578125" customWidth="1"/>
+    <col min="17" max="17" width="13.140625" customWidth="1"/>
+    <col min="18" max="18" width="17.42578125" customWidth="1"/>
+    <col min="19" max="19" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="14" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" s="14" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -15322,7 +15395,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="145" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" ht="150" x14ac:dyDescent="0.25">
       <c r="A2" s="11">
         <v>1</v>
       </c>
@@ -15381,7 +15454,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="145" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" ht="150" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>2</v>
       </c>
@@ -15440,7 +15513,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="145" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" ht="150" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
         <v>3</v>
       </c>
@@ -15499,7 +15572,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="145" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" ht="150" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
         <v>4</v>
       </c>
@@ -15558,7 +15631,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="174" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" ht="180" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <v>5</v>
       </c>
@@ -15617,7 +15690,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="145" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" ht="150" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <v>6</v>
       </c>
@@ -15676,7 +15749,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="145" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" ht="150" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
         <v>7</v>
       </c>
@@ -15735,7 +15808,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="145" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19" ht="150" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
         <v>8</v>
       </c>
@@ -15794,7 +15867,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="145" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:19" ht="150" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
         <v>9</v>
       </c>
@@ -15853,7 +15926,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="145" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:19" ht="150" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
         <v>10</v>
       </c>
@@ -15912,7 +15985,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="145" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:19" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
         <v>11</v>
       </c>
@@ -15971,7 +16044,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="145" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:19" ht="150" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
         <v>12</v>
       </c>
@@ -16030,7 +16103,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="145" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:19" ht="150" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
         <v>13</v>
       </c>
@@ -16089,7 +16162,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="145" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:19" ht="150" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
         <v>14</v>
       </c>
@@ -16148,7 +16221,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="145" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:19" ht="165" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
         <v>15</v>
       </c>
@@ -16207,7 +16280,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="145" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:19" ht="150" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
         <v>16</v>
       </c>
@@ -16266,7 +16339,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="145" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:19" ht="150" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
         <v>17</v>
       </c>
@@ -16325,7 +16398,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="145" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:19" ht="150" x14ac:dyDescent="0.25">
       <c r="A19" s="11">
         <v>18</v>
       </c>
@@ -16384,7 +16457,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="145" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:19" ht="165" x14ac:dyDescent="0.25">
       <c r="A20" s="11">
         <v>19</v>
       </c>
@@ -16443,7 +16516,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="145" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:19" ht="165" x14ac:dyDescent="0.25">
       <c r="A21" s="11">
         <v>20</v>
       </c>
@@ -16502,7 +16575,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="145" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:19" ht="165" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
         <v>21</v>
       </c>
@@ -16561,7 +16634,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:19" ht="165" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
         <v>22</v>
       </c>
@@ -16620,7 +16693,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:19" ht="165" x14ac:dyDescent="0.25">
       <c r="A24" s="11">
         <v>23</v>
       </c>
@@ -16679,7 +16752,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:19" ht="165" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
         <v>24</v>
       </c>
@@ -16738,7 +16811,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="42" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:19" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A26" s="11">
         <v>25</v>
       </c>
@@ -16785,7 +16858,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="145" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:19" ht="150" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
         <v>26</v>
       </c>
@@ -16844,7 +16917,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="145" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:19" ht="150" x14ac:dyDescent="0.25">
       <c r="A28" s="11">
         <v>27</v>
       </c>
@@ -16903,7 +16976,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="145" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:19" ht="150" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
         <v>28</v>
       </c>
@@ -16962,7 +17035,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:19" ht="360" x14ac:dyDescent="0.25">
       <c r="A30" s="11">
         <v>29</v>
       </c>
@@ -17018,9 +17091,9 @@
       <selection pane="bottomLeft" activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:17" s="14" customFormat="1" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:17" s="14" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -17073,7 +17146,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="126.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:17" ht="129" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
         <v>464</v>
       </c>
@@ -17114,7 +17187,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="126.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:17" ht="129" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="32" t="s">
         <v>506</v>
       </c>
@@ -17155,7 +17228,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="126.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:17" ht="129" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="32" t="s">
         <v>516</v>
       </c>
@@ -17204,18 +17277,18 @@
       <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="80" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="8.7265625" style="39"/>
-    <col min="4" max="4" width="23.1796875" style="39" customWidth="1"/>
-    <col min="5" max="5" width="20.08984375" style="39" customWidth="1"/>
-    <col min="6" max="6" width="5.54296875" style="39" customWidth="1"/>
-    <col min="7" max="7" width="23.6328125" style="39" customWidth="1"/>
-    <col min="8" max="8" width="20.1796875" style="39" customWidth="1"/>
-    <col min="9" max="16384" width="8.7265625" style="39"/>
+    <col min="1" max="3" width="8.7109375" style="39"/>
+    <col min="4" max="4" width="23.140625" style="39" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" style="39" customWidth="1"/>
+    <col min="6" max="6" width="5.5703125" style="39" customWidth="1"/>
+    <col min="7" max="7" width="23.5703125" style="39" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" style="39" customWidth="1"/>
+    <col min="9" max="16384" width="8.7109375" style="39"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="41" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" s="41" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
@@ -17262,7 +17335,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="120.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" ht="120.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
         <v>429</v>
       </c>
@@ -17287,7 +17360,7 @@
       <c r="J2" s="27"/>
       <c r="K2" s="27"/>
     </row>
-    <row r="3" spans="1:15" ht="147.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" ht="147.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
         <v>453</v>
       </c>
@@ -17310,7 +17383,7 @@
       <c r="H3" s="38"/>
       <c r="I3" s="40"/>
     </row>
-    <row r="4" spans="1:15" ht="80" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="38" t="s">
         <v>537</v>
       </c>
@@ -17341,15 +17414,15 @@
       <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.6328125" defaultRowHeight="80" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.1796875" customWidth="1"/>
-    <col min="2" max="2" width="12.453125" customWidth="1"/>
-    <col min="3" max="3" width="9.6328125" customWidth="1"/>
-    <col min="4" max="4" width="11.26953125" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="14" customFormat="1" ht="26" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:26" s="14" customFormat="1" ht="26.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -17396,7 +17469,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="115.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:26" ht="115.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
         <v>456</v>
       </c>
@@ -17440,7 +17513,7 @@
       <c r="Y2" s="32"/>
       <c r="Z2" s="32"/>
     </row>
-    <row r="3" spans="1:26" ht="110" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:26" ht="110.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="32" t="s">
         <v>552</v>
       </c>
@@ -17489,27 +17562,27 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF7BFF7B-5E59-40FB-93C7-19664CC11324}">
-  <dimension ref="A1:Z29"/>
+  <dimension ref="A1:AB29"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="Y7" sqref="Y7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="60" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="60" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="21"/>
-    <col min="2" max="2" width="11.81640625" style="21" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" style="21"/>
-    <col min="4" max="4" width="12.54296875" style="21" customWidth="1"/>
-    <col min="5" max="5" width="18.54296875" style="21" customWidth="1"/>
-    <col min="6" max="6" width="21.26953125" style="21" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" style="21"/>
+    <col min="2" max="2" width="11.85546875" style="21" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="21"/>
+    <col min="4" max="4" width="12.5703125" style="21" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" style="21" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" style="21" customWidth="1"/>
     <col min="7" max="7" width="18" style="21" customWidth="1"/>
-    <col min="8" max="8" width="26.54296875" style="21" customWidth="1"/>
-    <col min="9" max="16384" width="8.7265625" style="21"/>
+    <col min="8" max="8" width="26.5703125" style="21" customWidth="1"/>
+    <col min="9" max="16384" width="8.7109375" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="19" customFormat="1" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:28" s="19" customFormat="1" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
@@ -17549,8 +17622,38 @@
       <c r="M1" s="22" t="s">
         <v>817</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N1" s="24" t="s">
+        <v>847</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>807</v>
+      </c>
+      <c r="P1" s="24" t="s">
+        <v>849</v>
+      </c>
+      <c r="Q1" s="13" t="s">
+        <v>850</v>
+      </c>
+      <c r="R1" s="24" t="s">
+        <v>848</v>
+      </c>
+      <c r="S1" s="13" t="s">
+        <v>822</v>
+      </c>
+      <c r="T1" s="24" t="s">
+        <v>843</v>
+      </c>
+      <c r="U1" s="13" t="s">
+        <v>831</v>
+      </c>
+      <c r="V1" s="24" t="s">
+        <v>844</v>
+      </c>
+      <c r="W1" s="13" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
         <v>460</v>
       </c>
@@ -17590,21 +17693,43 @@
       <c r="M2" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="33"/>
-      <c r="V2" s="33"/>
-      <c r="W2" s="33"/>
+      <c r="N2" s="33" t="s">
+        <v>686</v>
+      </c>
+      <c r="O2" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2" s="33" t="s">
+        <v>851</v>
+      </c>
+      <c r="Q2" s="33" t="s">
+        <v>260</v>
+      </c>
+      <c r="R2" s="33" t="s">
+        <v>851</v>
+      </c>
+      <c r="S2" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="T2" s="33" t="s">
+        <v>851</v>
+      </c>
+      <c r="U2" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="V2" s="33" t="s">
+        <v>851</v>
+      </c>
+      <c r="W2" s="33" t="s">
+        <v>8</v>
+      </c>
       <c r="X2" s="33"/>
       <c r="Y2" s="33"/>
       <c r="Z2" s="33"/>
-    </row>
-    <row r="3" spans="1:26" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AA2" s="33"/>
+      <c r="AB2" s="33"/>
+    </row>
+    <row r="3" spans="1:28" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
         <v>511</v>
       </c>
@@ -17644,21 +17769,43 @@
       <c r="M3" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="33"/>
-      <c r="O3" s="33"/>
-      <c r="P3" s="33"/>
-      <c r="Q3" s="33"/>
-      <c r="R3" s="33"/>
-      <c r="S3" s="33"/>
-      <c r="T3" s="33"/>
-      <c r="U3" s="33"/>
-      <c r="V3" s="33"/>
-      <c r="W3" s="33"/>
+      <c r="N3" s="33" t="s">
+        <v>686</v>
+      </c>
+      <c r="O3" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3" s="33" t="s">
+        <v>851</v>
+      </c>
+      <c r="Q3" s="33" t="s">
+        <v>260</v>
+      </c>
+      <c r="R3" s="33" t="s">
+        <v>851</v>
+      </c>
+      <c r="S3" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="T3" s="33" t="s">
+        <v>851</v>
+      </c>
+      <c r="U3" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="V3" s="33" t="s">
+        <v>851</v>
+      </c>
+      <c r="W3" s="33" t="s">
+        <v>8</v>
+      </c>
       <c r="X3" s="33"/>
       <c r="Y3" s="33"/>
       <c r="Z3" s="33"/>
-    </row>
-    <row r="4" spans="1:26" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AA3" s="33"/>
+      <c r="AB3" s="33"/>
+    </row>
+    <row r="4" spans="1:28" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
         <v>523</v>
       </c>
@@ -17698,21 +17845,43 @@
       <c r="M4" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="N4" s="33"/>
-      <c r="O4" s="33"/>
-      <c r="P4" s="33"/>
-      <c r="Q4" s="33"/>
-      <c r="R4" s="33"/>
-      <c r="S4" s="33"/>
-      <c r="T4" s="33"/>
-      <c r="U4" s="33"/>
-      <c r="V4" s="33"/>
-      <c r="W4" s="33"/>
-      <c r="X4" s="33"/>
-      <c r="Y4" s="33"/>
-      <c r="Z4" s="33"/>
-    </row>
-    <row r="5" spans="1:26" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N4" s="33" t="s">
+        <v>686</v>
+      </c>
+      <c r="O4" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="P4" s="33" t="s">
+        <v>851</v>
+      </c>
+      <c r="Q4" s="33" t="s">
+        <v>260</v>
+      </c>
+      <c r="R4" s="33" t="s">
+        <v>851</v>
+      </c>
+      <c r="S4" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="T4" s="33" t="s">
+        <v>851</v>
+      </c>
+      <c r="U4" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="V4" s="33" t="s">
+        <v>851</v>
+      </c>
+      <c r="W4" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="X4" s="47"/>
+      <c r="Y4" s="47"/>
+      <c r="Z4" s="47"/>
+      <c r="AA4" s="47"/>
+      <c r="AB4" s="47"/>
+    </row>
+    <row r="5" spans="1:28" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="21">
         <v>16</v>
       </c>
@@ -17750,20 +17919,100 @@
       <c r="M5" s="31" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:26" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N5" s="31" t="s">
+        <v>693</v>
+      </c>
+      <c r="O5" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="P5" s="31" t="s">
+        <v>693</v>
+      </c>
+      <c r="Q5" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="R5" s="31" t="s">
+        <v>693</v>
+      </c>
+      <c r="S5" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="T5" s="31" t="s">
+        <v>693</v>
+      </c>
+      <c r="U5" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="V5" s="31" t="s">
+        <v>693</v>
+      </c>
+      <c r="W5" s="31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="31"/>
       <c r="C6" s="31"/>
       <c r="D6" s="31"/>
       <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
-    </row>
-    <row r="7" spans="1:26" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F6" s="31" t="s">
+        <v>852</v>
+      </c>
+      <c r="G6" s="31" t="s">
+        <v>671</v>
+      </c>
+      <c r="H6" s="31" t="s">
+        <v>686</v>
+      </c>
+      <c r="I6" s="31" t="s">
+        <v>260</v>
+      </c>
+      <c r="J6" s="31" t="s">
+        <v>671</v>
+      </c>
+      <c r="K6" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="L6" s="31" t="s">
+        <v>671</v>
+      </c>
+      <c r="M6" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="N6" s="31" t="s">
+        <v>671</v>
+      </c>
+      <c r="O6" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="P6" s="31" t="s">
+        <v>671</v>
+      </c>
+      <c r="Q6" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="R6" s="31" t="s">
+        <v>671</v>
+      </c>
+      <c r="S6" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="T6" s="31" t="s">
+        <v>671</v>
+      </c>
+      <c r="U6" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="V6" s="31" t="s">
+        <v>671</v>
+      </c>
+      <c r="W6" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="X6" s="31"/>
+      <c r="Y6" s="31"/>
+    </row>
+    <row r="7" spans="1:28" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="31"/>
       <c r="C7" s="31"/>
       <c r="D7" s="31"/>
@@ -17775,7 +18024,7 @@
       <c r="J7" s="31"/>
       <c r="K7" s="31"/>
     </row>
-    <row r="8" spans="1:26" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:28" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="31"/>
       <c r="C8" s="31"/>
       <c r="D8" s="31"/>
@@ -17787,7 +18036,7 @@
       <c r="J8" s="31"/>
       <c r="K8" s="31"/>
     </row>
-    <row r="9" spans="1:26" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:28" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="31"/>
       <c r="C9" s="31"/>
       <c r="D9" s="31"/>
@@ -17799,7 +18048,7 @@
       <c r="J9" s="31"/>
       <c r="K9" s="31"/>
     </row>
-    <row r="10" spans="1:26" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:28" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="31"/>
       <c r="C10" s="31"/>
       <c r="D10" s="31"/>
@@ -17811,7 +18060,7 @@
       <c r="J10" s="31"/>
       <c r="K10" s="31"/>
     </row>
-    <row r="11" spans="1:26" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:28" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="31"/>
       <c r="C11" s="31"/>
       <c r="D11" s="31"/>
@@ -17823,7 +18072,7 @@
       <c r="J11" s="31"/>
       <c r="K11" s="31"/>
     </row>
-    <row r="12" spans="1:26" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:28" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="31"/>
       <c r="C12" s="31"/>
       <c r="D12" s="31"/>
@@ -17835,7 +18084,7 @@
       <c r="J12" s="31"/>
       <c r="K12" s="31"/>
     </row>
-    <row r="13" spans="1:26" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:28" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="31"/>
       <c r="C13" s="31"/>
       <c r="D13" s="31"/>
@@ -17847,82 +18096,82 @@
       <c r="J13" s="31"/>
       <c r="K13" s="31"/>
     </row>
-    <row r="14" spans="1:26" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:28" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I14" s="31"/>
       <c r="J14" s="31"/>
       <c r="K14" s="31"/>
     </row>
-    <row r="15" spans="1:26" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:28" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I15" s="31"/>
       <c r="J15" s="31"/>
       <c r="K15" s="31"/>
     </row>
-    <row r="16" spans="1:26" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:28" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I16" s="31"/>
       <c r="J16" s="31"/>
       <c r="K16" s="31"/>
     </row>
-    <row r="17" spans="9:11" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="9:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I17" s="31"/>
       <c r="J17" s="31"/>
       <c r="K17" s="31"/>
     </row>
-    <row r="18" spans="9:11" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="9:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I18" s="31"/>
       <c r="J18" s="31"/>
       <c r="K18" s="31"/>
     </row>
-    <row r="19" spans="9:11" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="9:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I19" s="31"/>
       <c r="J19" s="31"/>
       <c r="K19" s="31"/>
     </row>
-    <row r="20" spans="9:11" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="9:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I20" s="31"/>
       <c r="J20" s="31"/>
       <c r="K20" s="31"/>
     </row>
-    <row r="21" spans="9:11" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="9:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I21" s="31"/>
       <c r="J21" s="31"/>
       <c r="K21" s="31"/>
     </row>
-    <row r="22" spans="9:11" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="9:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I22" s="31"/>
       <c r="J22" s="31"/>
       <c r="K22" s="31"/>
     </row>
-    <row r="23" spans="9:11" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="9:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I23" s="31"/>
       <c r="J23" s="31"/>
       <c r="K23" s="31"/>
     </row>
-    <row r="24" spans="9:11" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="9:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I24" s="31"/>
       <c r="J24" s="31"/>
       <c r="K24" s="31"/>
     </row>
-    <row r="25" spans="9:11" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="9:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I25" s="31"/>
       <c r="J25" s="31"/>
       <c r="K25" s="31"/>
     </row>
-    <row r="26" spans="9:11" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="9:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I26" s="31"/>
       <c r="J26" s="31"/>
       <c r="K26" s="31"/>
     </row>
-    <row r="27" spans="9:11" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="9:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I27" s="31"/>
       <c r="J27" s="31"/>
       <c r="K27" s="31"/>
     </row>
-    <row r="28" spans="9:11" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="9:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I28" s="31"/>
       <c r="J28" s="31"/>
       <c r="K28" s="31"/>
     </row>
-    <row r="29" spans="9:11" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="9:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I29" s="31"/>
       <c r="J29" s="31"/>
       <c r="K29" s="31"/>
@@ -17942,19 +18191,19 @@
       <selection pane="bottomLeft" activeCell="Q1" sqref="A1:Q1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6328125" defaultRowHeight="50" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.5703125" defaultRowHeight="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="10.6328125" style="21"/>
-    <col min="5" max="5" width="15.36328125" style="21" customWidth="1"/>
+    <col min="1" max="4" width="10.5703125" style="21"/>
+    <col min="5" max="5" width="15.42578125" style="21" customWidth="1"/>
     <col min="6" max="6" width="17" style="21" customWidth="1"/>
     <col min="7" max="7" width="18" style="21" customWidth="1"/>
-    <col min="8" max="8" width="21.7265625" style="21" customWidth="1"/>
-    <col min="9" max="15" width="10.6328125" style="21"/>
-    <col min="16" max="16" width="16.1796875" style="21" customWidth="1"/>
-    <col min="17" max="16384" width="10.6328125" style="21"/>
+    <col min="8" max="8" width="21.7109375" style="21" customWidth="1"/>
+    <col min="9" max="15" width="10.5703125" style="21"/>
+    <col min="16" max="16" width="16.140625" style="21" customWidth="1"/>
+    <col min="17" max="16384" width="10.5703125" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="19" customFormat="1" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:26" s="19" customFormat="1" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -18007,7 +18256,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:26" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
         <v>349</v>
       </c>
@@ -18060,7 +18309,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:26" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="32" t="s">
         <v>356</v>
       </c>
@@ -18113,7 +18362,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:26" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="32" t="s">
         <v>363</v>
       </c>
@@ -18166,7 +18415,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:26" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="32" t="s">
         <v>370</v>
       </c>
@@ -18219,7 +18468,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:26" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="32" t="s">
         <v>375</v>
       </c>
@@ -18272,7 +18521,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:26" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="32" t="s">
         <v>380</v>
       </c>
@@ -18325,7 +18574,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:26" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="32" t="s">
         <v>386</v>
       </c>
@@ -18378,7 +18627,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:26" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="32" t="s">
         <v>393</v>
       </c>
@@ -18431,7 +18680,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:26" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="32" t="s">
         <v>399</v>
       </c>
@@ -18484,7 +18733,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:26" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="32" t="s">
         <v>423</v>
       </c>
@@ -18546,7 +18795,7 @@
       <c r="Y11" s="32"/>
       <c r="Z11" s="32"/>
     </row>
-    <row r="12" spans="1:26" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:26" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="32" t="s">
         <v>443</v>
       </c>
@@ -18608,7 +18857,7 @@
       <c r="Y12" s="32"/>
       <c r="Z12" s="32"/>
     </row>
-    <row r="13" spans="1:26" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:26" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="32" t="s">
         <v>478</v>
       </c>
@@ -18661,7 +18910,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:26" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="32" t="s">
         <v>484</v>
       </c>
@@ -18714,7 +18963,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:26" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="32" t="s">
         <v>489</v>
       </c>
@@ -18767,7 +19016,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:26" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="32" t="s">
         <v>495</v>
       </c>
@@ -18820,7 +19069,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:17" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="32" t="s">
         <v>501</v>
       </c>
@@ -18873,7 +19122,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:17" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="34"/>
       <c r="B18" s="34"/>
       <c r="C18" s="34"/>
@@ -18883,7 +19132,7 @@
       <c r="G18" s="34"/>
       <c r="H18" s="34"/>
     </row>
-    <row r="19" spans="1:17" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:17" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="34"/>
       <c r="B19" s="34"/>
       <c r="C19" s="34"/>
@@ -18893,7 +19142,7 @@
       <c r="G19" s="34"/>
       <c r="H19" s="34"/>
     </row>
-    <row r="20" spans="1:17" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:17" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="34"/>
       <c r="B20" s="34"/>
       <c r="C20" s="34"/>
@@ -18903,7 +19152,7 @@
       <c r="G20" s="34"/>
       <c r="H20" s="34"/>
     </row>
-    <row r="21" spans="1:17" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:17" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="34"/>
       <c r="B21" s="34"/>
       <c r="C21" s="34"/>
@@ -18913,7 +19162,7 @@
       <c r="G21" s="34"/>
       <c r="H21" s="34"/>
     </row>
-    <row r="22" spans="1:17" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:17" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="34"/>
       <c r="B22" s="34"/>
       <c r="C22" s="34"/>
@@ -18923,7 +19172,7 @@
       <c r="G22" s="34"/>
       <c r="H22" s="34"/>
     </row>
-    <row r="23" spans="1:17" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:17" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="34"/>
       <c r="B23" s="35"/>
       <c r="C23" s="34"/>
@@ -18933,7 +19182,7 @@
       <c r="G23" s="34"/>
       <c r="H23" s="34"/>
     </row>
-    <row r="24" spans="1:17" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:17" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="34"/>
       <c r="B24" s="34"/>
       <c r="C24" s="34"/>
@@ -18943,7 +19192,7 @@
       <c r="G24" s="34"/>
       <c r="H24" s="34"/>
     </row>
-    <row r="25" spans="1:17" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:17" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="34"/>
       <c r="B25" s="34"/>
       <c r="C25" s="34"/>
@@ -18953,7 +19202,7 @@
       <c r="G25" s="34"/>
       <c r="H25" s="34"/>
     </row>
-    <row r="26" spans="1:17" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:17" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="34"/>
       <c r="B26" s="34"/>
       <c r="C26" s="34"/>
@@ -18963,7 +19212,7 @@
       <c r="G26" s="34"/>
       <c r="H26" s="34"/>
     </row>
-    <row r="27" spans="1:17" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:17" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="34"/>
       <c r="B27" s="34"/>
       <c r="C27" s="34"/>
@@ -18973,7 +19222,7 @@
       <c r="G27" s="34"/>
       <c r="H27" s="34"/>
     </row>
-    <row r="28" spans="1:17" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:17" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="34"/>
       <c r="B28" s="34"/>
       <c r="C28" s="34"/>
@@ -18983,7 +19232,7 @@
       <c r="G28" s="34"/>
       <c r="H28" s="34"/>
     </row>
-    <row r="29" spans="1:17" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:17" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="34"/>
       <c r="B29" s="34"/>
       <c r="C29" s="34"/>
@@ -18993,7 +19242,7 @@
       <c r="G29" s="34"/>
       <c r="H29" s="34"/>
     </row>
-    <row r="30" spans="1:17" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:17" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="34"/>
       <c r="B30" s="34"/>
       <c r="C30" s="34"/>
@@ -19017,9 +19266,9 @@
       <selection pane="bottomLeft" activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" s="14" customFormat="1" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" s="14" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -19060,7 +19309,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="76.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" ht="78" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
         <v>439</v>
       </c>
@@ -19101,7 +19350,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="76.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" ht="78" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="32" t="s">
         <v>532</v>
       </c>
@@ -19156,9 +19405,9 @@
       <selection pane="bottomLeft" activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" s="37" customFormat="1" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" s="37" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -19199,7 +19448,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="76.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" ht="78" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
         <v>434</v>
       </c>
@@ -19240,7 +19489,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="76.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" ht="78" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="32" t="s">
         <v>473</v>
       </c>
@@ -19294,14 +19543,14 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="10.36328125" customWidth="1"/>
-    <col min="7" max="7" width="18.6328125" customWidth="1"/>
-    <col min="8" max="8" width="17.54296875" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -19336,7 +19585,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="45">
         <v>1</v>
       </c>
@@ -19365,7 +19614,7 @@
       <c r="J2" s="45"/>
       <c r="K2" s="45"/>
     </row>
-    <row r="3" spans="1:11" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A3" s="45">
         <v>2</v>
       </c>
@@ -19394,7 +19643,7 @@
       <c r="J3" s="45"/>
       <c r="K3" s="45"/>
     </row>
-    <row r="4" spans="1:11" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -19423,7 +19672,7 @@
       <c r="J4" s="45"/>
       <c r="K4" s="45"/>
     </row>
-    <row r="5" spans="1:11" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -19452,7 +19701,7 @@
       <c r="J5" s="45"/>
       <c r="K5" s="45"/>
     </row>
-    <row r="6" spans="1:11" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -19481,7 +19730,7 @@
       <c r="J6" s="45"/>
       <c r="K6" s="45"/>
     </row>
-    <row r="7" spans="1:11" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -19510,7 +19759,7 @@
       <c r="J7" s="45"/>
       <c r="K7" s="45"/>
     </row>
-    <row r="8" spans="1:11" ht="325" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="344.25" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Update testcases (drop section) (manual & json)
Co-Authored-By: seehoe <seehoe@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/testing/testcases.xlsx
+++ b/testing/testcases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\project-g5t4\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE0EC1EA-71A3-4C4A-BC44-B9A109B4E67C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7788A7DF-1CE2-4D4C-B68B-3C7F9AEAE76D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="844" activeTab="4" xr2:uid="{F747292D-6CBE-43A0-AF24-F2F7C25CEB64}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="844" activeTab="1" xr2:uid="{F747292D-6CBE-43A0-AF24-F2F7C25CEB64}"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 3 - JSON - BidDump" sheetId="20" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3086" uniqueCount="853">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3135" uniqueCount="886">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -6800,6 +6800,132 @@
   </si>
   <si>
     <t>r={"course": "IS100","section": "S11"}</t>
+  </si>
+  <si>
+    <t>call Json_checker dump.php for 041-drop-section.txt</t>
+  </si>
+  <si>
+    <t>call Json_checker dump.php for 052-drop-section.txt</t>
+  </si>
+  <si>
+    <t>call Json_checker dump.php for 054-drop-section.txt</t>
+  </si>
+  <si>
+    <t>call Json_checker dump.php for 055-drop-section.txt</t>
+  </si>
+  <si>
+    <t>call Json_checker dump.php for 056-drop-section.txt</t>
+  </si>
+  <si>
+    <t>r={"userid":"amy.ng.2009","course":"IS100","section":"S1"}</t>
+  </si>
+  <si>
+    <t>r={"userid": "amy.ng.2009","course": "IS100","section": "S1"}</t>
+  </si>
+  <si>
+    <t>r={"userid":"amy.ng.2009","course":"IS1000","section":"S1"}</t>
+  </si>
+  <si>
+    <t>r={"userid":"amy.ng.2009","course":"IS100","section":"S100"}</t>
+  </si>
+  <si>
+    <t>{
+    "status": "error",
+    "message": [
+        "round not active"
+    ]
+}</t>
+  </si>
+  <si>
+    <t>Pass/Fail 17/10/19</t>
+  </si>
+  <si>
+    <t>{
+    "status": "error",
+    "message": [
+        "invalid userid"
+    ]
+}</t>
+  </si>
+  <si>
+    <t>{
+    "status": "success"
+}</t>
+  </si>
+  <si>
+    <t>{
+    "status": "error",
+    "message": [
+        "invalid course"
+    ]
+}</t>
+  </si>
+  <si>
+    <t>{
+    "status": "error",
+    "message": [
+        "invalid section"
+    ]
+}</t>
+  </si>
+  <si>
+    <t>Admin try to drop a section that student enrolled with an incorrect userid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admin can drop a section that a student had enrolled when round is inactive </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admin can drop a section that a student had enrolled when round is active </t>
+  </si>
+  <si>
+    <t>admin drop a section that a student enrolled with an invalid course code</t>
+  </si>
+  <si>
+    <t>admin drop a section that a student enrolled with an invalid section code</t>
+  </si>
+  <si>
+    <t>drop section by proiding a student userid, section &amp; course enrolled, when round is inactive</t>
+  </si>
+  <si>
+    <t>drop section by proiding a incorrect student userid, correct section &amp; course enrolled, when round is active</t>
+  </si>
+  <si>
+    <t>drop section by proiding a correct student userid, correct section &amp; course enrolled, when round is active</t>
+  </si>
+  <si>
+    <t>drop section by proiding a correct student userid, correct section &amp; incorrect course enrolled, when round is active</t>
+  </si>
+  <si>
+    <t>drop section by proiding a correct student userid, inccorrect section &amp; correct course enrolled, when round is active</t>
+  </si>
+  <si>
+    <t>Assume it is bootstrappedm bids are placed &amp; it is either round 1 or round 2 and inactive</t>
+  </si>
+  <si>
+    <t>Assume it is bootstrappedm bids are placed &amp; it is round 2 and active</t>
+  </si>
+  <si>
+    <t>Result 1 17/10/19</t>
+  </si>
+  <si>
+    <t>Result 2 22/10/19</t>
+  </si>
+  <si>
+    <t>Result 5 9/11/19</t>
+  </si>
+  <si>
+    <t>Pass/Fail 29/10/19</t>
+  </si>
+  <si>
+    <t>Result 3 29/10/19</t>
+  </si>
+  <si>
+    <t>{
+    "status": "error",
+    "message": [
+        "no such enrollment record"
+    ]
+}</t>
   </si>
 </sst>
 </file>
@@ -6947,7 +7073,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -7079,6 +7205,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -17084,16 +17213,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4E86E5B-DBBE-4F0A-9FF6-23DFDAE91C03}">
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView zoomScale="87" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="87" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="9.85546875" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" customWidth="1"/>
+    <col min="11" max="13" width="9.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="14" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -17116,22 +17251,22 @@
         <v>6</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>799</v>
+        <v>880</v>
       </c>
       <c r="I1" s="22" t="s">
-        <v>793</v>
+        <v>863</v>
       </c>
       <c r="J1" s="22" t="s">
-        <v>800</v>
+        <v>881</v>
       </c>
       <c r="K1" s="22" t="s">
-        <v>801</v>
+        <v>817</v>
       </c>
       <c r="L1" s="22" t="s">
-        <v>816</v>
+        <v>884</v>
       </c>
       <c r="M1" s="22" t="s">
-        <v>817</v>
+        <v>883</v>
       </c>
       <c r="N1" s="22" t="s">
         <v>826</v>
@@ -17140,126 +17275,274 @@
         <v>828</v>
       </c>
       <c r="P1" s="22" t="s">
-        <v>829</v>
+        <v>882</v>
       </c>
       <c r="Q1" s="22" t="s">
         <v>830</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="129" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="32" t="s">
+    <row r="2" spans="1:17" ht="195" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>464</v>
       </c>
-      <c r="B2" s="32" t="s">
-        <v>465</v>
-      </c>
-      <c r="C2" s="32" t="s">
-        <v>466</v>
-      </c>
-      <c r="D2" s="32" t="s">
-        <v>467</v>
-      </c>
-      <c r="E2" s="32" t="s">
-        <v>468</v>
-      </c>
-      <c r="F2" s="32" t="s">
+      <c r="B2" s="5" t="s">
+        <v>869</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>873</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>878</v>
+      </c>
+      <c r="E2" s="38" t="s">
+        <v>853</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>858</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>862</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>862</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>862</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>862</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>862</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>862</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="225" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>506</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>868</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>874</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>879</v>
+      </c>
+      <c r="E3" s="38" t="s">
+        <v>854</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>668</v>
       </c>
-      <c r="G2" s="32" t="s">
-        <v>687</v>
-      </c>
-      <c r="H2" s="32" t="s">
-        <v>687</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="32" t="s">
-        <v>687</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="L2" s="32" t="s">
-        <v>687</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="129" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="32" t="s">
-        <v>506</v>
-      </c>
-      <c r="B3" s="32" t="s">
-        <v>507</v>
-      </c>
-      <c r="C3" s="32" t="s">
-        <v>508</v>
-      </c>
-      <c r="D3" s="32" t="s">
-        <v>509</v>
-      </c>
-      <c r="E3" s="32" t="s">
-        <v>510</v>
-      </c>
-      <c r="F3" s="32" t="s">
-        <v>668</v>
-      </c>
-      <c r="G3" s="32" t="s">
-        <v>687</v>
-      </c>
-      <c r="H3" s="32" t="s">
-        <v>687</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="J3" s="32" t="s">
-        <v>687</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="L3" s="32" t="s">
-        <v>687</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="129" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="32" t="s">
+      <c r="G3" s="5" t="s">
+        <v>864</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>864</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>864</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>885</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>864</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>864</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="210" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>516</v>
       </c>
-      <c r="B4" s="32" t="s">
-        <v>517</v>
-      </c>
-      <c r="C4" s="32" t="s">
-        <v>518</v>
-      </c>
-      <c r="D4" s="32" t="s">
-        <v>519</v>
-      </c>
-      <c r="E4" s="32" t="s">
-        <v>520</v>
-      </c>
-      <c r="F4" s="32" t="s">
-        <v>668</v>
-      </c>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32" t="s">
-        <v>687</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>260</v>
-      </c>
-      <c r="J4" s="32"/>
-      <c r="K4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="L4" s="32"/>
-      <c r="M4" s="6" t="s">
+      <c r="B4" s="5" t="s">
+        <v>870</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>875</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>879</v>
+      </c>
+      <c r="E4" s="38" t="s">
+        <v>855</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>859</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>865</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>865</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>865</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>865</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>865</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>865</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="240" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>521</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>871</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>876</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>879</v>
+      </c>
+      <c r="E5" s="38" t="s">
+        <v>856</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>860</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>866</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>866</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>866</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>866</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>866</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>866</v>
+      </c>
+      <c r="Q5" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="225" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>522</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>872</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>877</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>879</v>
+      </c>
+      <c r="E6" s="38" t="s">
+        <v>857</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>861</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>867</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>867</v>
+      </c>
+      <c r="I6" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>867</v>
+      </c>
+      <c r="K6" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>867</v>
+      </c>
+      <c r="M6" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>867</v>
+      </c>
+      <c r="O6" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>867</v>
+      </c>
+      <c r="Q6" s="48" t="s">
         <v>8</v>
       </c>
     </row>
@@ -17274,7 +17557,7 @@
   <sheetViews>
     <sheetView zoomScale="83" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -17564,9 +17847,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF7BFF7B-5E59-40FB-93C7-19664CC11324}">
   <dimension ref="A1:AB29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y7" sqref="Y7"/>
+      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="60" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update Testcases for Json Start.php
Update Testcases for Json Start.php
</commit_message>
<xml_diff>
--- a/testing/testcases.xlsx
+++ b/testing/testcases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lai See Hoe\Documents\GitHub\project-g5t4\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CFDDE4D-16B0-4741-93AA-1CE97FDC99C9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F8CF7F-9424-4005-B61E-758B65FE7AEF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="844" firstSheet="12" activeTab="15" xr2:uid="{F747292D-6CBE-43A0-AF24-F2F7C25CEB64}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="844" firstSheet="5" activeTab="6" xr2:uid="{F747292D-6CBE-43A0-AF24-F2F7C25CEB64}"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 3 - JSON - BidDump" sheetId="20" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3369" uniqueCount="911">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3402" uniqueCount="920">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -7015,6 +7015,36 @@
   </si>
   <si>
     <t>Bid did not update</t>
+  </si>
+  <si>
+    <t>Start round 2 when round 2 is already active</t>
+  </si>
+  <si>
+    <t>Round 2 Active</t>
+  </si>
+  <si>
+    <t>call Json_checker start.php for 046a-start.txt</t>
+  </si>
+  <si>
+    <t>/046a</t>
+  </si>
+  <si>
+    <t>Pass/Fail 6/11/19</t>
+  </si>
+  <si>
+    <t>Result  6/11/19</t>
+  </si>
+  <si>
+    <t>Result 15/10/19</t>
+  </si>
+  <si>
+    <t>Pass/Fail 12/11/19</t>
+  </si>
+  <si>
+    <t>{ 
+"status": "s+M3uccess", 
+"round": 1 
+}</t>
   </si>
 </sst>
 </file>
@@ -8079,7 +8109,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="113.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="101" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -13255,8 +13285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D48F8994-0480-456C-9C73-8DEBC1CF05E8}">
   <dimension ref="A1:AD26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="U14" sqref="U14"/>
     </sheetView>
   </sheetViews>
@@ -20335,16 +20365,16 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3B503BA-8B4E-40C3-ABBB-6DE7E1EE984E}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J11" sqref="J11"/>
+      <selection pane="bottomLeft" activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:13" s="14" customFormat="1" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:17" s="14" customFormat="1" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -20366,26 +20396,38 @@
       <c r="G1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="22" t="s">
-        <v>799</v>
-      </c>
-      <c r="I1" s="22" t="s">
+      <c r="H1" s="13" t="s">
+        <v>917</v>
+      </c>
+      <c r="I1" s="13" t="s">
         <v>793</v>
       </c>
-      <c r="J1" s="22" t="s">
-        <v>800</v>
-      </c>
-      <c r="K1" s="22" t="s">
+      <c r="J1" s="13" t="s">
+        <v>841</v>
+      </c>
+      <c r="K1" s="13" t="s">
         <v>801</v>
       </c>
-      <c r="L1" s="22" t="s">
-        <v>816</v>
-      </c>
-      <c r="M1" s="22" t="s">
+      <c r="L1" s="13" t="s">
+        <v>840</v>
+      </c>
+      <c r="M1" s="13" t="s">
         <v>817</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" ht="76.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N1" s="13" t="s">
+        <v>916</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>915</v>
+      </c>
+      <c r="P1" s="13" t="s">
+        <v>843</v>
+      </c>
+      <c r="Q1" s="13" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="76.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="32" t="s">
         <v>439</v>
       </c>
@@ -20426,7 +20468,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="76.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:17" ht="76.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="32" t="s">
         <v>532</v>
       </c>
@@ -20474,16 +20516,16 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12CEDDF5-69A9-4C14-973B-D1519D988698}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O2" sqref="O2"/>
+      <selection pane="bottomLeft" activeCell="Q1" sqref="A1:Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:13" s="37" customFormat="1" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:17" s="37" customFormat="1" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -20506,25 +20548,37 @@
         <v>6</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>799</v>
+        <v>917</v>
       </c>
       <c r="I1" s="13" t="s">
         <v>793</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>800</v>
+        <v>841</v>
       </c>
       <c r="K1" s="13" t="s">
         <v>801</v>
       </c>
       <c r="L1" s="13" t="s">
-        <v>816</v>
+        <v>840</v>
       </c>
       <c r="M1" s="13" t="s">
         <v>817</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" ht="76.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N1" s="13" t="s">
+        <v>916</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>915</v>
+      </c>
+      <c r="P1" s="13" t="s">
+        <v>843</v>
+      </c>
+      <c r="Q1" s="13" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="76.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="32" t="s">
         <v>434</v>
       </c>
@@ -20559,13 +20613,25 @@
         <v>8</v>
       </c>
       <c r="L2" s="32" t="s">
-        <v>678</v>
+        <v>919</v>
       </c>
       <c r="M2" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="76.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N2" s="32" t="s">
+        <v>919</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2" s="32" t="s">
+        <v>919</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="76.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="32" t="s">
         <v>473</v>
       </c>
@@ -20603,6 +20669,71 @@
         <v>688</v>
       </c>
       <c r="M3" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="N3" s="32" t="s">
+        <v>688</v>
+      </c>
+      <c r="O3" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3" s="32" t="s">
+        <v>688</v>
+      </c>
+      <c r="Q3" s="42" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="76.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="32" t="s">
+        <v>914</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>474</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>911</v>
+      </c>
+      <c r="D4" s="42" t="s">
+        <v>912</v>
+      </c>
+      <c r="E4" s="32" t="s">
+        <v>913</v>
+      </c>
+      <c r="F4" s="32" t="s">
+        <v>676</v>
+      </c>
+      <c r="G4" s="32" t="s">
+        <v>688</v>
+      </c>
+      <c r="H4" s="32" t="s">
+        <v>688</v>
+      </c>
+      <c r="I4" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="32" t="s">
+        <v>688</v>
+      </c>
+      <c r="K4" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" s="32" t="s">
+        <v>688</v>
+      </c>
+      <c r="M4" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="N4" s="32" t="s">
+        <v>688</v>
+      </c>
+      <c r="O4" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="P4" s="32" t="s">
+        <v>688</v>
+      </c>
+      <c r="Q4" s="42" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated Testcases.xlsx for testcases on json stop round
Updated Testcases.xlsx for testcases on json stop round
</commit_message>
<xml_diff>
--- a/testing/testcases.xlsx
+++ b/testing/testcases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lai See Hoe\Documents\GitHub\project-g5t4\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F8CF7F-9424-4005-B61E-758B65FE7AEF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB64C1B-E122-4440-89BE-DA11AD57A76E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="844" firstSheet="5" activeTab="6" xr2:uid="{F747292D-6CBE-43A0-AF24-F2F7C25CEB64}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3402" uniqueCount="920">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3444" uniqueCount="928">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -7044,6 +7044,33 @@
     <t>{ 
 "status": "s+M3uccess", 
 "round": 1 
+}</t>
+  </si>
+  <si>
+    <t>stop round 2</t>
+  </si>
+  <si>
+    <t>/034a</t>
+  </si>
+  <si>
+    <t>Stop round 1 after it is inactive</t>
+  </si>
+  <si>
+    <t>call Json_checker stop.php for 034a-stop.txt</t>
+  </si>
+  <si>
+    <t>call Json_checker stop.php for 062a-stop.txt</t>
+  </si>
+  <si>
+    <t>/062a</t>
+  </si>
+  <si>
+    <t>stop round 2 after it is inactive</t>
+  </si>
+  <si>
+    <t>{
+ "status": "error",
+ "message": [ "round already ended" ]
 }</t>
   </si>
 </sst>
@@ -20365,11 +20392,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3B503BA-8B4E-40C3-ABBB-6DE7E1EE984E}">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P2" sqref="P2"/>
+      <selection pane="bottomLeft" activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20467,50 +20494,181 @@
       <c r="M2" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" ht="76.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N2" s="32" t="s">
+        <v>675</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2" s="32" t="s">
+        <v>675</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="114" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="32" t="s">
-        <v>532</v>
+        <v>921</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>533</v>
+        <v>440</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>534</v>
+        <v>922</v>
       </c>
       <c r="D3" s="32" t="s">
-        <v>535</v>
+        <v>446</v>
       </c>
       <c r="E3" s="32" t="s">
-        <v>536</v>
+        <v>923</v>
       </c>
       <c r="F3" s="32" t="s">
         <v>676</v>
       </c>
       <c r="G3" s="32" t="s">
+        <v>927</v>
+      </c>
+      <c r="H3" s="32" t="s">
+        <v>927</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="32" t="s">
+        <v>927</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="32" t="s">
+        <v>927</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="N3" s="32" t="s">
+        <v>927</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3" s="32" t="s">
+        <v>927</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="76.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="32" t="s">
+        <v>532</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>533</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>920</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>535</v>
+      </c>
+      <c r="E4" s="32" t="s">
+        <v>536</v>
+      </c>
+      <c r="F4" s="32" t="s">
+        <v>676</v>
+      </c>
+      <c r="G4" s="32" t="s">
         <v>675</v>
       </c>
-      <c r="H3" s="32" t="s">
+      <c r="H4" s="32" t="s">
         <v>675</v>
       </c>
-      <c r="I3" s="42" t="s">
-        <v>8</v>
-      </c>
-      <c r="J3" s="32" t="s">
+      <c r="I4" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="32" t="s">
         <v>675</v>
       </c>
-      <c r="K3" s="42" t="s">
-        <v>8</v>
-      </c>
-      <c r="L3" s="32" t="s">
+      <c r="K4" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" s="32" t="s">
         <v>675</v>
       </c>
-      <c r="M3" s="42" t="s">
+      <c r="M4" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="N4" s="32" t="s">
+        <v>675</v>
+      </c>
+      <c r="O4" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="P4" s="32" t="s">
+        <v>675</v>
+      </c>
+      <c r="Q4" s="42" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="145.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="32" t="s">
+        <v>925</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>533</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>926</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>534</v>
+      </c>
+      <c r="E5" s="32" t="s">
+        <v>924</v>
+      </c>
+      <c r="F5" s="32" t="s">
+        <v>676</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>927</v>
+      </c>
+      <c r="H5" s="32" t="s">
+        <v>927</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="32" t="s">
+        <v>927</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="L5" s="32" t="s">
+        <v>927</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="N5" s="32" t="s">
+        <v>927</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="P5" s="32" t="s">
+        <v>927</v>
+      </c>
+      <c r="Q5" s="6" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated test case for correct dates on Start and Stop json testcases
Updated test case for correct dates on Start and Stop json testcases
</commit_message>
<xml_diff>
--- a/testing/testcases.xlsx
+++ b/testing/testcases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lai See Hoe\Documents\GitHub\project-g5t4\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB64C1B-E122-4440-89BE-DA11AD57A76E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B2A2BD-CB28-4BBC-BF42-599A7B910374}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="844" firstSheet="5" activeTab="6" xr2:uid="{F747292D-6CBE-43A0-AF24-F2F7C25CEB64}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="844" firstSheet="6" activeTab="7" xr2:uid="{F747292D-6CBE-43A0-AF24-F2F7C25CEB64}"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 3 - JSON - BidDump" sheetId="20" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3444" uniqueCount="928">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3432" uniqueCount="929">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -7041,12 +7041,6 @@
     <t>Pass/Fail 12/11/19</t>
   </si>
   <si>
-    <t>{ 
-"status": "s+M3uccess", 
-"round": 1 
-}</t>
-  </si>
-  <si>
     <t>stop round 2</t>
   </si>
   <si>
@@ -7072,6 +7066,12 @@
  "status": "error",
  "message": [ "round already ended" ]
 }</t>
+  </si>
+  <si>
+    <t>Result 14/11/19</t>
+  </si>
+  <si>
+    <t>Pass/Fail 14/11/19</t>
   </si>
 </sst>
 </file>
@@ -7219,7 +7219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -7354,6 +7354,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7878,7 +7884,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01360F1A-846B-44B4-BA3B-EAE40848B114}">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
@@ -20392,16 +20398,16 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3B503BA-8B4E-40C3-ABBB-6DE7E1EE984E}">
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N3" sqref="N3"/>
+      <selection pane="bottomLeft" activeCell="R1" sqref="R1:S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:17" s="14" customFormat="1" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:19" s="14" customFormat="1" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -20453,216 +20459,206 @@
       <c r="Q1" s="13" t="s">
         <v>918</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" ht="76.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="32" t="s">
+      <c r="R1" s="13" t="s">
+        <v>927</v>
+      </c>
+      <c r="S1" s="13" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="75.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="49" t="s">
         <v>439</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="49" t="s">
         <v>440</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="49" t="s">
         <v>441</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="49" t="s">
         <v>437</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="49" t="s">
         <v>442</v>
       </c>
-      <c r="F2" s="32" t="s">
+      <c r="F2" s="49" t="s">
         <v>676</v>
       </c>
-      <c r="G2" s="32" t="s">
+      <c r="G2" s="49" t="s">
         <v>675</v>
       </c>
-      <c r="H2" s="32" t="s">
+      <c r="H2" s="49" t="s">
         <v>675</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="32" t="s">
+      <c r="I2" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="49" t="s">
         <v>675</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="L2" s="32" t="s">
+      <c r="K2" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="49" t="s">
         <v>675</v>
       </c>
-      <c r="M2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="N2" s="32" t="s">
+      <c r="M2" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" s="49" t="s">
         <v>675</v>
       </c>
-      <c r="O2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="P2" s="32" t="s">
+      <c r="O2" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2" s="49" t="s">
         <v>675</v>
       </c>
-      <c r="Q2" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="114" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="32" t="s">
+      <c r="Q2" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="R2" s="49" t="s">
+        <v>675</v>
+      </c>
+      <c r="S2" s="45" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="113" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="49" t="s">
+        <v>920</v>
+      </c>
+      <c r="B3" s="49" t="s">
+        <v>440</v>
+      </c>
+      <c r="C3" s="49" t="s">
         <v>921</v>
       </c>
-      <c r="B3" s="32" t="s">
-        <v>440</v>
-      </c>
-      <c r="C3" s="32" t="s">
+      <c r="D3" s="49" t="s">
+        <v>446</v>
+      </c>
+      <c r="E3" s="49" t="s">
         <v>922</v>
       </c>
-      <c r="D3" s="32" t="s">
-        <v>446</v>
-      </c>
-      <c r="E3" s="32" t="s">
+      <c r="F3" s="49" t="s">
+        <v>676</v>
+      </c>
+      <c r="G3" s="49" t="s">
+        <v>926</v>
+      </c>
+      <c r="H3" s="49"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="45"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="45"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="45"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="49" t="s">
+        <v>926</v>
+      </c>
+      <c r="S3" s="45" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="75.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="49" t="s">
+        <v>532</v>
+      </c>
+      <c r="B4" s="49" t="s">
+        <v>533</v>
+      </c>
+      <c r="C4" s="49" t="s">
+        <v>919</v>
+      </c>
+      <c r="D4" s="49" t="s">
+        <v>535</v>
+      </c>
+      <c r="E4" s="49" t="s">
+        <v>536</v>
+      </c>
+      <c r="F4" s="49" t="s">
+        <v>676</v>
+      </c>
+      <c r="G4" s="49" t="s">
+        <v>675</v>
+      </c>
+      <c r="H4" s="49" t="s">
+        <v>675</v>
+      </c>
+      <c r="I4" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="49" t="s">
+        <v>675</v>
+      </c>
+      <c r="K4" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" s="49" t="s">
+        <v>675</v>
+      </c>
+      <c r="M4" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="N4" s="49" t="s">
+        <v>675</v>
+      </c>
+      <c r="O4" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="P4" s="49" t="s">
+        <v>675</v>
+      </c>
+      <c r="Q4" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="R4" s="49" t="s">
+        <v>675</v>
+      </c>
+      <c r="S4" s="50" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="145.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="49" t="s">
+        <v>924</v>
+      </c>
+      <c r="B5" s="49" t="s">
+        <v>533</v>
+      </c>
+      <c r="C5" s="49" t="s">
+        <v>925</v>
+      </c>
+      <c r="D5" s="49" t="s">
+        <v>534</v>
+      </c>
+      <c r="E5" s="49" t="s">
         <v>923</v>
       </c>
-      <c r="F3" s="32" t="s">
+      <c r="F5" s="49" t="s">
         <v>676</v>
       </c>
-      <c r="G3" s="32" t="s">
-        <v>927</v>
-      </c>
-      <c r="H3" s="32" t="s">
-        <v>927</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="J3" s="32" t="s">
-        <v>927</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="L3" s="32" t="s">
-        <v>927</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="N3" s="32" t="s">
-        <v>927</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="P3" s="32" t="s">
-        <v>927</v>
-      </c>
-      <c r="Q3" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="76.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="32" t="s">
-        <v>532</v>
-      </c>
-      <c r="B4" s="32" t="s">
-        <v>533</v>
-      </c>
-      <c r="C4" s="32" t="s">
-        <v>920</v>
-      </c>
-      <c r="D4" s="32" t="s">
-        <v>535</v>
-      </c>
-      <c r="E4" s="32" t="s">
-        <v>536</v>
-      </c>
-      <c r="F4" s="32" t="s">
-        <v>676</v>
-      </c>
-      <c r="G4" s="32" t="s">
-        <v>675</v>
-      </c>
-      <c r="H4" s="32" t="s">
-        <v>675</v>
-      </c>
-      <c r="I4" s="42" t="s">
-        <v>8</v>
-      </c>
-      <c r="J4" s="32" t="s">
-        <v>675</v>
-      </c>
-      <c r="K4" s="42" t="s">
-        <v>8</v>
-      </c>
-      <c r="L4" s="32" t="s">
-        <v>675</v>
-      </c>
-      <c r="M4" s="42" t="s">
-        <v>8</v>
-      </c>
-      <c r="N4" s="32" t="s">
-        <v>675</v>
-      </c>
-      <c r="O4" s="42" t="s">
-        <v>8</v>
-      </c>
-      <c r="P4" s="32" t="s">
-        <v>675</v>
-      </c>
-      <c r="Q4" s="42" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="145.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="32" t="s">
-        <v>925</v>
-      </c>
-      <c r="B5" s="32" t="s">
-        <v>533</v>
-      </c>
-      <c r="C5" s="32" t="s">
+      <c r="G5" s="2" t="s">
         <v>926</v>
       </c>
-      <c r="D5" s="32" t="s">
-        <v>534</v>
-      </c>
-      <c r="E5" s="32" t="s">
-        <v>924</v>
-      </c>
-      <c r="F5" s="32" t="s">
-        <v>676</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>927</v>
-      </c>
-      <c r="H5" s="32" t="s">
-        <v>927</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="J5" s="32" t="s">
-        <v>927</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="L5" s="32" t="s">
-        <v>927</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="N5" s="32" t="s">
-        <v>927</v>
-      </c>
-      <c r="O5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="P5" s="32" t="s">
-        <v>927</v>
-      </c>
-      <c r="Q5" s="6" t="s">
+      <c r="H5" s="49"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="45"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="45"/>
+      <c r="N5" s="49"/>
+      <c r="O5" s="45"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="49" t="s">
+        <v>926</v>
+      </c>
+      <c r="S5" s="45" t="s">
         <v>8</v>
       </c>
     </row>
@@ -20674,16 +20670,16 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12CEDDF5-69A9-4C14-973B-D1519D988698}">
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q1" sqref="A1:Q1"/>
+      <selection pane="bottomLeft" activeCell="O4" sqref="H4:O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:17" s="37" customFormat="1" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:19" s="37" customFormat="1" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -20735,8 +20731,14 @@
       <c r="Q1" s="13" t="s">
         <v>918</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" ht="76.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="R1" s="13" t="s">
+        <v>927</v>
+      </c>
+      <c r="S1" s="13" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="76.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="32" t="s">
         <v>434</v>
       </c>
@@ -20771,25 +20773,31 @@
         <v>8</v>
       </c>
       <c r="L2" s="32" t="s">
-        <v>919</v>
+        <v>678</v>
       </c>
       <c r="M2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="N2" s="32" t="s">
-        <v>919</v>
+        <v>678</v>
       </c>
       <c r="O2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="P2" s="32" t="s">
-        <v>919</v>
+        <v>678</v>
       </c>
       <c r="Q2" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" ht="76.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="R2" s="32" t="s">
+        <v>678</v>
+      </c>
+      <c r="S2" s="45" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="76.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="32" t="s">
         <v>473</v>
       </c>
@@ -20841,8 +20849,14 @@
       <c r="Q3" s="42" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" ht="76.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="R3" s="32" t="s">
+        <v>688</v>
+      </c>
+      <c r="S3" s="42" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="76.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="32" t="s">
         <v>914</v>
       </c>
@@ -20864,34 +20878,18 @@
       <c r="G4" s="32" t="s">
         <v>688</v>
       </c>
-      <c r="H4" s="32" t="s">
+      <c r="H4" s="32"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="32"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="32"/>
+      <c r="O4" s="42"/>
+      <c r="R4" s="32" t="s">
         <v>688</v>
       </c>
-      <c r="I4" s="42" t="s">
-        <v>8</v>
-      </c>
-      <c r="J4" s="32" t="s">
-        <v>688</v>
-      </c>
-      <c r="K4" s="42" t="s">
-        <v>8</v>
-      </c>
-      <c r="L4" s="32" t="s">
-        <v>688</v>
-      </c>
-      <c r="M4" s="42" t="s">
-        <v>8</v>
-      </c>
-      <c r="N4" s="32" t="s">
-        <v>688</v>
-      </c>
-      <c r="O4" s="42" t="s">
-        <v>8</v>
-      </c>
-      <c r="P4" s="32" t="s">
-        <v>688</v>
-      </c>
-      <c r="Q4" s="42" t="s">
+      <c r="S4" s="42" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update testcases.xlsx regarding bootstrap
update testcases.xlsx regarding bootstrap
</commit_message>
<xml_diff>
--- a/testing/testcases.xlsx
+++ b/testing/testcases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Serene\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lai See Hoe\Documents\GitHub\project-g5t4\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A4641A-4280-4747-B697-A9E610CCD28B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D404EF1-8FBF-4B20-AA1D-4A7A0256B1E0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="844" firstSheet="15" activeTab="18" xr2:uid="{F747292D-6CBE-43A0-AF24-F2F7C25CEB64}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3648" uniqueCount="798">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3775" uniqueCount="805">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -12861,6 +12861,52 @@
         }
     ]
 }</t>
+  </si>
+  <si>
+    <t>Admin uploads sectiontest2.zip</t>
+  </si>
+  <si>
+    <t>sectiontest2.zip</t>
+  </si>
+  <si>
+    <t>Bootstrap sectiontest2.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Bootstrap Results
+Status	error
+bid.csv	0
+course.csv	24
+course_completed.csv	2
+prerequisite.csv	8
+section.csv	34
+student.csv	14
+course_completed.csv	Line: 3	invalid userid
+course_completed.csv	Line: 4	invalid userid invalid course completed
+section.csv	Line: 32	invalid course
+student.csv	Line: 3	invalid e-dollar</t>
+  </si>
+  <si>
+    <t>Result 16/11/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pass/Fail 16/11/19 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Bootstrap Results
+Status	error
+bid.csv	0
+course.csv	24
+course_completed.csv	2
+prerequisite.csv	8
+section.csv	33
+student.csv	14
+course_completed.csv	Line: 3	invalid userid
+course_completed.csv	Line: 4	invalid userid invalid course completed
+section.csv	Line: 2	invalid section
+section.csv	Line: 32	invalid course
+student.csv	Line: 3	invalid e-dollar</t>
   </si>
 </sst>
 </file>
@@ -13952,7 +13998,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" ht="387.5" x14ac:dyDescent="0.35">
       <c r="A8" s="25" t="s">
         <v>671</v>
       </c>
@@ -22653,11 +22699,11 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77076042-100F-4228-9C99-338194152E9B}">
-  <dimension ref="A1:R30"/>
+  <dimension ref="A1:V32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="72" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V32" sqref="V32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -22666,7 +22712,7 @@
     <col min="2" max="2" width="20.6328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.7265625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="26.81640625" customWidth="1"/>
-    <col min="6" max="6" width="15.54296875" customWidth="1"/>
+    <col min="6" max="6" width="25.81640625" customWidth="1"/>
     <col min="7" max="8" width="18.453125" customWidth="1"/>
     <col min="9" max="9" width="16.7265625" customWidth="1"/>
     <col min="10" max="10" width="21.1796875" customWidth="1"/>
@@ -22676,9 +22722,11 @@
     <col min="16" max="16" width="13.1796875" customWidth="1"/>
     <col min="17" max="17" width="17.453125" customWidth="1"/>
     <col min="18" max="18" width="13.7265625" customWidth="1"/>
+    <col min="19" max="19" width="17.81640625" customWidth="1"/>
+    <col min="21" max="21" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="12" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" s="12" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>567</v>
       </c>
@@ -22733,8 +22781,20 @@
       <c r="R1" s="11" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" ht="145" x14ac:dyDescent="0.35">
+      <c r="S1" s="22" t="s">
+        <v>802</v>
+      </c>
+      <c r="T1" s="11" t="s">
+        <v>803</v>
+      </c>
+      <c r="U1" s="22" t="s">
+        <v>802</v>
+      </c>
+      <c r="V1" s="11" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" ht="232" x14ac:dyDescent="0.35">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -22789,8 +22849,20 @@
       <c r="R2" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" ht="145" x14ac:dyDescent="0.35">
+      <c r="S2" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="T2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="U2" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="V2" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="232" x14ac:dyDescent="0.35">
       <c r="A3" s="9">
         <v>2</v>
       </c>
@@ -22845,8 +22917,20 @@
       <c r="R3" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" ht="145" x14ac:dyDescent="0.35">
+      <c r="S3" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="T3" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="U3" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="V3" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A4" s="9">
         <v>3</v>
       </c>
@@ -22901,8 +22985,20 @@
       <c r="R4" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" ht="145" x14ac:dyDescent="0.35">
+      <c r="S4" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="T4" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="U4" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="V4" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A5" s="9">
         <v>4</v>
       </c>
@@ -22957,8 +23053,20 @@
       <c r="R5" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" ht="174" x14ac:dyDescent="0.35">
+      <c r="S5" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="T5" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="U5" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="V5" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="261" x14ac:dyDescent="0.35">
       <c r="A6" s="9">
         <v>5</v>
       </c>
@@ -23013,8 +23121,20 @@
       <c r="R6" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" ht="145" x14ac:dyDescent="0.35">
+      <c r="S6" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="T6" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="U6" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="V6" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" ht="232" x14ac:dyDescent="0.35">
       <c r="A7" s="9">
         <v>6</v>
       </c>
@@ -23069,8 +23189,20 @@
       <c r="R7" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" ht="145" x14ac:dyDescent="0.35">
+      <c r="S7" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="T7" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="U7" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="V7" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A8" s="9">
         <v>7</v>
       </c>
@@ -23125,8 +23257,20 @@
       <c r="R8" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" ht="145" x14ac:dyDescent="0.35">
+      <c r="S8" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="T8" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="U8" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="V8" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A9" s="9">
         <v>8</v>
       </c>
@@ -23181,8 +23325,20 @@
       <c r="R9" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" ht="145" x14ac:dyDescent="0.35">
+      <c r="S9" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="T9" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="U9" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="V9" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A10" s="9">
         <v>9</v>
       </c>
@@ -23237,8 +23393,20 @@
       <c r="R10" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" ht="145" x14ac:dyDescent="0.35">
+      <c r="S10" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="T10" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="U10" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="V10" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="232" x14ac:dyDescent="0.35">
       <c r="A11" s="9">
         <v>10</v>
       </c>
@@ -23293,8 +23461,20 @@
       <c r="R11" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" ht="145" x14ac:dyDescent="0.35">
+      <c r="S11" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="T11" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="U11" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="V11" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A12" s="9">
         <v>11</v>
       </c>
@@ -23349,8 +23529,20 @@
       <c r="R12" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" ht="145" x14ac:dyDescent="0.35">
+      <c r="S12" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="T12" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="U12" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="V12" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" ht="232" x14ac:dyDescent="0.35">
       <c r="A13" s="9">
         <v>12</v>
       </c>
@@ -23405,8 +23597,20 @@
       <c r="R13" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" ht="145" x14ac:dyDescent="0.35">
+      <c r="S13" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="T13" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="U13" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="V13" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" ht="232" x14ac:dyDescent="0.35">
       <c r="A14" s="9">
         <v>13</v>
       </c>
@@ -23461,8 +23665,20 @@
       <c r="R14" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" ht="145" x14ac:dyDescent="0.35">
+      <c r="S14" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="T14" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="U14" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="V14" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" ht="232" x14ac:dyDescent="0.35">
       <c r="A15" s="9">
         <v>14</v>
       </c>
@@ -23517,8 +23733,20 @@
       <c r="R15" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" ht="145" x14ac:dyDescent="0.35">
+      <c r="S15" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="T15" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="U15" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="V15" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" ht="232" x14ac:dyDescent="0.35">
       <c r="A16" s="9">
         <v>15</v>
       </c>
@@ -23573,8 +23801,20 @@
       <c r="R16" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" ht="145" x14ac:dyDescent="0.35">
+      <c r="S16" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="T16" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="U16" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="V16" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" ht="232" x14ac:dyDescent="0.35">
       <c r="A17" s="9">
         <v>16</v>
       </c>
@@ -23629,8 +23869,20 @@
       <c r="R17" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" ht="145" x14ac:dyDescent="0.35">
+      <c r="S17" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="T17" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="U17" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="V17" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A18" s="9">
         <v>17</v>
       </c>
@@ -23685,8 +23937,20 @@
       <c r="R18" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" ht="145" x14ac:dyDescent="0.35">
+      <c r="S18" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="T18" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="U18" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="V18" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" ht="232" x14ac:dyDescent="0.35">
       <c r="A19" s="9">
         <v>18</v>
       </c>
@@ -23741,8 +24005,20 @@
       <c r="R19" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" ht="145" x14ac:dyDescent="0.35">
+      <c r="S19" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="T19" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="U19" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="V19" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A20" s="9">
         <v>19</v>
       </c>
@@ -23797,8 +24073,20 @@
       <c r="R20" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" ht="145" x14ac:dyDescent="0.35">
+      <c r="S20" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="T20" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="U20" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="V20" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A21" s="9">
         <v>20</v>
       </c>
@@ -23853,8 +24141,20 @@
       <c r="R21" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" ht="145" x14ac:dyDescent="0.35">
+      <c r="S21" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="T21" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="U21" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="V21" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" ht="232" x14ac:dyDescent="0.35">
       <c r="A22" s="9">
         <v>21</v>
       </c>
@@ -23909,8 +24209,20 @@
       <c r="R22" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="S22" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="T22" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="U22" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="V22" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A23" s="9">
         <v>22</v>
       </c>
@@ -23965,8 +24277,20 @@
       <c r="R23" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="S23" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="T23" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="U23" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="V23" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" ht="232" x14ac:dyDescent="0.35">
       <c r="A24" s="9">
         <v>23</v>
       </c>
@@ -24021,8 +24345,20 @@
       <c r="R24" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="S24" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="T24" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="U24" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="V24" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" ht="232" x14ac:dyDescent="0.35">
       <c r="A25" s="9">
         <v>24</v>
       </c>
@@ -24077,8 +24413,20 @@
       <c r="R25" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="S25" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="T25" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="U25" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="V25" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" ht="28" x14ac:dyDescent="0.35">
       <c r="A26" s="9">
         <v>25</v>
       </c>
@@ -24121,8 +24469,16 @@
       <c r="R26" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="1:18" ht="145" x14ac:dyDescent="0.35">
+      <c r="S26" s="10"/>
+      <c r="T26" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="U26" s="10"/>
+      <c r="V26" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A27" s="9">
         <v>26</v>
       </c>
@@ -24177,8 +24533,20 @@
       <c r="R27" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:18" ht="145" x14ac:dyDescent="0.35">
+      <c r="S27" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="T27" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="U27" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="V27" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A28" s="9">
         <v>27</v>
       </c>
@@ -24233,8 +24601,20 @@
       <c r="R28" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="29" spans="1:18" ht="145" x14ac:dyDescent="0.35">
+      <c r="S28" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="T28" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="U28" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="V28" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" ht="232" x14ac:dyDescent="0.35">
       <c r="A29" s="9">
         <v>28</v>
       </c>
@@ -24289,8 +24669,20 @@
       <c r="R29" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:18" ht="333.5" x14ac:dyDescent="0.35">
+      <c r="S29" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="T29" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="U29" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="V29" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A30" s="9">
         <v>29</v>
       </c>
@@ -24327,6 +24719,53 @@
       <c r="R30" s="7" t="s">
         <v>4</v>
       </c>
+      <c r="S30" s="10" t="s">
+        <v>450</v>
+      </c>
+      <c r="T30" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="U30" s="10" t="s">
+        <v>450</v>
+      </c>
+      <c r="V30" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" ht="333.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="9">
+        <v>30</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>571</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>798</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>799</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>800</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>804</v>
+      </c>
+      <c r="S31" s="1" t="s">
+        <v>801</v>
+      </c>
+      <c r="T31" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="U31" s="1" t="s">
+        <v>804</v>
+      </c>
+      <c r="V31" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="D32" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update Testcase for manual testing for functions done in iteration 1
Update Testcase for manual testing for functions done in iteration 1
</commit_message>
<xml_diff>
--- a/testing/testcases.xlsx
+++ b/testing/testcases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chen yibing\Documents\GitHub\project-g5t4\testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lai See Hoe\Documents\GitHub\project-g5t4\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AA18D20-4D52-4A78-9460-79E388BE863E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6540EA9D-6F06-4140-A462-BE9AE983A8E8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" tabRatio="844" xr2:uid="{F747292D-6CBE-43A0-AF24-F2F7C25CEB64}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="844" firstSheet="16" activeTab="17" xr2:uid="{F747292D-6CBE-43A0-AF24-F2F7C25CEB64}"/>
   </bookViews>
   <sheets>
     <sheet name="Test plan" sheetId="22" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3801" uniqueCount="831">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3927" uniqueCount="850">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -12986,6 +12986,92 @@
   </si>
   <si>
     <t>To ensure iteration 1 and 2 codes are still working and prepare the new features listed for release</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Bootstrap Results
+Status	success
+bid.csv	11
+course.csv	13
+course_completed.csv	5
+prerequisite.csv	2
+section.csv	57
+student.csv	14
+</t>
+  </si>
+  <si>
+    <t>Admin uploads uat-data1.zip</t>
+  </si>
+  <si>
+    <t>uat-data1.zip</t>
+  </si>
+  <si>
+    <t>Bootstrap uat-data1.zip</t>
+  </si>
+  <si>
+    <t>Validate for correct user and password</t>
+  </si>
+  <si>
+    <t>username:amy
+password: 1234</t>
+  </si>
+  <si>
+    <t>amy enters correct username and password</t>
+  </si>
+  <si>
+    <t>Student wants to bid for a course that is not part of his school</t>
+  </si>
+  <si>
+    <t>user: amy
+Course: CS001
+Section: 1
+Amount: 10.00</t>
+  </si>
+  <si>
+    <t>Student tries to find and bid for CS001</t>
+  </si>
+  <si>
+    <t>Student cannot find course CS001</t>
+  </si>
+  <si>
+    <t>Course: IS003
+Section: S1
+Bid Amount: 10.00
+Status: Fail</t>
+  </si>
+  <si>
+    <t>Course: IS003
+Section: S1
+Bid Amount: 11.00
+Status: Success</t>
+  </si>
+  <si>
+    <t>Course: IS003
+Section: S1
+Bid Amount: 10.00
+Status: Success</t>
+  </si>
+  <si>
+    <t>Course: IS003
+Section: S1
+Bid Amount: 10.00
+Status: Pending</t>
+  </si>
+  <si>
+    <t>Select view bidding status after amy gets out bidded by charlie in IS003 S1</t>
+  </si>
+  <si>
+    <t>Course: ECON001 
+Section: S1
+Bid Amount: 20.00
+Status: Success
+Minimum bid: $11</t>
+  </si>
+  <si>
+    <t>Message: Bid placed successfully! Amount left: $191</t>
+  </si>
+  <si>
+    <t>Student cannot find course CS002</t>
   </si>
 </sst>
 </file>
@@ -13340,14 +13426,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -13665,126 +13751,126 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7674409B-922A-4ACF-BCB5-9D6A022E081E}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="34.3671875" customWidth="1"/>
-    <col min="3" max="3" width="29.5234375" customWidth="1"/>
-    <col min="4" max="4" width="32.62890625" customWidth="1"/>
-    <col min="5" max="5" width="46.62890625" customWidth="1"/>
+    <col min="2" max="2" width="34.36328125" customWidth="1"/>
+    <col min="3" max="3" width="29.54296875" customWidth="1"/>
+    <col min="4" max="4" width="32.6328125" customWidth="1"/>
+    <col min="5" max="5" width="46.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="57" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="60" t="s">
         <v>805</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="58" t="s">
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="57" t="s">
         <v>806</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="57" t="s">
         <v>807</v>
       </c>
-      <c r="C2" s="58" t="s">
+      <c r="C2" s="57" t="s">
         <v>808</v>
       </c>
-      <c r="D2" s="58" t="s">
+      <c r="D2" s="57" t="s">
         <v>809</v>
       </c>
-      <c r="E2" s="58" t="s">
+      <c r="E2" s="57" t="s">
         <v>810</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="61.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="58">
+    <row r="3" spans="1:5" ht="75" x14ac:dyDescent="0.35">
+      <c r="A3" s="57">
         <v>1</v>
       </c>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="58" t="s">
         <v>811</v>
       </c>
-      <c r="C3" s="60" t="s">
+      <c r="C3" s="59" t="s">
         <v>812</v>
       </c>
-      <c r="D3" s="59" t="s">
+      <c r="D3" s="58" t="s">
         <v>813</v>
       </c>
-      <c r="E3" s="59" t="s">
+      <c r="E3" s="58" t="s">
         <v>814</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="61.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="58">
+    <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.35">
+      <c r="A4" s="57">
         <v>2</v>
       </c>
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="58" t="s">
         <v>815</v>
       </c>
-      <c r="C4" s="59" t="s">
+      <c r="C4" s="58" t="s">
         <v>816</v>
       </c>
-      <c r="D4" s="59" t="s">
+      <c r="D4" s="58" t="s">
         <v>817</v>
       </c>
-      <c r="E4" s="59" t="s">
+      <c r="E4" s="58" t="s">
         <v>818</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="86.1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="58">
+    <row r="5" spans="1:5" ht="87.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="57">
         <v>3</v>
       </c>
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="58" t="s">
         <v>819</v>
       </c>
-      <c r="C5" s="59" t="s">
+      <c r="C5" s="58" t="s">
         <v>830</v>
       </c>
-      <c r="D5" s="59" t="s">
+      <c r="D5" s="58" t="s">
         <v>820</v>
       </c>
-      <c r="E5" s="59" t="s">
+      <c r="E5" s="58" t="s">
         <v>821</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="73.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="58">
-        <v>4</v>
-      </c>
-      <c r="B6" s="59" t="s">
+    <row r="6" spans="1:5" ht="87.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="57">
+        <v>4</v>
+      </c>
+      <c r="B6" s="58" t="s">
         <v>822</v>
       </c>
-      <c r="C6" s="59" t="s">
+      <c r="C6" s="58" t="s">
         <v>823</v>
       </c>
-      <c r="D6" s="59" t="s">
+      <c r="D6" s="58" t="s">
         <v>824</v>
       </c>
-      <c r="E6" s="59" t="s">
+      <c r="E6" s="58" t="s">
         <v>825</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="24.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="58">
+    <row r="7" spans="1:5" ht="25" x14ac:dyDescent="0.35">
+      <c r="A7" s="57">
         <v>5</v>
       </c>
-      <c r="B7" s="59" t="s">
+      <c r="B7" s="58" t="s">
         <v>826</v>
       </c>
-      <c r="C7" s="59" t="s">
+      <c r="C7" s="58" t="s">
         <v>827</v>
       </c>
-      <c r="D7" s="59" t="s">
+      <c r="D7" s="58" t="s">
         <v>828</v>
       </c>
-      <c r="E7" s="59" t="s">
+      <c r="E7" s="58" t="s">
         <v>829</v>
       </c>
     </row>
@@ -13806,12 +13892,12 @@
       <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="9.734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="35" customFormat="1" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:16" s="35" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="11" t="s">
         <v>567</v>
       </c>
@@ -13861,7 +13947,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="62.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:16" ht="76.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="25" t="s">
         <v>703</v>
       </c>
@@ -13911,7 +13997,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="62.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:16" ht="76.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="25" t="s">
         <v>719</v>
       </c>
@@ -13961,7 +14047,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="62.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:16" ht="76.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="30" t="s">
         <v>761</v>
       </c>
@@ -14004,19 +14090,19 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="20" style="19" customWidth="1"/>
-    <col min="3" max="3" width="18.26171875" style="19" customWidth="1"/>
-    <col min="4" max="4" width="20.734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5234375" customWidth="1"/>
+    <col min="3" max="3" width="18.26953125" style="19" customWidth="1"/>
+    <col min="4" max="4" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.54296875" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.3671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.3671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.3671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>567</v>
       </c>
@@ -14054,7 +14140,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:12" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A2" s="25" t="s">
         <v>664</v>
       </c>
@@ -14092,7 +14178,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:12" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A3" s="25" t="s">
         <v>665</v>
       </c>
@@ -14130,7 +14216,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:12" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A4" s="25" t="s">
         <v>666</v>
       </c>
@@ -14168,7 +14254,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:12" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A5" s="25" t="s">
         <v>667</v>
       </c>
@@ -14206,7 +14292,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:12" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A6" s="25" t="s">
         <v>668</v>
       </c>
@@ -14244,7 +14330,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:12" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A7" s="25" t="s">
         <v>670</v>
       </c>
@@ -14282,7 +14368,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="369" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:12" ht="387.5" x14ac:dyDescent="0.35">
       <c r="A8" s="25" t="s">
         <v>671</v>
       </c>
@@ -14333,17 +14419,17 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="14.15625" customWidth="1"/>
-    <col min="3" max="3" width="20.62890625" customWidth="1"/>
-    <col min="4" max="4" width="17.7890625" customWidth="1"/>
-    <col min="5" max="5" width="22.15625" customWidth="1"/>
-    <col min="6" max="6" width="11.7890625" customWidth="1"/>
-    <col min="7" max="7" width="16.7890625" customWidth="1"/>
+    <col min="2" max="2" width="14.1796875" customWidth="1"/>
+    <col min="3" max="3" width="20.6328125" customWidth="1"/>
+    <col min="4" max="4" width="17.81640625" customWidth="1"/>
+    <col min="5" max="5" width="22.1796875" customWidth="1"/>
+    <col min="6" max="6" width="11.81640625" customWidth="1"/>
+    <col min="7" max="7" width="16.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="23" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:14" s="23" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>567</v>
       </c>
@@ -14387,7 +14473,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="308.39999999999998" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:14" ht="338.5" x14ac:dyDescent="0.35">
       <c r="A2" s="25" t="s">
         <v>656</v>
       </c>
@@ -14431,7 +14517,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="136.19999999999999" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:14" ht="138.5" x14ac:dyDescent="0.35">
       <c r="A3" s="25" t="s">
         <v>657</v>
       </c>
@@ -14475,7 +14561,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="123.9" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:14" ht="138.5" x14ac:dyDescent="0.35">
       <c r="A4" s="25" t="s">
         <v>658</v>
       </c>
@@ -14519,7 +14605,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="123.9" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:14" ht="138.5" x14ac:dyDescent="0.35">
       <c r="A5" s="25" t="s">
         <v>659</v>
       </c>
@@ -14563,7 +14649,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="160.80000000000001" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:14" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A6" s="25" t="s">
         <v>660</v>
       </c>
@@ -14607,7 +14693,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="136.19999999999999" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:14" ht="138.5" x14ac:dyDescent="0.35">
       <c r="A7" s="25" t="s">
         <v>661</v>
       </c>
@@ -14651,7 +14737,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="136.19999999999999" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:14" ht="138.5" x14ac:dyDescent="0.35">
       <c r="A8" s="25" t="s">
         <v>662</v>
       </c>
@@ -14695,7 +14781,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="296.10000000000002" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:14" ht="338.5" x14ac:dyDescent="0.35">
       <c r="A9" s="25" t="s">
         <v>663</v>
       </c>
@@ -14753,20 +14839,20 @@
       <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.734375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.5234375" style="26" customWidth="1"/>
-    <col min="2" max="2" width="14.734375" style="26" customWidth="1"/>
-    <col min="3" max="3" width="38.7890625" style="26" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.734375" style="26" customWidth="1"/>
-    <col min="5" max="5" width="25.5234375" style="26" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.54296875" style="26" customWidth="1"/>
+    <col min="2" max="2" width="14.7265625" style="26" customWidth="1"/>
+    <col min="3" max="3" width="38.81640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.7265625" style="26" customWidth="1"/>
+    <col min="5" max="5" width="25.54296875" style="26" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" style="26" customWidth="1"/>
-    <col min="7" max="7" width="10.7890625" style="26" customWidth="1"/>
-    <col min="8" max="8" width="8.47265625" style="26" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.734375" style="26"/>
+    <col min="7" max="7" width="10.81640625" style="26" customWidth="1"/>
+    <col min="8" max="8" width="8.453125" style="26" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.7265625" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="28" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" s="28" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>567</v>
       </c>
@@ -14804,7 +14890,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="296.10000000000002" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:12" ht="338.5" x14ac:dyDescent="0.35">
       <c r="A2" s="25" t="s">
         <v>656</v>
       </c>
@@ -14846,7 +14932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="136.19999999999999" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:12" ht="138.5" x14ac:dyDescent="0.35">
       <c r="A3" s="25" t="s">
         <v>657</v>
       </c>
@@ -14884,7 +14970,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="123.9" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:12" ht="138.5" x14ac:dyDescent="0.35">
       <c r="A4" s="25" t="s">
         <v>658</v>
       </c>
@@ -14922,7 +15008,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="123.9" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:12" ht="138.5" x14ac:dyDescent="0.35">
       <c r="A5" s="25" t="s">
         <v>659</v>
       </c>
@@ -14960,7 +15046,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="160.80000000000001" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:12" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A6" s="25" t="s">
         <v>660</v>
       </c>
@@ -14998,7 +15084,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="136.19999999999999" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:12" ht="138.5" x14ac:dyDescent="0.35">
       <c r="A7" s="25" t="s">
         <v>661</v>
       </c>
@@ -15036,7 +15122,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="136.19999999999999" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:12" ht="138.5" x14ac:dyDescent="0.35">
       <c r="A8" s="25" t="s">
         <v>662</v>
       </c>
@@ -15074,7 +15160,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="296.10000000000002" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:12" ht="338.5" x14ac:dyDescent="0.35">
       <c r="A9" s="25" t="s">
         <v>663</v>
       </c>
@@ -15104,7 +15190,7 @@
       </c>
       <c r="L9" s="25"/>
     </row>
-    <row r="10" spans="1:12" ht="409.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:12" ht="409.6" x14ac:dyDescent="0.35">
       <c r="A10" s="25" t="s">
         <v>664</v>
       </c>
@@ -15142,7 +15228,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="409.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:12" ht="409.6" x14ac:dyDescent="0.35">
       <c r="A11" s="25" t="s">
         <v>665</v>
       </c>
@@ -15180,7 +15266,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="409.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:12" ht="409.6" x14ac:dyDescent="0.35">
       <c r="A12" s="25" t="s">
         <v>666</v>
       </c>
@@ -15218,7 +15304,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="409.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:12" ht="409.6" x14ac:dyDescent="0.35">
       <c r="A13" s="25" t="s">
         <v>667</v>
       </c>
@@ -15256,7 +15342,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="409.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:12" ht="409.6" x14ac:dyDescent="0.35">
       <c r="A14" s="25" t="s">
         <v>668</v>
       </c>
@@ -15294,7 +15380,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="409.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:12" ht="409.6" x14ac:dyDescent="0.35">
       <c r="A15" s="25" t="s">
         <v>670</v>
       </c>
@@ -15332,7 +15418,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="406.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:12" ht="409.6" x14ac:dyDescent="0.35">
       <c r="A16" s="25" t="s">
         <v>671</v>
       </c>
@@ -15370,7 +15456,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="160.80000000000001" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:12" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A17" s="25" t="s">
         <v>673</v>
       </c>
@@ -15408,7 +15494,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="160.80000000000001" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:12" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A18" s="25" t="s">
         <v>675</v>
       </c>
@@ -15446,7 +15532,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="123.9" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:12" ht="126" x14ac:dyDescent="0.35">
       <c r="A19" s="25" t="s">
         <v>677</v>
       </c>
@@ -15484,7 +15570,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="123.9" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:12" ht="126" x14ac:dyDescent="0.35">
       <c r="A20" s="25" t="s">
         <v>679</v>
       </c>
@@ -15522,7 +15608,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="123.9" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:12" ht="126" x14ac:dyDescent="0.35">
       <c r="A21" s="25" t="s">
         <v>681</v>
       </c>
@@ -15560,7 +15646,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="136.19999999999999" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:12" ht="138.5" x14ac:dyDescent="0.35">
       <c r="A22" s="25" t="s">
         <v>683</v>
       </c>
@@ -15598,7 +15684,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="123.9" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:12" ht="126" x14ac:dyDescent="0.35">
       <c r="A23" s="25" t="s">
         <v>685</v>
       </c>
@@ -15636,7 +15722,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" s="25" t="s">
         <v>189</v>
       </c>
@@ -15652,7 +15738,7 @@
       <c r="K24" s="25"/>
       <c r="L24" s="25"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25" s="25" t="s">
         <v>190</v>
       </c>
@@ -15668,7 +15754,7 @@
       <c r="K25" s="25"/>
       <c r="L25" s="25"/>
     </row>
-    <row r="26" spans="1:12" ht="160.80000000000001" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:12" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A26" s="25" t="s">
         <v>687</v>
       </c>
@@ -15706,7 +15792,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="123.9" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:12" ht="126" x14ac:dyDescent="0.35">
       <c r="A27" s="25" t="s">
         <v>689</v>
       </c>
@@ -15744,7 +15830,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28" s="25" t="s">
         <v>195</v>
       </c>
@@ -15760,7 +15846,7 @@
       <c r="K28" s="25"/>
       <c r="L28" s="25"/>
     </row>
-    <row r="29" spans="1:12" ht="111.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:12" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A29" s="25" t="s">
         <v>691</v>
       </c>
@@ -15796,7 +15882,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="111.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:12" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A30" s="25" t="s">
         <v>693</v>
       </c>
@@ -15834,7 +15920,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="128.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:12" ht="128.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="25" t="s">
         <v>695</v>
       </c>
@@ -15872,7 +15958,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="50.1" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:12" ht="51" x14ac:dyDescent="0.35">
       <c r="A32" s="25" t="s">
         <v>697</v>
       </c>
@@ -15910,7 +15996,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="50.1" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:12" ht="51" x14ac:dyDescent="0.35">
       <c r="A33" s="25" t="s">
         <v>699</v>
       </c>
@@ -15948,7 +16034,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="409.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:12" ht="409.6" x14ac:dyDescent="0.35">
       <c r="A34" s="25" t="s">
         <v>701</v>
       </c>
@@ -15986,7 +16072,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="62.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:12" ht="76" x14ac:dyDescent="0.35">
       <c r="A35" s="25" t="s">
         <v>703</v>
       </c>
@@ -16024,7 +16110,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="50.1" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:12" ht="51" x14ac:dyDescent="0.35">
       <c r="A36" s="25" t="s">
         <v>705</v>
       </c>
@@ -16062,7 +16148,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="136.19999999999999" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:12" ht="138.5" x14ac:dyDescent="0.35">
       <c r="A37" s="25" t="s">
         <v>707</v>
       </c>
@@ -16100,7 +16186,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="111.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:12" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A38" s="25" t="s">
         <v>709</v>
       </c>
@@ -16138,7 +16224,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39" s="25" t="s">
         <v>208</v>
       </c>
@@ -16154,7 +16240,7 @@
       <c r="K39" s="25"/>
       <c r="L39" s="25"/>
     </row>
-    <row r="40" spans="1:12" ht="409.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:12" ht="409.6" x14ac:dyDescent="0.35">
       <c r="A40" s="25" t="s">
         <v>711</v>
       </c>
@@ -16190,7 +16276,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="222.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:12" ht="238.5" x14ac:dyDescent="0.35">
       <c r="A41" s="25" t="s">
         <v>713</v>
       </c>
@@ -16228,7 +16314,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="409.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:12" ht="409.6" x14ac:dyDescent="0.35">
       <c r="A42" s="25" t="s">
         <v>715</v>
       </c>
@@ -16266,7 +16352,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="123.9" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:12" ht="126" x14ac:dyDescent="0.35">
       <c r="A43" s="25" t="s">
         <v>717</v>
       </c>
@@ -16304,7 +16390,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44" s="25" t="s">
         <v>214</v>
       </c>
@@ -16320,7 +16406,7 @@
       <c r="K44" s="25"/>
       <c r="L44" s="25"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45" s="25" t="s">
         <v>215</v>
       </c>
@@ -16336,7 +16422,7 @@
       <c r="K45" s="25"/>
       <c r="L45" s="25"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46" s="25" t="s">
         <v>216</v>
       </c>
@@ -16352,7 +16438,7 @@
       <c r="K46" s="25"/>
       <c r="L46" s="25"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47" s="25" t="s">
         <v>217</v>
       </c>
@@ -16368,7 +16454,7 @@
       <c r="K47" s="25"/>
       <c r="L47" s="25"/>
     </row>
-    <row r="48" spans="1:12" ht="62.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:12" ht="76" x14ac:dyDescent="0.35">
       <c r="A48" s="25" t="s">
         <v>719</v>
       </c>
@@ -16406,7 +16492,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="111.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:12" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A49" s="25" t="s">
         <v>721</v>
       </c>
@@ -16444,7 +16530,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="136.19999999999999" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:12" ht="138.5" x14ac:dyDescent="0.35">
       <c r="A50" s="25" t="s">
         <v>723</v>
       </c>
@@ -16482,7 +16568,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="50.1" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:12" ht="51" x14ac:dyDescent="0.35">
       <c r="A51" s="25" t="s">
         <v>725</v>
       </c>
@@ -16520,7 +16606,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="50.1" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:12" ht="51" x14ac:dyDescent="0.35">
       <c r="A52" s="25" t="s">
         <v>727</v>
       </c>
@@ -16558,7 +16644,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="50.1" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:12" ht="51" x14ac:dyDescent="0.35">
       <c r="A53" s="25" t="s">
         <v>729</v>
       </c>
@@ -16596,7 +16682,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="123.9" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:12" ht="126" x14ac:dyDescent="0.35">
       <c r="A54" s="25" t="s">
         <v>731</v>
       </c>
@@ -16634,7 +16720,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="409.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:12" ht="409.6" x14ac:dyDescent="0.35">
       <c r="A55" s="25" t="s">
         <v>733</v>
       </c>
@@ -16672,7 +16758,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="123.9" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:12" ht="126" x14ac:dyDescent="0.35">
       <c r="A56" s="25" t="s">
         <v>735</v>
       </c>
@@ -16710,7 +16796,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A57" s="25" t="s">
         <v>233</v>
       </c>
@@ -16726,7 +16812,7 @@
       <c r="K57" s="25"/>
       <c r="L57" s="25"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A58" s="25" t="s">
         <v>234</v>
       </c>
@@ -16742,7 +16828,7 @@
       <c r="K58" s="25"/>
       <c r="L58" s="25"/>
     </row>
-    <row r="59" spans="1:12" ht="409.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:12" ht="409.6" x14ac:dyDescent="0.35">
       <c r="A59" s="25" t="s">
         <v>737</v>
       </c>
@@ -16780,7 +16866,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A60" s="25" t="s">
         <v>237</v>
       </c>
@@ -16796,7 +16882,7 @@
       <c r="K60" s="25"/>
       <c r="L60" s="25"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A61" s="25" t="s">
         <v>238</v>
       </c>
@@ -16812,7 +16898,7 @@
       <c r="K61" s="25"/>
       <c r="L61" s="25"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A62" s="25" t="s">
         <v>239</v>
       </c>
@@ -16828,7 +16914,7 @@
       <c r="K62" s="25"/>
       <c r="L62" s="25"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A63" s="25" t="s">
         <v>240</v>
       </c>
@@ -16844,7 +16930,7 @@
       <c r="K63" s="25"/>
       <c r="L63" s="25"/>
     </row>
-    <row r="64" spans="1:12" ht="50.1" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:12" ht="51" x14ac:dyDescent="0.35">
       <c r="A64" s="25" t="s">
         <v>739</v>
       </c>
@@ -16882,7 +16968,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="409.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:12" ht="409.6" x14ac:dyDescent="0.35">
       <c r="A65" s="25" t="s">
         <v>741</v>
       </c>
@@ -16918,7 +17004,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:12" ht="111.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:12" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A66" s="25" t="s">
         <v>743</v>
       </c>
@@ -16956,7 +17042,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:12" ht="111.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:12" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A67" s="25" t="s">
         <v>745</v>
       </c>
@@ -16994,7 +17080,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:12" ht="409.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:12" ht="409.6" x14ac:dyDescent="0.35">
       <c r="A68" s="25" t="s">
         <v>747</v>
       </c>
@@ -17032,7 +17118,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:12" ht="111.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:12" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A69" s="25" t="s">
         <v>749</v>
       </c>
@@ -17070,7 +17156,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:12" ht="409.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:12" ht="409.6" x14ac:dyDescent="0.35">
       <c r="A70" s="25" t="s">
         <v>751</v>
       </c>
@@ -17108,7 +17194,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A71" s="25" t="s">
         <v>253</v>
       </c>
@@ -17124,7 +17210,7 @@
       <c r="K71" s="25"/>
       <c r="L71" s="25"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A72" s="25" t="s">
         <v>254</v>
       </c>
@@ -17140,7 +17226,7 @@
       <c r="K72" s="25"/>
       <c r="L72" s="25"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A73" s="25" t="s">
         <v>255</v>
       </c>
@@ -17156,7 +17242,7 @@
       <c r="K73" s="25"/>
       <c r="L73" s="25"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A74" s="25" t="s">
         <v>256</v>
       </c>
@@ -17172,7 +17258,7 @@
       <c r="K74" s="25"/>
       <c r="L74" s="25"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A75" s="25" t="s">
         <v>257</v>
       </c>
@@ -17188,7 +17274,7 @@
       <c r="K75" s="25"/>
       <c r="L75" s="25"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A76" s="25" t="s">
         <v>258</v>
       </c>
@@ -17204,7 +17290,7 @@
       <c r="K76" s="25"/>
       <c r="L76" s="25"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A77" s="25" t="s">
         <v>259</v>
       </c>
@@ -17218,7 +17304,7 @@
       <c r="J77" s="25"/>
       <c r="L77" s="25"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A78" s="25" t="s">
         <v>260</v>
       </c>
@@ -17232,7 +17318,7 @@
       <c r="J78" s="25"/>
       <c r="L78" s="25"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A79" s="25" t="s">
         <v>261</v>
       </c>
@@ -17246,7 +17332,7 @@
       <c r="J79" s="25"/>
       <c r="L79" s="25"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A80" s="25" t="s">
         <v>262</v>
       </c>
@@ -17260,7 +17346,7 @@
       <c r="J80" s="25"/>
       <c r="L80" s="25"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A81" s="25" t="s">
         <v>263</v>
       </c>
@@ -17274,7 +17360,7 @@
       <c r="J81" s="25"/>
       <c r="L81" s="25"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A82" s="25" t="s">
         <v>264</v>
       </c>
@@ -17288,7 +17374,7 @@
       <c r="J82" s="25"/>
       <c r="L82" s="25"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A83" s="25" t="s">
         <v>265</v>
       </c>
@@ -17302,7 +17388,7 @@
       <c r="J83" s="25"/>
       <c r="L83" s="25"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A84" s="25" t="s">
         <v>266</v>
       </c>
@@ -17316,7 +17402,7 @@
       <c r="J84" s="25"/>
       <c r="L84" s="25"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A85" s="25" t="s">
         <v>267</v>
       </c>
@@ -17330,7 +17416,7 @@
       <c r="J85" s="25"/>
       <c r="L85" s="25"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A86" s="25" t="s">
         <v>268</v>
       </c>
@@ -17344,7 +17430,7 @@
       <c r="J86" s="25"/>
       <c r="L86" s="25"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A87" s="25" t="s">
         <v>269</v>
       </c>
@@ -17358,7 +17444,7 @@
       <c r="J87" s="25"/>
       <c r="L87" s="25"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A88" s="25" t="s">
         <v>270</v>
       </c>
@@ -17372,7 +17458,7 @@
       <c r="J88" s="25"/>
       <c r="L88" s="25"/>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A89" s="25" t="s">
         <v>271</v>
       </c>
@@ -17386,7 +17472,7 @@
       <c r="J89" s="25"/>
       <c r="L89" s="25"/>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A90" s="25" t="s">
         <v>272</v>
       </c>
@@ -17400,7 +17486,7 @@
       <c r="J90" s="25"/>
       <c r="L90" s="25"/>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A91" s="25" t="s">
         <v>273</v>
       </c>
@@ -17414,7 +17500,7 @@
       <c r="J91" s="25"/>
       <c r="L91" s="25"/>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A92" s="25" t="s">
         <v>274</v>
       </c>
@@ -17428,7 +17514,7 @@
       <c r="J92" s="25"/>
       <c r="L92" s="25"/>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A93" s="25" t="s">
         <v>275</v>
       </c>
@@ -17442,7 +17528,7 @@
       <c r="J93" s="25"/>
       <c r="L93" s="25"/>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A94" s="25" t="s">
         <v>276</v>
       </c>
@@ -17456,7 +17542,7 @@
       <c r="J94" s="25"/>
       <c r="L94" s="25"/>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A95" s="25" t="s">
         <v>277</v>
       </c>
@@ -17470,7 +17556,7 @@
       <c r="J95" s="25"/>
       <c r="L95" s="25"/>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A96" s="25" t="s">
         <v>278</v>
       </c>
@@ -17484,7 +17570,7 @@
       <c r="J96" s="25"/>
       <c r="L96" s="25"/>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A97" s="25" t="s">
         <v>279</v>
       </c>
@@ -17498,7 +17584,7 @@
       <c r="J97" s="25"/>
       <c r="L97" s="25"/>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A98" s="25" t="s">
         <v>280</v>
       </c>
@@ -17512,7 +17598,7 @@
       <c r="J98" s="25"/>
       <c r="L98" s="25"/>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A99" s="25" t="s">
         <v>281</v>
       </c>
@@ -17526,7 +17612,7 @@
       <c r="J99" s="25"/>
       <c r="L99" s="25"/>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A100" s="25" t="s">
         <v>282</v>
       </c>
@@ -17540,7 +17626,7 @@
       <c r="J100" s="25"/>
       <c r="L100" s="25"/>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A101" s="25" t="s">
         <v>283</v>
       </c>
@@ -17554,7 +17640,7 @@
       <c r="J101" s="25"/>
       <c r="L101" s="25"/>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A102" s="25" t="s">
         <v>284</v>
       </c>
@@ -17568,7 +17654,7 @@
       <c r="J102" s="25"/>
       <c r="L102" s="25"/>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A103" s="25" t="s">
         <v>285</v>
       </c>
@@ -17582,7 +17668,7 @@
       <c r="J103" s="25"/>
       <c r="L103" s="25"/>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A104" s="25" t="s">
         <v>286</v>
       </c>
@@ -17596,7 +17682,7 @@
       <c r="J104" s="25"/>
       <c r="L104" s="25"/>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A105" s="25" t="s">
         <v>287</v>
       </c>
@@ -17610,7 +17696,7 @@
       <c r="J105" s="25"/>
       <c r="L105" s="25"/>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A106" s="25" t="s">
         <v>288</v>
       </c>
@@ -17624,7 +17710,7 @@
       <c r="J106" s="25"/>
       <c r="L106" s="25"/>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A107" s="25" t="s">
         <v>289</v>
       </c>
@@ -17638,7 +17724,7 @@
       <c r="J107" s="25"/>
       <c r="L107" s="25"/>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A108" s="25" t="s">
         <v>290</v>
       </c>
@@ -17652,7 +17738,7 @@
       <c r="J108" s="25"/>
       <c r="L108" s="25"/>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A109" s="25" t="s">
         <v>291</v>
       </c>
@@ -17666,7 +17752,7 @@
       <c r="J109" s="25"/>
       <c r="L109" s="25"/>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A110" s="25" t="s">
         <v>292</v>
       </c>
@@ -17680,7 +17766,7 @@
       <c r="J110" s="25"/>
       <c r="L110" s="25"/>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A111" s="25" t="s">
         <v>293</v>
       </c>
@@ -17694,7 +17780,7 @@
       <c r="J111" s="25"/>
       <c r="L111" s="25"/>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A112" s="25" t="s">
         <v>294</v>
       </c>
@@ -17708,7 +17794,7 @@
       <c r="J112" s="25"/>
       <c r="L112" s="25"/>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A113" s="25" t="s">
         <v>295</v>
       </c>
@@ -17722,7 +17808,7 @@
       <c r="J113" s="25"/>
       <c r="L113" s="25"/>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A114" s="25" t="s">
         <v>296</v>
       </c>
@@ -17736,7 +17822,7 @@
       <c r="J114" s="25"/>
       <c r="L114" s="25"/>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A115" s="25" t="s">
         <v>297</v>
       </c>
@@ -17750,7 +17836,7 @@
       <c r="J115" s="25"/>
       <c r="L115" s="25"/>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A116" s="25" t="s">
         <v>298</v>
       </c>
@@ -17764,7 +17850,7 @@
       <c r="J116" s="25"/>
       <c r="L116" s="25"/>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A117" s="25" t="s">
         <v>299</v>
       </c>
@@ -17778,7 +17864,7 @@
       <c r="J117" s="25"/>
       <c r="L117" s="25"/>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A118" s="25" t="s">
         <v>300</v>
       </c>
@@ -17792,7 +17878,7 @@
       <c r="J118" s="25"/>
       <c r="L118" s="25"/>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A119" s="25" t="s">
         <v>301</v>
       </c>
@@ -17806,7 +17892,7 @@
       <c r="J119" s="25"/>
       <c r="L119" s="25"/>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A120" s="25" t="s">
         <v>302</v>
       </c>
@@ -17820,7 +17906,7 @@
       <c r="J120" s="25"/>
       <c r="L120" s="25"/>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A121" s="25" t="s">
         <v>303</v>
       </c>
@@ -17834,7 +17920,7 @@
       <c r="J121" s="25"/>
       <c r="L121" s="25"/>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A122" s="25" t="s">
         <v>304</v>
       </c>
@@ -17848,7 +17934,7 @@
       <c r="J122" s="25"/>
       <c r="L122" s="25"/>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A123" s="25" t="s">
         <v>305</v>
       </c>
@@ -17860,7 +17946,7 @@
       <c r="G123" s="25"/>
       <c r="H123" s="25"/>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A124" s="25" t="s">
         <v>306</v>
       </c>
@@ -17872,7 +17958,7 @@
       <c r="G124" s="25"/>
       <c r="H124" s="25"/>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A125" s="25" t="s">
         <v>307</v>
       </c>
@@ -17884,7 +17970,7 @@
       <c r="G125" s="25"/>
       <c r="H125" s="25"/>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A126" s="25" t="s">
         <v>308</v>
       </c>
@@ -17896,7 +17982,7 @@
       <c r="G126" s="25"/>
       <c r="H126" s="25"/>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A127" s="25" t="s">
         <v>309</v>
       </c>
@@ -17908,7 +17994,7 @@
       <c r="G127" s="25"/>
       <c r="H127" s="25"/>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A128" s="25" t="s">
         <v>310</v>
       </c>
@@ -17920,7 +18006,7 @@
       <c r="G128" s="25"/>
       <c r="H128" s="25"/>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A129" s="25" t="s">
         <v>311</v>
       </c>
@@ -17932,7 +18018,7 @@
       <c r="G129" s="25"/>
       <c r="H129" s="25"/>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A130" s="25" t="s">
         <v>312</v>
       </c>
@@ -17944,7 +18030,7 @@
       <c r="G130" s="25"/>
       <c r="H130" s="25"/>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A131" s="25" t="s">
         <v>313</v>
       </c>
@@ -17956,7 +18042,7 @@
       <c r="G131" s="25"/>
       <c r="H131" s="25"/>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A132" s="25" t="s">
         <v>314</v>
       </c>
@@ -17968,7 +18054,7 @@
       <c r="G132" s="25"/>
       <c r="H132" s="25"/>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A133" s="25" t="s">
         <v>315</v>
       </c>
@@ -17980,7 +18066,7 @@
       <c r="G133" s="25"/>
       <c r="H133" s="25"/>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A134" s="25" t="s">
         <v>316</v>
       </c>
@@ -17992,7 +18078,7 @@
       <c r="G134" s="25"/>
       <c r="H134" s="25"/>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A135" s="25" t="s">
         <v>317</v>
       </c>
@@ -18004,7 +18090,7 @@
       <c r="G135" s="25"/>
       <c r="H135" s="25"/>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A136" s="25" t="s">
         <v>318</v>
       </c>
@@ -18016,7 +18102,7 @@
       <c r="G136" s="25"/>
       <c r="H136" s="25"/>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A137" s="25" t="s">
         <v>319</v>
       </c>
@@ -18028,7 +18114,7 @@
       <c r="G137" s="25"/>
       <c r="H137" s="25"/>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A138" s="25" t="s">
         <v>320</v>
       </c>
@@ -18040,7 +18126,7 @@
       <c r="G138" s="25"/>
       <c r="H138" s="25"/>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A139" s="25" t="s">
         <v>321</v>
       </c>
@@ -18052,7 +18138,7 @@
       <c r="G139" s="25"/>
       <c r="H139" s="25"/>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A140" s="25" t="s">
         <v>322</v>
       </c>
@@ -18064,7 +18150,7 @@
       <c r="G140" s="25"/>
       <c r="H140" s="25"/>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A141" s="25" t="s">
         <v>323</v>
       </c>
@@ -18076,7 +18162,7 @@
       <c r="G141" s="25"/>
       <c r="H141" s="25"/>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A142" s="25" t="s">
         <v>324</v>
       </c>
@@ -18088,7 +18174,7 @@
       <c r="G142" s="25"/>
       <c r="H142" s="25"/>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A143" s="25" t="s">
         <v>325</v>
       </c>
@@ -18100,7 +18186,7 @@
       <c r="G143" s="25"/>
       <c r="H143" s="25"/>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A144" s="25" t="s">
         <v>326</v>
       </c>
@@ -18112,7 +18198,7 @@
       <c r="G144" s="25"/>
       <c r="H144" s="25"/>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A145" s="25" t="s">
         <v>327</v>
       </c>
@@ -18124,7 +18210,7 @@
       <c r="G145" s="25"/>
       <c r="H145" s="25"/>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A146" s="25" t="s">
         <v>328</v>
       </c>
@@ -18136,7 +18222,7 @@
       <c r="G146" s="25"/>
       <c r="H146" s="25"/>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A147" s="25" t="s">
         <v>329</v>
       </c>
@@ -18148,7 +18234,7 @@
       <c r="G147" s="25"/>
       <c r="H147" s="25"/>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A148" s="25" t="s">
         <v>330</v>
       </c>
@@ -18160,7 +18246,7 @@
       <c r="G148" s="25"/>
       <c r="H148" s="25"/>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A149" s="25" t="s">
         <v>331</v>
       </c>
@@ -18172,7 +18258,7 @@
       <c r="G149" s="25"/>
       <c r="H149" s="25"/>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A150" s="25" t="s">
         <v>332</v>
       </c>
@@ -18184,7 +18270,7 @@
       <c r="G150" s="25"/>
       <c r="H150" s="25"/>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A151" s="25" t="s">
         <v>333</v>
       </c>
@@ -18196,7 +18282,7 @@
       <c r="G151" s="25"/>
       <c r="H151" s="25"/>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A152" s="25" t="s">
         <v>334</v>
       </c>
@@ -18208,7 +18294,7 @@
       <c r="G152" s="25"/>
       <c r="H152" s="25"/>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A153" s="25" t="s">
         <v>335</v>
       </c>
@@ -18220,7 +18306,7 @@
       <c r="G153" s="25"/>
       <c r="H153" s="25"/>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A154" s="25" t="s">
         <v>336</v>
       </c>
@@ -18232,7 +18318,7 @@
       <c r="G154" s="25"/>
       <c r="H154" s="25"/>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A155" s="25" t="s">
         <v>337</v>
       </c>
@@ -18244,7 +18330,7 @@
       <c r="G155" s="25"/>
       <c r="H155" s="25"/>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A156" s="25" t="s">
         <v>338</v>
       </c>
@@ -18256,7 +18342,7 @@
       <c r="G156" s="25"/>
       <c r="H156" s="25"/>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A157" s="25" t="s">
         <v>339</v>
       </c>
@@ -18268,7 +18354,7 @@
       <c r="G157" s="25"/>
       <c r="H157" s="25"/>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A158" s="25" t="s">
         <v>340</v>
       </c>
@@ -18280,7 +18366,7 @@
       <c r="G158" s="25"/>
       <c r="H158" s="25"/>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A159" s="25" t="s">
         <v>341</v>
       </c>
@@ -18292,7 +18378,7 @@
       <c r="G159" s="25"/>
       <c r="H159" s="25"/>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A160" s="25" t="s">
         <v>342</v>
       </c>
@@ -18304,7 +18390,7 @@
       <c r="G160" s="25"/>
       <c r="H160" s="25"/>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A161" s="25" t="s">
         <v>343</v>
       </c>
@@ -18316,7 +18402,7 @@
       <c r="G161" s="25"/>
       <c r="H161" s="25"/>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A162" s="25" t="s">
         <v>344</v>
       </c>
@@ -18328,7 +18414,7 @@
       <c r="G162" s="25"/>
       <c r="H162" s="25"/>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A163" s="25" t="s">
         <v>345</v>
       </c>
@@ -18340,7 +18426,7 @@
       <c r="G163" s="25"/>
       <c r="H163" s="25"/>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A164" s="25" t="s">
         <v>346</v>
       </c>
@@ -18352,7 +18438,7 @@
       <c r="G164" s="25"/>
       <c r="H164" s="25"/>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A165" s="25" t="s">
         <v>347</v>
       </c>
@@ -18379,18 +18465,18 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="15.5234375" customWidth="1"/>
-    <col min="4" max="4" width="26.7890625" customWidth="1"/>
-    <col min="5" max="5" width="21.7890625" customWidth="1"/>
-    <col min="6" max="8" width="15.5234375" customWidth="1"/>
-    <col min="9" max="9" width="13.15625" customWidth="1"/>
-    <col min="10" max="10" width="13.7890625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.47265625" customWidth="1"/>
+    <col min="1" max="3" width="15.54296875" customWidth="1"/>
+    <col min="4" max="4" width="26.81640625" customWidth="1"/>
+    <col min="5" max="5" width="21.81640625" customWidth="1"/>
+    <col min="6" max="8" width="15.54296875" customWidth="1"/>
+    <col min="9" max="9" width="13.1796875" customWidth="1"/>
+    <col min="10" max="10" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="14" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:16" s="14" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>567</v>
       </c>
@@ -18440,7 +18526,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="4" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:16" s="4" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -18490,7 +18576,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="4" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:16" s="4" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -18540,7 +18626,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="4" customFormat="1" ht="144" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:16" s="4" customFormat="1" ht="145" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -18590,7 +18676,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="4" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:16" s="4" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -18640,7 +18726,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="4" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:16" s="4" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -18690,7 +18776,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:16" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -18740,7 +18826,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="4" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:16" s="4" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -18790,7 +18876,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -18800,7 +18886,7 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -18810,7 +18896,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -18820,9 +18906,9 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="13" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="14" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="12" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -18838,23 +18924,23 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.734375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="15.5234375" style="19" customWidth="1"/>
-    <col min="4" max="4" width="14.5234375" style="19" customWidth="1"/>
-    <col min="5" max="5" width="14.15625" style="19" customWidth="1"/>
-    <col min="6" max="8" width="15.5234375" style="19" customWidth="1"/>
-    <col min="9" max="9" width="14.26171875" style="19" customWidth="1"/>
-    <col min="10" max="10" width="11.26171875" style="19" customWidth="1"/>
-    <col min="11" max="11" width="11.5234375" style="19" customWidth="1"/>
-    <col min="12" max="12" width="12.47265625" style="19" customWidth="1"/>
-    <col min="13" max="14" width="8.734375" style="19"/>
-    <col min="15" max="15" width="11.1015625" style="19" customWidth="1"/>
-    <col min="16" max="16" width="11.47265625" style="19" customWidth="1"/>
-    <col min="17" max="16384" width="8.734375" style="19"/>
+    <col min="1" max="3" width="15.54296875" style="19" customWidth="1"/>
+    <col min="4" max="4" width="14.54296875" style="19" customWidth="1"/>
+    <col min="5" max="5" width="14.1796875" style="19" customWidth="1"/>
+    <col min="6" max="8" width="15.54296875" style="19" customWidth="1"/>
+    <col min="9" max="9" width="14.26953125" style="19" customWidth="1"/>
+    <col min="10" max="10" width="11.26953125" style="19" customWidth="1"/>
+    <col min="11" max="11" width="11.54296875" style="19" customWidth="1"/>
+    <col min="12" max="12" width="12.453125" style="19" customWidth="1"/>
+    <col min="13" max="14" width="8.7265625" style="19"/>
+    <col min="15" max="15" width="11.08984375" style="19" customWidth="1"/>
+    <col min="16" max="16" width="11.453125" style="19" customWidth="1"/>
+    <col min="17" max="16384" width="8.7265625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="21" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:16" s="21" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>567</v>
       </c>
@@ -18904,7 +18990,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="18" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:16" s="18" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18">
         <v>1</v>
       </c>
@@ -18954,7 +19040,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="18" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:16" s="18" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="18">
         <v>2</v>
       </c>
@@ -19004,7 +19090,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="18" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:16" s="18" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A4" s="18">
         <v>3</v>
       </c>
@@ -19054,7 +19140,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="40" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:16" s="40" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="40">
         <v>4</v>
       </c>
@@ -19104,16 +19190,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="7" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="8" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="9" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="10" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="11" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="12" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="13" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="14" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="15" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="6" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="9" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -19121,26 +19207,27 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{038D9871-6BF2-4210-AB19-5595569BDB87}">
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:R16"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="15.5234375" customWidth="1"/>
-    <col min="4" max="4" width="26.7890625" customWidth="1"/>
-    <col min="5" max="5" width="21.7890625" customWidth="1"/>
-    <col min="6" max="8" width="15.5234375" customWidth="1"/>
-    <col min="9" max="9" width="16.734375" customWidth="1"/>
-    <col min="10" max="10" width="14.15625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.7890625" customWidth="1"/>
-    <col min="12" max="12" width="15.7890625" customWidth="1"/>
+    <col min="1" max="3" width="15.54296875" customWidth="1"/>
+    <col min="4" max="4" width="26.81640625" customWidth="1"/>
+    <col min="5" max="5" width="21.81640625" customWidth="1"/>
+    <col min="6" max="8" width="15.54296875" customWidth="1"/>
+    <col min="9" max="9" width="16.7265625" customWidth="1"/>
+    <col min="10" max="10" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.81640625" customWidth="1"/>
+    <col min="12" max="12" width="15.81640625" customWidth="1"/>
+    <col min="17" max="17" width="15.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:18" s="12" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>567</v>
       </c>
@@ -19189,8 +19276,14 @@
       <c r="P1" s="48" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q1" s="22" t="s">
+        <v>802</v>
+      </c>
+      <c r="R1" s="11" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -19239,8 +19332,14 @@
       <c r="P2" s="6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q2" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -19289,8 +19388,14 @@
       <c r="P3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" s="4" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q3" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" s="4" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -19339,8 +19444,14 @@
       <c r="P4" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" s="4" customFormat="1" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q4" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" s="4" customFormat="1" ht="174" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -19389,8 +19500,14 @@
       <c r="P5" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" ht="124.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q5" s="1" t="s">
+        <v>847</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="124.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -19439,8 +19556,14 @@
       <c r="P6" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" ht="124.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q6" s="8" t="s">
+        <v>413</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="124.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -19489,8 +19612,14 @@
       <c r="P7" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q7" s="8" t="s">
+        <v>413</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -19539,8 +19668,14 @@
       <c r="P8" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q8" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -19557,40 +19692,46 @@
         <v>392</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>429</v>
+        <v>845</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>429</v>
+        <v>845</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>4</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>429</v>
+        <v>845</v>
       </c>
       <c r="J9" s="7" t="s">
         <v>4</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>429</v>
+        <v>845</v>
       </c>
       <c r="L9" s="7" t="s">
         <v>4</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>429</v>
+        <v>845</v>
       </c>
       <c r="N9" s="7" t="s">
         <v>4</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>429</v>
+        <v>845</v>
       </c>
       <c r="P9" s="7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q9" s="1" t="s">
+        <v>845</v>
+      </c>
+      <c r="R9" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -19639,8 +19780,14 @@
       <c r="P10" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q10" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A11" s="7">
         <v>9</v>
       </c>
@@ -19689,8 +19836,14 @@
       <c r="P11" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q11" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A12" s="7">
         <v>10</v>
       </c>
@@ -19707,40 +19860,46 @@
         <v>392</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>430</v>
+        <v>844</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>430</v>
+        <v>844</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>430</v>
+        <v>844</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>430</v>
+        <v>844</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>4</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>430</v>
+        <v>844</v>
       </c>
       <c r="N12" s="1" t="s">
         <v>4</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>430</v>
+        <v>844</v>
       </c>
       <c r="P12" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q12" s="1" t="s">
+        <v>844</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A13" s="7">
         <v>11</v>
       </c>
@@ -19756,8 +19915,8 @@
       <c r="E13" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="F13" s="4" t="s">
-        <v>443</v>
+      <c r="F13" s="1" t="s">
+        <v>430</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>430</v>
@@ -19789,8 +19948,14 @@
       <c r="P13" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q13" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A14" s="7">
         <v>12</v>
       </c>
@@ -19807,40 +19972,46 @@
         <v>392</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>443</v>
+        <v>842</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>443</v>
+        <v>842</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>443</v>
+        <v>842</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>443</v>
+        <v>842</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>4</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>443</v>
+        <v>842</v>
       </c>
       <c r="N14" s="1" t="s">
         <v>4</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>443</v>
+        <v>842</v>
       </c>
       <c r="P14" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q14" s="4" t="s">
+        <v>842</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A15" s="7">
         <v>13</v>
       </c>
@@ -19857,36 +20028,68 @@
         <v>392</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>430</v>
+        <v>843</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>430</v>
+        <v>843</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>430</v>
+        <v>843</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>430</v>
+        <v>843</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>4</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>430</v>
+        <v>843</v>
       </c>
       <c r="N15" s="1" t="s">
         <v>4</v>
       </c>
       <c r="O15" s="4" t="s">
-        <v>430</v>
+        <v>843</v>
       </c>
       <c r="P15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q15" s="4" t="s">
+        <v>843</v>
+      </c>
+      <c r="R15" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="7">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>846</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>842</v>
+      </c>
+      <c r="Q16" s="4" t="s">
+        <v>842</v>
+      </c>
+      <c r="R16" t="s">
         <v>4</v>
       </c>
     </row>
@@ -19902,22 +20105,22 @@
   <sheetViews>
     <sheetView zoomScale="72" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W7" sqref="W7:X7"/>
+      <selection pane="bottomLeft" activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="15.5234375" customWidth="1"/>
-    <col min="4" max="4" width="26.7890625" customWidth="1"/>
-    <col min="5" max="5" width="21.7890625" customWidth="1"/>
-    <col min="6" max="6" width="15.5234375" customWidth="1"/>
-    <col min="7" max="7" width="11.734375" customWidth="1"/>
-    <col min="8" max="9" width="11.7890625" customWidth="1"/>
-    <col min="17" max="17" width="12.26171875" customWidth="1"/>
-    <col min="18" max="18" width="12.5234375" customWidth="1"/>
+    <col min="1" max="3" width="15.54296875" customWidth="1"/>
+    <col min="4" max="4" width="26.81640625" customWidth="1"/>
+    <col min="5" max="5" width="21.81640625" customWidth="1"/>
+    <col min="6" max="6" width="15.54296875" customWidth="1"/>
+    <col min="7" max="7" width="11.7265625" customWidth="1"/>
+    <col min="8" max="9" width="11.81640625" customWidth="1"/>
+    <col min="17" max="17" width="12.26953125" customWidth="1"/>
+    <col min="18" max="18" width="12.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:24" s="12" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>567</v>
       </c>
@@ -19981,17 +20184,17 @@
       <c r="U1" s="27" t="s">
         <v>639</v>
       </c>
-      <c r="V1" s="27" t="s">
+      <c r="V1" s="11" t="s">
         <v>640</v>
       </c>
-      <c r="W1" s="22" t="s">
+      <c r="W1" s="11" t="s">
         <v>630</v>
       </c>
       <c r="X1" s="11" t="s">
         <v>631</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:24" ht="116" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -20065,7 +20268,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:24" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -20139,7 +20342,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:24" ht="145" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -20213,7 +20416,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:24" ht="345.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:24" ht="348" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -20287,7 +20490,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:24" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -20361,7 +20564,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:24" ht="87" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -20442,24 +20645,24 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D48F8994-0480-456C-9C73-8DEBC1CF05E8}">
-  <dimension ref="A1:Z25"/>
+  <dimension ref="A1:AB26"/>
   <sheetViews>
-    <sheetView zoomScale="74" zoomScaleNormal="78" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="74" zoomScaleNormal="78" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Z26" sqref="Y26:Z26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="4" width="15.5234375" customWidth="1"/>
-    <col min="5" max="5" width="23.1015625" customWidth="1"/>
-    <col min="6" max="6" width="15.5234375" customWidth="1"/>
-    <col min="7" max="7" width="16.89453125" customWidth="1"/>
-    <col min="8" max="8" width="16.47265625" customWidth="1"/>
-    <col min="15" max="15" width="15.26171875" customWidth="1"/>
+    <col min="1" max="4" width="15.54296875" customWidth="1"/>
+    <col min="5" max="5" width="23.08984375" customWidth="1"/>
+    <col min="6" max="6" width="15.54296875" customWidth="1"/>
+    <col min="7" max="7" width="16.90625" customWidth="1"/>
+    <col min="8" max="8" width="16.453125" customWidth="1"/>
+    <col min="15" max="15" width="15.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="24" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:28" s="24" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>567</v>
       </c>
@@ -20538,8 +20741,14 @@
       <c r="Z1" s="11" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="AA1" s="22" t="s">
+        <v>802</v>
+      </c>
+      <c r="AB1" s="11" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -20618,8 +20827,14 @@
       <c r="Z2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="AA2" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" ht="87" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -20698,8 +20913,14 @@
       <c r="Z3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="AA3" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -20778,8 +20999,14 @@
       <c r="Z4" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:26" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="AA4" s="1" t="s">
+        <v>848</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -20858,8 +21085,14 @@
       <c r="Z5" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:26" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="AA5" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -20938,8 +21171,14 @@
       <c r="Z6" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:26" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="AA6" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" ht="87" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -21018,8 +21257,14 @@
       <c r="Z7" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:26" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="AA7" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="AB7" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -21098,8 +21343,14 @@
       <c r="Z8" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:26" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="AA8" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="AB8" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" ht="87" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -21178,8 +21429,14 @@
       <c r="Z9" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:26" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="AA9" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB9" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -21258,8 +21515,14 @@
       <c r="Z10" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:26" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="AA10" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AB10" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -21338,8 +21601,14 @@
       <c r="Z11" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:26" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="AA11" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AB11" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" ht="58" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -21418,8 +21687,14 @@
       <c r="Z12" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:26" ht="144" x14ac:dyDescent="0.55000000000000004">
+      <c r="AA12" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AB12" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" ht="145" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -21498,8 +21773,14 @@
       <c r="Z13" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:26" ht="144" x14ac:dyDescent="0.55000000000000004">
+      <c r="AA13" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="AB13" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" ht="145" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -21578,8 +21859,14 @@
       <c r="Z14" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:26" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AA14" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="AB14" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" ht="203" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -21658,8 +21945,14 @@
       <c r="Z15" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:26" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="AA15" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AB15" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" ht="87" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -21738,8 +22031,14 @@
       <c r="Z16" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:26" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="AA16" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="AB16" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -21818,8 +22117,14 @@
       <c r="Z17" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:26" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="AA17" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="AB17" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" ht="87" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -21898,8 +22203,14 @@
       <c r="Z18" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:26" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="AA18" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AB18" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" ht="87" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -21978,8 +22289,14 @@
       <c r="Z19" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:26" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="AA19" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="AB19" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -22042,8 +22359,14 @@
       <c r="Z20" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:26" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="AA20" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AB20" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" ht="58" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -22122,8 +22445,14 @@
       <c r="Z21" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:26" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="AA21" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="AB21" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -22202,8 +22531,14 @@
       <c r="Z22" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:26" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="AA22" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="AB22" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -22282,8 +22617,14 @@
       <c r="Z23" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:26" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="AA23" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="AB23" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" ht="87" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -22362,8 +22703,14 @@
       <c r="Z24" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="25" spans="1:26" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="AA24" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="AB24" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" ht="58" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -22440,6 +22787,40 @@
         <v>442</v>
       </c>
       <c r="Z25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA25" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="AB25" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>838</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>839</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>840</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>841</v>
+      </c>
+      <c r="Y26" s="1"/>
+      <c r="Z26" s="1"/>
+      <c r="AA26" s="1" t="s">
+        <v>849</v>
+      </c>
+      <c r="AB26" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -22450,28 +22831,29 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55C5E1F7-185F-4415-A762-CA1DF36823C6}">
-  <dimension ref="A1:R9"/>
+  <dimension ref="A1:T10"/>
   <sheetViews>
     <sheetView zoomScale="69" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S1" sqref="S1:T1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="15.5234375" customWidth="1"/>
-    <col min="4" max="4" width="14.47265625" customWidth="1"/>
-    <col min="5" max="5" width="13.47265625" customWidth="1"/>
-    <col min="6" max="7" width="15.5234375" customWidth="1"/>
-    <col min="8" max="8" width="8.47265625" customWidth="1"/>
-    <col min="9" max="9" width="12.5234375" customWidth="1"/>
+    <col min="1" max="3" width="15.54296875" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" customWidth="1"/>
+    <col min="5" max="5" width="13.453125" customWidth="1"/>
+    <col min="6" max="7" width="15.54296875" customWidth="1"/>
+    <col min="8" max="8" width="8.453125" customWidth="1"/>
+    <col min="9" max="9" width="12.54296875" customWidth="1"/>
     <col min="11" max="11" width="13" customWidth="1"/>
-    <col min="12" max="12" width="12.7890625" customWidth="1"/>
-    <col min="13" max="13" width="12.15625" customWidth="1"/>
-    <col min="14" max="14" width="14.47265625" customWidth="1"/>
+    <col min="12" max="12" width="12.81640625" customWidth="1"/>
+    <col min="13" max="13" width="12.1796875" customWidth="1"/>
+    <col min="14" max="14" width="14.453125" customWidth="1"/>
+    <col min="19" max="19" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:20" s="16" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>567</v>
       </c>
@@ -22526,8 +22908,14 @@
       <c r="R1" s="11" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="S1" s="22" t="s">
+        <v>802</v>
+      </c>
+      <c r="T1" s="11" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="87" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -22582,8 +22970,14 @@
       <c r="R2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="S2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="87" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -22638,8 +23032,14 @@
       <c r="R3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="S3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -22694,8 +23094,14 @@
       <c r="R4" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="S4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -22750,8 +23156,14 @@
       <c r="R5" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="S5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="145" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -22806,8 +23218,14 @@
       <c r="R6" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="S6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="87" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -22862,8 +23280,14 @@
       <c r="R7" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="S7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="87" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -22918,8 +23342,14 @@
       <c r="R8" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="S8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="87" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -22972,6 +23402,38 @@
         <v>33</v>
       </c>
       <c r="R9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="58" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>581</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>835</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>837</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="T10" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -22989,13 +23451,13 @@
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="14.734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7890625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -23021,7 +23483,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="50.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:8" ht="50.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>780</v>
       </c>
@@ -23047,7 +23509,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="63.55" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:8" ht="63.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>790</v>
       </c>
@@ -23073,7 +23535,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="50.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:8" ht="50.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>791</v>
       </c>
@@ -23099,7 +23561,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="45.55" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:8" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>792</v>
       </c>
@@ -23135,31 +23597,31 @@
   <dimension ref="A1:V32"/>
   <sheetViews>
     <sheetView topLeftCell="F1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V32" sqref="V32"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U1" sqref="U1:V1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.5234375" customWidth="1"/>
-    <col min="2" max="2" width="20.62890625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="26.7890625" customWidth="1"/>
-    <col min="6" max="6" width="25.7890625" customWidth="1"/>
-    <col min="7" max="8" width="18.47265625" customWidth="1"/>
-    <col min="9" max="9" width="16.734375" customWidth="1"/>
-    <col min="10" max="10" width="21.15625" customWidth="1"/>
-    <col min="11" max="11" width="17.7890625" customWidth="1"/>
-    <col min="12" max="12" width="17.15625" customWidth="1"/>
-    <col min="13" max="15" width="17.47265625" customWidth="1"/>
-    <col min="16" max="16" width="13.15625" customWidth="1"/>
-    <col min="17" max="17" width="17.47265625" customWidth="1"/>
-    <col min="18" max="18" width="13.734375" customWidth="1"/>
-    <col min="19" max="19" width="17.7890625" customWidth="1"/>
-    <col min="21" max="21" width="17.47265625" customWidth="1"/>
+    <col min="1" max="1" width="15.54296875" customWidth="1"/>
+    <col min="2" max="2" width="20.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="26.81640625" customWidth="1"/>
+    <col min="6" max="6" width="25.81640625" customWidth="1"/>
+    <col min="7" max="8" width="18.453125" customWidth="1"/>
+    <col min="9" max="9" width="16.7265625" customWidth="1"/>
+    <col min="10" max="10" width="21.1796875" customWidth="1"/>
+    <col min="11" max="11" width="17.81640625" customWidth="1"/>
+    <col min="12" max="12" width="17.1796875" customWidth="1"/>
+    <col min="13" max="15" width="17.453125" customWidth="1"/>
+    <col min="16" max="16" width="13.1796875" customWidth="1"/>
+    <col min="17" max="17" width="17.453125" customWidth="1"/>
+    <col min="18" max="18" width="13.7265625" customWidth="1"/>
+    <col min="19" max="19" width="17.81640625" customWidth="1"/>
+    <col min="21" max="21" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="12" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:22" s="12" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>567</v>
       </c>
@@ -23227,7 +23689,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:22" ht="145" x14ac:dyDescent="0.35">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -23295,7 +23757,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:22" ht="145" x14ac:dyDescent="0.35">
       <c r="A3" s="9">
         <v>2</v>
       </c>
@@ -23363,7 +23825,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:22" ht="145" x14ac:dyDescent="0.35">
       <c r="A4" s="9">
         <v>3</v>
       </c>
@@ -23431,7 +23893,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:22" ht="145" x14ac:dyDescent="0.35">
       <c r="A5" s="9">
         <v>4</v>
       </c>
@@ -23499,7 +23961,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:22" ht="174" x14ac:dyDescent="0.35">
       <c r="A6" s="9">
         <v>5</v>
       </c>
@@ -23567,7 +24029,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:22" ht="145" x14ac:dyDescent="0.35">
       <c r="A7" s="9">
         <v>6</v>
       </c>
@@ -23635,7 +24097,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:22" ht="145" x14ac:dyDescent="0.35">
       <c r="A8" s="9">
         <v>7</v>
       </c>
@@ -23703,7 +24165,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:22" ht="145" x14ac:dyDescent="0.35">
       <c r="A9" s="9">
         <v>8</v>
       </c>
@@ -23771,7 +24233,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:22" ht="145" x14ac:dyDescent="0.35">
       <c r="A10" s="9">
         <v>9</v>
       </c>
@@ -23839,7 +24301,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:22" ht="145" x14ac:dyDescent="0.35">
       <c r="A11" s="9">
         <v>10</v>
       </c>
@@ -23907,7 +24369,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:22" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:22" ht="145" x14ac:dyDescent="0.35">
       <c r="A12" s="9">
         <v>11</v>
       </c>
@@ -23975,7 +24437,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:22" ht="145" x14ac:dyDescent="0.35">
       <c r="A13" s="9">
         <v>12</v>
       </c>
@@ -24043,7 +24505,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:22" ht="145" x14ac:dyDescent="0.35">
       <c r="A14" s="9">
         <v>13</v>
       </c>
@@ -24111,7 +24573,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:22" ht="145" x14ac:dyDescent="0.35">
       <c r="A15" s="9">
         <v>14</v>
       </c>
@@ -24179,7 +24641,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:22" ht="145" x14ac:dyDescent="0.35">
       <c r="A16" s="9">
         <v>15</v>
       </c>
@@ -24247,7 +24709,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:22" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:22" ht="145" x14ac:dyDescent="0.35">
       <c r="A17" s="9">
         <v>16</v>
       </c>
@@ -24315,7 +24777,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:22" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:22" ht="145" x14ac:dyDescent="0.35">
       <c r="A18" s="9">
         <v>17</v>
       </c>
@@ -24383,7 +24845,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:22" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:22" ht="145" x14ac:dyDescent="0.35">
       <c r="A19" s="9">
         <v>18</v>
       </c>
@@ -24451,7 +24913,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:22" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:22" ht="145" x14ac:dyDescent="0.35">
       <c r="A20" s="9">
         <v>19</v>
       </c>
@@ -24519,7 +24981,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:22" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:22" ht="145" x14ac:dyDescent="0.35">
       <c r="A21" s="9">
         <v>20</v>
       </c>
@@ -24587,7 +25049,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:22" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:22" ht="145" x14ac:dyDescent="0.35">
       <c r="A22" s="9">
         <v>21</v>
       </c>
@@ -24655,7 +25117,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:22" ht="144" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:22" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A23" s="9">
         <v>22</v>
       </c>
@@ -24723,7 +25185,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:22" ht="144" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:22" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A24" s="9">
         <v>23</v>
       </c>
@@ -24791,7 +25253,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:22" ht="144" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:22" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A25" s="9">
         <v>24</v>
       </c>
@@ -24859,7 +25321,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:22" ht="27.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:22" ht="28" x14ac:dyDescent="0.35">
       <c r="A26" s="9">
         <v>25</v>
       </c>
@@ -24911,7 +25373,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:22" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:22" ht="145" x14ac:dyDescent="0.35">
       <c r="A27" s="9">
         <v>26</v>
       </c>
@@ -24979,7 +25441,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:22" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:22" ht="145" x14ac:dyDescent="0.35">
       <c r="A28" s="9">
         <v>27</v>
       </c>
@@ -25047,7 +25509,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:22" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:22" ht="145" x14ac:dyDescent="0.35">
       <c r="A29" s="9">
         <v>28</v>
       </c>
@@ -25115,7 +25577,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:22" ht="316.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:22" ht="333.5" x14ac:dyDescent="0.35">
       <c r="A30" s="9">
         <v>29</v>
       </c>
@@ -25165,7 +25627,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:22" ht="331.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:22" ht="333.5" x14ac:dyDescent="0.35">
       <c r="A31" s="9">
         <v>30</v>
       </c>
@@ -25197,8 +25659,31 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.55000000000000004">
-      <c r="D32" s="10"/>
+    <row r="32" spans="1:22" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="A32" s="9">
+        <v>31</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>571</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>832</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>833</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>834</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>831</v>
+      </c>
+      <c r="U32" s="4" t="s">
+        <v>831</v>
+      </c>
+      <c r="V32" s="10" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -25215,9 +25700,9 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.5234375" defaultRowHeight="50.25" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="15.54296875" defaultRowHeight="50.25" customHeight="1" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:14" s="35" customFormat="1" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:14" s="35" customFormat="1" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="11" t="s">
         <v>567</v>
       </c>
@@ -25261,7 +25746,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:14" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="30" t="s">
         <v>743</v>
       </c>
@@ -25305,7 +25790,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:14" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="30" t="s">
         <v>745</v>
       </c>
@@ -25349,7 +25834,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:14" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="30" t="s">
         <v>747</v>
       </c>
@@ -25407,15 +25892,15 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="7" max="7" width="10.47265625" customWidth="1"/>
-    <col min="8" max="8" width="10.15625" customWidth="1"/>
-    <col min="9" max="9" width="9.734375" customWidth="1"/>
-    <col min="10" max="12" width="9.7890625" customWidth="1"/>
+    <col min="7" max="7" width="10.453125" customWidth="1"/>
+    <col min="8" max="8" width="10.1796875" customWidth="1"/>
+    <col min="9" max="9" width="9.7265625" customWidth="1"/>
+    <col min="10" max="12" width="9.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="12" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:18" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>567</v>
       </c>
@@ -25471,7 +25956,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="187.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:18" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>717</v>
       </c>
@@ -25527,7 +26012,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:18" ht="174" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>731</v>
       </c>
@@ -25583,7 +26068,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="144" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:18" ht="145" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>735</v>
       </c>
@@ -25639,7 +26124,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:18" ht="174" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>772</v>
       </c>
@@ -25695,7 +26180,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:18" ht="174" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>774</v>
       </c>
@@ -25765,16 +26250,16 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.734375" defaultRowHeight="80.25" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="80.25" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="8.734375" style="37"/>
-    <col min="3" max="3" width="20.15625" style="37" customWidth="1"/>
-    <col min="4" max="4" width="23.5234375" style="37" customWidth="1"/>
-    <col min="5" max="5" width="20.15625" style="37" customWidth="1"/>
-    <col min="6" max="16384" width="8.734375" style="37"/>
+    <col min="1" max="2" width="8.7265625" style="37"/>
+    <col min="3" max="3" width="20.1796875" style="37" customWidth="1"/>
+    <col min="4" max="4" width="23.54296875" style="37" customWidth="1"/>
+    <col min="5" max="5" width="20.1796875" style="37" customWidth="1"/>
+    <col min="6" max="16384" width="8.7265625" style="37"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="38" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:18" s="38" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>567</v>
       </c>
@@ -25830,7 +26315,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="120.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:18" ht="120.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="36" t="s">
         <v>701</v>
       </c>
@@ -25886,7 +26371,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="147.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:18" ht="147.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="36" t="s">
         <v>711</v>
       </c>
@@ -25942,7 +26427,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="80.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:18" ht="80.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="36" t="s">
         <v>741</v>
       </c>
@@ -26007,18 +26492,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D18B630D-E2D0-4A83-A583-A6ADEDF36778}">
   <dimension ref="A1:Y3"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView topLeftCell="I1" zoomScale="60" zoomScaleNormal="55" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.5234375" defaultRowHeight="80.25" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="16.54296875" defaultRowHeight="80.25" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.15625" customWidth="1"/>
-    <col min="2" max="2" width="12.47265625" customWidth="1"/>
+    <col min="1" max="1" width="10.1796875" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="12" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:25" s="12" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="11" t="s">
         <v>567</v>
       </c>
@@ -26068,7 +26553,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="115.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:25" ht="115.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="30" t="s">
         <v>713</v>
       </c>
@@ -26127,7 +26612,7 @@
       <c r="X2" s="30"/>
       <c r="Y2" s="30"/>
     </row>
-    <row r="3" spans="1:25" ht="110.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:25" ht="110.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="30" t="s">
         <v>749</v>
       </c>
@@ -26200,18 +26685,18 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.734375" defaultRowHeight="60" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="60" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.734375" style="19"/>
-    <col min="2" max="2" width="11.7890625" style="19" customWidth="1"/>
-    <col min="3" max="3" width="18.5234375" style="19" customWidth="1"/>
-    <col min="4" max="4" width="21.26171875" style="19" customWidth="1"/>
+    <col min="1" max="1" width="8.7265625" style="19"/>
+    <col min="2" max="2" width="11.81640625" style="19" customWidth="1"/>
+    <col min="3" max="3" width="18.54296875" style="19" customWidth="1"/>
+    <col min="4" max="4" width="21.26953125" style="19" customWidth="1"/>
     <col min="5" max="5" width="18" style="19" customWidth="1"/>
-    <col min="6" max="6" width="26.5234375" style="19" customWidth="1"/>
-    <col min="7" max="16384" width="8.734375" style="19"/>
+    <col min="6" max="6" width="26.54296875" style="19" customWidth="1"/>
+    <col min="7" max="16384" width="8.7265625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="17" customFormat="1" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:21" s="17" customFormat="1" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="20" t="s">
         <v>567</v>
       </c>
@@ -26276,7 +26761,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:21" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="31" t="s">
         <v>715</v>
       </c>
@@ -26341,7 +26826,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:21" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="31" t="s">
         <v>733</v>
       </c>
@@ -26406,7 +26891,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:21" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="31" t="s">
         <v>737</v>
       </c>
@@ -26471,7 +26956,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="96.55" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:21" ht="96.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="18" t="s">
         <v>768</v>
       </c>
@@ -26536,7 +27021,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="94.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:21" ht="94.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="18" t="s">
         <v>751</v>
       </c>
@@ -26601,7 +27086,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="60" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:21" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="29"/>
       <c r="C8" s="29"/>
       <c r="D8" s="29"/>
@@ -26611,7 +27096,7 @@
       <c r="H8" s="29"/>
       <c r="I8" s="29"/>
     </row>
-    <row r="9" spans="1:21" ht="60" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:21" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="29"/>
       <c r="C9" s="29"/>
       <c r="D9" s="29"/>
@@ -26621,7 +27106,7 @@
       <c r="H9" s="29"/>
       <c r="I9" s="29"/>
     </row>
-    <row r="10" spans="1:21" ht="60" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:21" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="29"/>
       <c r="C10" s="29"/>
       <c r="D10" s="29"/>
@@ -26631,7 +27116,7 @@
       <c r="H10" s="29"/>
       <c r="I10" s="29"/>
     </row>
-    <row r="11" spans="1:21" ht="60" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:21" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="29"/>
       <c r="C11" s="29"/>
       <c r="D11" s="29"/>
@@ -26641,7 +27126,7 @@
       <c r="H11" s="29"/>
       <c r="I11" s="29"/>
     </row>
-    <row r="12" spans="1:21" ht="60" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:21" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="29"/>
       <c r="C12" s="29"/>
       <c r="D12" s="29"/>
@@ -26651,7 +27136,7 @@
       <c r="H12" s="29"/>
       <c r="I12" s="29"/>
     </row>
-    <row r="13" spans="1:21" ht="60" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:21" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="29"/>
       <c r="C13" s="29"/>
       <c r="D13" s="29"/>
@@ -26661,7 +27146,7 @@
       <c r="H13" s="29"/>
       <c r="I13" s="29"/>
     </row>
-    <row r="14" spans="1:21" ht="60" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:21" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="29"/>
       <c r="C14" s="29"/>
       <c r="D14" s="29"/>
@@ -26671,82 +27156,82 @@
       <c r="H14" s="29"/>
       <c r="I14" s="29"/>
     </row>
-    <row r="15" spans="1:21" ht="60" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:21" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G15" s="29"/>
       <c r="H15" s="29"/>
       <c r="I15" s="29"/>
     </row>
-    <row r="16" spans="1:21" ht="60" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:21" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G16" s="29"/>
       <c r="H16" s="29"/>
       <c r="I16" s="29"/>
     </row>
-    <row r="17" spans="7:9" ht="60" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="7:9" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G17" s="29"/>
       <c r="H17" s="29"/>
       <c r="I17" s="29"/>
     </row>
-    <row r="18" spans="7:9" ht="60" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="7:9" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G18" s="29"/>
       <c r="H18" s="29"/>
       <c r="I18" s="29"/>
     </row>
-    <row r="19" spans="7:9" ht="60" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="7:9" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G19" s="29"/>
       <c r="H19" s="29"/>
       <c r="I19" s="29"/>
     </row>
-    <row r="20" spans="7:9" ht="60" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="7:9" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G20" s="29"/>
       <c r="H20" s="29"/>
       <c r="I20" s="29"/>
     </row>
-    <row r="21" spans="7:9" ht="60" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="7:9" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G21" s="29"/>
       <c r="H21" s="29"/>
       <c r="I21" s="29"/>
     </row>
-    <row r="22" spans="7:9" ht="60" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="7:9" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G22" s="29"/>
       <c r="H22" s="29"/>
       <c r="I22" s="29"/>
     </row>
-    <row r="23" spans="7:9" ht="60" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="7:9" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G23" s="29"/>
       <c r="H23" s="29"/>
       <c r="I23" s="29"/>
     </row>
-    <row r="24" spans="7:9" ht="60" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="7:9" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G24" s="29"/>
       <c r="H24" s="29"/>
       <c r="I24" s="29"/>
     </row>
-    <row r="25" spans="7:9" ht="60" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="7:9" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G25" s="29"/>
       <c r="H25" s="29"/>
       <c r="I25" s="29"/>
     </row>
-    <row r="26" spans="7:9" ht="60" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="7:9" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G26" s="29"/>
       <c r="H26" s="29"/>
       <c r="I26" s="29"/>
     </row>
-    <row r="27" spans="7:9" ht="60" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="7:9" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G27" s="29"/>
       <c r="H27" s="29"/>
       <c r="I27" s="29"/>
     </row>
-    <row r="28" spans="7:9" ht="60" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="7:9" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G28" s="29"/>
       <c r="H28" s="29"/>
       <c r="I28" s="29"/>
     </row>
-    <row r="29" spans="7:9" ht="60" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="7:9" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G29" s="29"/>
       <c r="H29" s="29"/>
       <c r="I29" s="29"/>
     </row>
-    <row r="30" spans="7:9" ht="60" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="7:9" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G30" s="29"/>
       <c r="H30" s="29"/>
       <c r="I30" s="29"/>
@@ -26766,19 +27251,19 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="50.25" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="50.25" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.26171875" style="19" customWidth="1"/>
-    <col min="2" max="2" width="10.5234375" style="19"/>
-    <col min="3" max="3" width="15.47265625" style="19" customWidth="1"/>
+    <col min="1" max="1" width="15.26953125" style="19" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" style="19"/>
+    <col min="3" max="3" width="15.453125" style="19" customWidth="1"/>
     <col min="4" max="4" width="18" style="19" customWidth="1"/>
-    <col min="5" max="5" width="21.734375" style="19" customWidth="1"/>
-    <col min="6" max="12" width="10.5234375" style="19"/>
-    <col min="13" max="13" width="16.15625" style="19" customWidth="1"/>
-    <col min="14" max="16384" width="10.5234375" style="19"/>
+    <col min="5" max="5" width="21.7265625" style="19" customWidth="1"/>
+    <col min="6" max="12" width="10.54296875" style="19"/>
+    <col min="13" max="13" width="16.1796875" style="19" customWidth="1"/>
+    <col min="14" max="16384" width="10.54296875" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="17" customFormat="1" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:23" s="17" customFormat="1" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="11" t="s">
         <v>567</v>
       </c>
@@ -26822,7 +27307,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="30" t="s">
         <v>673</v>
       </c>
@@ -26866,7 +27351,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="30" t="s">
         <v>675</v>
       </c>
@@ -26910,7 +27395,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="30" t="s">
         <v>677</v>
       </c>
@@ -26954,7 +27439,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="30" t="s">
         <v>679</v>
       </c>
@@ -26998,7 +27483,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="30" t="s">
         <v>681</v>
       </c>
@@ -27042,7 +27527,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="30" t="s">
         <v>683</v>
       </c>
@@ -27086,7 +27571,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="30" t="s">
         <v>685</v>
       </c>
@@ -27130,7 +27615,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="9" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="30" t="s">
         <v>687</v>
       </c>
@@ -27174,7 +27659,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="10" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="30" t="s">
         <v>689</v>
       </c>
@@ -27218,7 +27703,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="30" t="s">
         <v>699</v>
       </c>
@@ -27263,7 +27748,7 @@
       </c>
       <c r="W11" s="30"/>
     </row>
-    <row r="12" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="30" t="s">
         <v>707</v>
       </c>
@@ -27308,7 +27793,7 @@
       </c>
       <c r="W12" s="30"/>
     </row>
-    <row r="13" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="13" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="30" t="s">
         <v>721</v>
       </c>
@@ -27352,7 +27837,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="14" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="30" t="s">
         <v>723</v>
       </c>
@@ -27396,7 +27881,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="15" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="30" t="s">
         <v>725</v>
       </c>
@@ -27440,7 +27925,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="16" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="30" t="s">
         <v>727</v>
       </c>
@@ -27484,7 +27969,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="17" spans="1:14" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="30" t="s">
         <v>729</v>
       </c>
@@ -27528,91 +28013,91 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="18" spans="1:14" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="32"/>
       <c r="B18" s="32"/>
       <c r="C18" s="32"/>
       <c r="D18" s="32"/>
       <c r="E18" s="32"/>
     </row>
-    <row r="19" spans="1:14" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="19" spans="1:14" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="32"/>
       <c r="B19" s="32"/>
       <c r="C19" s="32"/>
       <c r="D19" s="32"/>
       <c r="E19" s="32"/>
     </row>
-    <row r="20" spans="1:14" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="20" spans="1:14" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="32"/>
       <c r="B20" s="32"/>
       <c r="C20" s="32"/>
       <c r="D20" s="32"/>
       <c r="E20" s="32"/>
     </row>
-    <row r="21" spans="1:14" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="21" spans="1:14" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="32"/>
       <c r="B21" s="32"/>
       <c r="C21" s="32"/>
       <c r="D21" s="32"/>
       <c r="E21" s="32"/>
     </row>
-    <row r="22" spans="1:14" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="22" spans="1:14" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="32"/>
       <c r="B22" s="32"/>
       <c r="C22" s="32"/>
       <c r="D22" s="32"/>
       <c r="E22" s="32"/>
     </row>
-    <row r="23" spans="1:14" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="23" spans="1:14" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="32"/>
       <c r="B23" s="33"/>
       <c r="C23" s="32"/>
       <c r="D23" s="32"/>
       <c r="E23" s="32"/>
     </row>
-    <row r="24" spans="1:14" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="24" spans="1:14" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="32"/>
       <c r="B24" s="32"/>
       <c r="C24" s="32"/>
       <c r="D24" s="32"/>
       <c r="E24" s="32"/>
     </row>
-    <row r="25" spans="1:14" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="25" spans="1:14" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="32"/>
       <c r="B25" s="32"/>
       <c r="C25" s="32"/>
       <c r="D25" s="32"/>
       <c r="E25" s="32"/>
     </row>
-    <row r="26" spans="1:14" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="26" spans="1:14" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="32"/>
       <c r="B26" s="32"/>
       <c r="C26" s="32"/>
       <c r="D26" s="32"/>
       <c r="E26" s="32"/>
     </row>
-    <row r="27" spans="1:14" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="27" spans="1:14" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="32"/>
       <c r="B27" s="32"/>
       <c r="C27" s="32"/>
       <c r="D27" s="32"/>
       <c r="E27" s="32"/>
     </row>
-    <row r="28" spans="1:14" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="28" spans="1:14" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="32"/>
       <c r="B28" s="32"/>
       <c r="C28" s="32"/>
       <c r="D28" s="32"/>
       <c r="E28" s="32"/>
     </row>
-    <row r="29" spans="1:14" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="29" spans="1:14" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="32"/>
       <c r="B29" s="32"/>
       <c r="C29" s="32"/>
       <c r="D29" s="32"/>
       <c r="E29" s="32"/>
     </row>
-    <row r="30" spans="1:14" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="30" spans="1:14" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="32"/>
       <c r="B30" s="32"/>
       <c r="C30" s="32"/>
@@ -27633,9 +28118,9 @@
       <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:16" s="12" customFormat="1" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:16" s="12" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="11" t="s">
         <v>567</v>
       </c>
@@ -27685,7 +28170,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="49.5" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:16" ht="50.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="45" t="s">
         <v>705</v>
       </c>
@@ -27735,7 +28220,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="111" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:16" ht="113" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="45" t="s">
         <v>764</v>
       </c>
@@ -27765,7 +28250,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="49.5" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:16" ht="50.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="45" t="s">
         <v>739</v>
       </c>
@@ -27815,7 +28300,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="144.30000000000001" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:16" ht="145.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="45" t="s">
         <v>766</v>
       </c>

</xml_diff>

<commit_message>
Updated Test cases for Iteration 2 and 3 functionalities
Updated Test cases for Iteration 2 and 3 functionalities
</commit_message>
<xml_diff>
--- a/testing/testcases.xlsx
+++ b/testing/testcases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lai See Hoe\Documents\GitHub\project-g5t4\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6540EA9D-6F06-4140-A462-BE9AE983A8E8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9910B0E-CBD3-4EA5-B0B3-C2D64E3993D3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="844" firstSheet="16" activeTab="17" xr2:uid="{F747292D-6CBE-43A0-AF24-F2F7C25CEB64}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="844" firstSheet="15" activeTab="16" xr2:uid="{F747292D-6CBE-43A0-AF24-F2F7C25CEB64}"/>
   </bookViews>
   <sheets>
     <sheet name="Test plan" sheetId="22" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3927" uniqueCount="850">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3994" uniqueCount="861">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -12141,9 +12141,6 @@
     <t>Student is logged in and select IS100. Student selects section, enter amount and click on 'submit' button</t>
   </si>
   <si>
-    <t>Clearing round 1 - inactive</t>
-  </si>
-  <si>
     <t xml:space="preserve">round = '1' 
 status = 'inactive' </t>
   </si>
@@ -13072,6 +13069,50 @@
   </si>
   <si>
     <t>Student cannot find course CS002</t>
+  </si>
+  <si>
+    <t>Course dropped successfully</t>
+  </si>
+  <si>
+    <t>User: benny
+course:IS004 
+Section:S3
+amount: 10.01</t>
+  </si>
+  <si>
+    <t>amy.ng.2009, you have $200.00 in your account.
+You did not bid a course in round2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delete bid when round 1 is active </t>
+  </si>
+  <si>
+    <t>Course: IS003
+section: S1
+user: amy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bid drop successfully! You have $50 left. </t>
+  </si>
+  <si>
+    <t>Clearing round 1 after starting round 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">round = '2' 
+status = 'active' </t>
+  </si>
+  <si>
+    <t>Admin press clear round 2</t>
+  </si>
+  <si>
+    <t>Clearing round 1 after clearing round 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">round = '2' 
+status = 'inactive' </t>
+  </si>
+  <si>
+    <t>Admin press clear round 3</t>
   </si>
 </sst>
 </file>
@@ -13765,7 +13806,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="60" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="B1" s="60"/>
       <c r="C1" s="60"/>
@@ -13774,19 +13815,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="57" t="s">
+        <v>805</v>
+      </c>
+      <c r="B2" s="57" t="s">
         <v>806</v>
       </c>
-      <c r="B2" s="57" t="s">
+      <c r="C2" s="57" t="s">
         <v>807</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="D2" s="57" t="s">
         <v>808</v>
       </c>
-      <c r="D2" s="57" t="s">
+      <c r="E2" s="57" t="s">
         <v>809</v>
-      </c>
-      <c r="E2" s="57" t="s">
-        <v>810</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="75" x14ac:dyDescent="0.35">
@@ -13794,16 +13835,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="58" t="s">
+        <v>810</v>
+      </c>
+      <c r="C3" s="59" t="s">
         <v>811</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="D3" s="58" t="s">
         <v>812</v>
       </c>
-      <c r="D3" s="58" t="s">
+      <c r="E3" s="58" t="s">
         <v>813</v>
-      </c>
-      <c r="E3" s="58" t="s">
-        <v>814</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.35">
@@ -13811,16 +13852,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="58" t="s">
+        <v>814</v>
+      </c>
+      <c r="C4" s="58" t="s">
         <v>815</v>
       </c>
-      <c r="C4" s="58" t="s">
+      <c r="D4" s="58" t="s">
         <v>816</v>
       </c>
-      <c r="D4" s="58" t="s">
+      <c r="E4" s="58" t="s">
         <v>817</v>
-      </c>
-      <c r="E4" s="58" t="s">
-        <v>818</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="87.5" x14ac:dyDescent="0.35">
@@ -13828,16 +13869,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="58" t="s">
+        <v>818</v>
+      </c>
+      <c r="C5" s="58" t="s">
+        <v>829</v>
+      </c>
+      <c r="D5" s="58" t="s">
         <v>819</v>
       </c>
-      <c r="C5" s="58" t="s">
-        <v>830</v>
-      </c>
-      <c r="D5" s="58" t="s">
+      <c r="E5" s="58" t="s">
         <v>820</v>
-      </c>
-      <c r="E5" s="58" t="s">
-        <v>821</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="87.5" x14ac:dyDescent="0.35">
@@ -13845,16 +13886,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="58" t="s">
+        <v>821</v>
+      </c>
+      <c r="C6" s="58" t="s">
         <v>822</v>
       </c>
-      <c r="C6" s="58" t="s">
+      <c r="D6" s="58" t="s">
         <v>823</v>
       </c>
-      <c r="D6" s="58" t="s">
+      <c r="E6" s="58" t="s">
         <v>824</v>
-      </c>
-      <c r="E6" s="58" t="s">
-        <v>825</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="25" x14ac:dyDescent="0.35">
@@ -13862,16 +13903,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="58" t="s">
+        <v>825</v>
+      </c>
+      <c r="C7" s="58" t="s">
         <v>826</v>
       </c>
-      <c r="C7" s="58" t="s">
+      <c r="D7" s="58" t="s">
         <v>827</v>
       </c>
-      <c r="D7" s="58" t="s">
+      <c r="E7" s="58" t="s">
         <v>828</v>
-      </c>
-      <c r="E7" s="58" t="s">
-        <v>829</v>
       </c>
     </row>
   </sheetData>
@@ -13905,7 +13946,7 @@
         <v>569</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>3</v>
@@ -13949,13 +13990,13 @@
     </row>
     <row r="2" spans="1:16" ht="76.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="25" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B2" s="30" t="s">
         <v>204</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="D2" s="30" t="s">
         <v>366</v>
@@ -13999,13 +14040,13 @@
     </row>
     <row r="3" spans="1:16" ht="76.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="25" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B3" s="30" t="s">
         <v>218</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="D3" s="30" t="s">
         <v>374</v>
@@ -14049,13 +14090,13 @@
     </row>
     <row r="4" spans="1:16" ht="76.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="30" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="B4" s="30" t="s">
         <v>539</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="D4" s="30" t="s">
         <v>374</v>
@@ -14110,39 +14151,39 @@
         <v>569</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="11" t="s">
+        <v>751</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>752</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>753</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>754</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="I1" s="49" t="s">
         <v>755</v>
       </c>
-      <c r="I1" s="49" t="s">
+      <c r="J1" s="49" t="s">
+        <v>757</v>
+      </c>
+      <c r="K1" s="49" t="s">
         <v>756</v>
       </c>
-      <c r="J1" s="49" t="s">
+      <c r="L1" s="49" t="s">
         <v>758</v>
-      </c>
-      <c r="K1" s="49" t="s">
-        <v>757</v>
-      </c>
-      <c r="L1" s="49" t="s">
-        <v>759</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A2" s="25" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B2" s="29" t="s">
         <v>159</v>
@@ -14180,7 +14221,7 @@
     </row>
     <row r="3" spans="1:12" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A3" s="25" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B3" s="29" t="s">
         <v>161</v>
@@ -14218,7 +14259,7 @@
     </row>
     <row r="4" spans="1:12" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A4" s="25" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="B4" s="29" t="s">
         <v>163</v>
@@ -14256,7 +14297,7 @@
     </row>
     <row r="5" spans="1:12" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A5" s="25" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B5" s="29" t="s">
         <v>165</v>
@@ -14294,7 +14335,7 @@
     </row>
     <row r="6" spans="1:12" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A6" s="25" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B6" s="29" t="s">
         <v>167</v>
@@ -14332,13 +14373,13 @@
     </row>
     <row r="7" spans="1:12" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A7" s="25" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B7" s="29" t="s">
         <v>169</v>
       </c>
       <c r="C7" s="50" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="D7" s="42" t="s">
         <v>354</v>
@@ -14370,7 +14411,7 @@
     </row>
     <row r="8" spans="1:12" ht="387.5" x14ac:dyDescent="0.35">
       <c r="A8" s="25" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B8" s="29" t="s">
         <v>170</v>
@@ -14437,51 +14478,51 @@
         <v>569</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="11" t="s">
+        <v>751</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>752</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>753</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>754</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="I1" s="49" t="s">
         <v>755</v>
       </c>
-      <c r="I1" s="49" t="s">
-        <v>756</v>
-      </c>
       <c r="J1" s="49" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="K1" s="49" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="L1" s="49" t="s">
         <v>556</v>
       </c>
       <c r="M1" s="49" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="N1" s="49" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="338.5" x14ac:dyDescent="0.35">
       <c r="A2" s="25" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>108</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>151</v>
@@ -14519,13 +14560,13 @@
     </row>
     <row r="3" spans="1:14" ht="138.5" x14ac:dyDescent="0.35">
       <c r="A3" s="25" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>103</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>152</v>
@@ -14563,13 +14604,13 @@
     </row>
     <row r="4" spans="1:14" ht="138.5" x14ac:dyDescent="0.35">
       <c r="A4" s="25" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>104</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>485</v>
@@ -14607,13 +14648,13 @@
     </row>
     <row r="5" spans="1:14" ht="138.5" x14ac:dyDescent="0.35">
       <c r="A5" s="25" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>105</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>484</v>
@@ -14651,13 +14692,13 @@
     </row>
     <row r="6" spans="1:14" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A6" s="25" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>106</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>486</v>
@@ -14695,13 +14736,13 @@
     </row>
     <row r="7" spans="1:14" ht="138.5" x14ac:dyDescent="0.35">
       <c r="A7" s="25" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>156</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>152</v>
@@ -14739,13 +14780,13 @@
     </row>
     <row r="8" spans="1:14" ht="138.5" x14ac:dyDescent="0.35">
       <c r="A8" s="25" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>109</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>152</v>
@@ -14783,13 +14824,13 @@
     </row>
     <row r="9" spans="1:14" ht="338.5" x14ac:dyDescent="0.35">
       <c r="A9" s="25" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>157</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>348</v>
@@ -14860,7 +14901,7 @@
         <v>569</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>3</v>
@@ -14884,7 +14925,7 @@
         <v>467</v>
       </c>
       <c r="K1" s="11" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="L1" s="11" t="s">
         <v>482</v>
@@ -14892,13 +14933,13 @@
     </row>
     <row r="2" spans="1:12" ht="338.5" x14ac:dyDescent="0.35">
       <c r="A2" s="25" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B2" s="25" t="s">
         <v>108</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="D2" s="25" t="s">
         <v>151</v>
@@ -14934,13 +14975,13 @@
     </row>
     <row r="3" spans="1:12" ht="138.5" x14ac:dyDescent="0.35">
       <c r="A3" s="25" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B3" s="25" t="s">
         <v>103</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="D3" s="25" t="s">
         <v>152</v>
@@ -14972,13 +15013,13 @@
     </row>
     <row r="4" spans="1:12" ht="138.5" x14ac:dyDescent="0.35">
       <c r="A4" s="25" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B4" s="25" t="s">
         <v>104</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="D4" s="25" t="s">
         <v>153</v>
@@ -15010,13 +15051,13 @@
     </row>
     <row r="5" spans="1:12" ht="138.5" x14ac:dyDescent="0.35">
       <c r="A5" s="25" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B5" s="25" t="s">
         <v>105</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="D5" s="25" t="s">
         <v>154</v>
@@ -15048,13 +15089,13 @@
     </row>
     <row r="6" spans="1:12" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A6" s="25" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B6" s="25" t="s">
         <v>106</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="D6" s="25" t="s">
         <v>155</v>
@@ -15086,13 +15127,13 @@
     </row>
     <row r="7" spans="1:12" ht="138.5" x14ac:dyDescent="0.35">
       <c r="A7" s="25" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B7" s="25" t="s">
         <v>156</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="D7" s="25" t="s">
         <v>152</v>
@@ -15124,13 +15165,13 @@
     </row>
     <row r="8" spans="1:12" ht="138.5" x14ac:dyDescent="0.35">
       <c r="A8" s="25" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B8" s="25" t="s">
         <v>109</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="D8" s="25" t="s">
         <v>152</v>
@@ -15162,13 +15203,13 @@
     </row>
     <row r="9" spans="1:12" ht="338.5" x14ac:dyDescent="0.35">
       <c r="A9" s="25" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B9" s="25" t="s">
         <v>157</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="D9" s="25" t="s">
         <v>348</v>
@@ -15192,7 +15233,7 @@
     </row>
     <row r="10" spans="1:12" ht="409.6" x14ac:dyDescent="0.35">
       <c r="A10" s="25" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B10" s="25" t="s">
         <v>159</v>
@@ -15230,7 +15271,7 @@
     </row>
     <row r="11" spans="1:12" ht="409.6" x14ac:dyDescent="0.35">
       <c r="A11" s="25" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B11" s="25" t="s">
         <v>161</v>
@@ -15268,7 +15309,7 @@
     </row>
     <row r="12" spans="1:12" ht="409.6" x14ac:dyDescent="0.35">
       <c r="A12" s="25" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="B12" s="25" t="s">
         <v>163</v>
@@ -15306,7 +15347,7 @@
     </row>
     <row r="13" spans="1:12" ht="409.6" x14ac:dyDescent="0.35">
       <c r="A13" s="25" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B13" s="25" t="s">
         <v>165</v>
@@ -15344,7 +15385,7 @@
     </row>
     <row r="14" spans="1:12" ht="409.6" x14ac:dyDescent="0.35">
       <c r="A14" s="25" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B14" s="25" t="s">
         <v>167</v>
@@ -15382,13 +15423,13 @@
     </row>
     <row r="15" spans="1:12" ht="409.6" x14ac:dyDescent="0.35">
       <c r="A15" s="25" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B15" s="25" t="s">
         <v>169</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="D15" s="25" t="s">
         <v>354</v>
@@ -15420,7 +15461,7 @@
     </row>
     <row r="16" spans="1:12" ht="409.6" x14ac:dyDescent="0.35">
       <c r="A16" s="25" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B16" s="25" t="s">
         <v>170</v>
@@ -15458,13 +15499,13 @@
     </row>
     <row r="17" spans="1:12" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A17" s="25" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B17" s="25" t="s">
         <v>173</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="D17" s="25" t="s">
         <v>174</v>
@@ -15496,13 +15537,13 @@
     </row>
     <row r="18" spans="1:12" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A18" s="25" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B18" s="25" t="s">
         <v>176</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="D18" s="25" t="s">
         <v>177</v>
@@ -15534,13 +15575,13 @@
     </row>
     <row r="19" spans="1:12" ht="126" x14ac:dyDescent="0.35">
       <c r="A19" s="25" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B19" s="25" t="s">
         <v>179</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="D19" s="25" t="s">
         <v>180</v>
@@ -15572,13 +15613,13 @@
     </row>
     <row r="20" spans="1:12" ht="126" x14ac:dyDescent="0.35">
       <c r="A20" s="25" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B20" s="25" t="s">
         <v>126</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="D20" s="25" t="s">
         <v>357</v>
@@ -15610,13 +15651,13 @@
     </row>
     <row r="21" spans="1:12" ht="126" x14ac:dyDescent="0.35">
       <c r="A21" s="25" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B21" s="25" t="s">
         <v>183</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="D21" s="25" t="s">
         <v>358</v>
@@ -15648,13 +15689,13 @@
     </row>
     <row r="22" spans="1:12" ht="138.5" x14ac:dyDescent="0.35">
       <c r="A22" s="25" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B22" s="25" t="s">
         <v>185</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="D22" s="25" t="s">
         <v>186</v>
@@ -15686,13 +15727,13 @@
     </row>
     <row r="23" spans="1:12" ht="126" x14ac:dyDescent="0.35">
       <c r="A23" s="25" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B23" s="25" t="s">
         <v>123</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="D23" s="25" t="s">
         <v>188</v>
@@ -15756,13 +15797,13 @@
     </row>
     <row r="26" spans="1:12" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A26" s="25" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B26" s="25" t="s">
         <v>192</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="D26" s="25" t="s">
         <v>359</v>
@@ -15794,13 +15835,13 @@
     </row>
     <row r="27" spans="1:12" ht="126" x14ac:dyDescent="0.35">
       <c r="A27" s="25" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B27" s="25" t="s">
         <v>194</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="D27" s="25" t="s">
         <v>360</v>
@@ -15848,13 +15889,13 @@
     </row>
     <row r="29" spans="1:12" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A29" s="25" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B29" s="25" t="s">
         <v>196</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="D29" s="25"/>
       <c r="E29" s="25" t="s">
@@ -15884,13 +15925,13 @@
     </row>
     <row r="30" spans="1:12" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A30" s="25" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="B30" s="25" t="s">
         <v>197</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="D30" s="25" t="s">
         <v>362</v>
@@ -15922,13 +15963,13 @@
     </row>
     <row r="31" spans="1:12" ht="128.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="25" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B31" s="25" t="s">
         <v>198</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D31" s="25" t="s">
         <v>363</v>
@@ -15960,13 +16001,13 @@
     </row>
     <row r="32" spans="1:12" ht="51" x14ac:dyDescent="0.35">
       <c r="A32" s="25" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="B32" s="25" t="s">
         <v>199</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="D32" s="25" t="s">
         <v>364</v>
@@ -15998,13 +16039,13 @@
     </row>
     <row r="33" spans="1:12" ht="51" x14ac:dyDescent="0.35">
       <c r="A33" s="25" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="B33" s="25" t="s">
         <v>201</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="D33" s="25" t="s">
         <v>364</v>
@@ -16036,13 +16077,13 @@
     </row>
     <row r="34" spans="1:12" ht="409.6" x14ac:dyDescent="0.35">
       <c r="A34" s="25" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B34" s="25" t="s">
         <v>203</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="D34" s="25" t="s">
         <v>365</v>
@@ -16074,13 +16115,13 @@
     </row>
     <row r="35" spans="1:12" ht="76" x14ac:dyDescent="0.35">
       <c r="A35" s="25" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B35" s="25" t="s">
         <v>204</v>
       </c>
       <c r="C35" s="25" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="D35" s="25" t="s">
         <v>366</v>
@@ -16112,13 +16153,13 @@
     </row>
     <row r="36" spans="1:12" ht="51" x14ac:dyDescent="0.35">
       <c r="A36" s="25" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="B36" s="25" t="s">
         <v>205</v>
       </c>
       <c r="C36" s="25" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="D36" s="25" t="s">
         <v>364</v>
@@ -16150,13 +16191,13 @@
     </row>
     <row r="37" spans="1:12" ht="138.5" x14ac:dyDescent="0.35">
       <c r="A37" s="25" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B37" s="25" t="s">
         <v>207</v>
       </c>
       <c r="C37" s="25" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D37" s="25" t="s">
         <v>367</v>
@@ -16188,13 +16229,13 @@
     </row>
     <row r="38" spans="1:12" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A38" s="25" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="B38" s="25" t="s">
         <v>207</v>
       </c>
       <c r="C38" s="25" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="D38" s="25" t="s">
         <v>368</v>
@@ -16242,13 +16283,13 @@
     </row>
     <row r="40" spans="1:12" ht="409.6" x14ac:dyDescent="0.35">
       <c r="A40" s="25" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="B40" s="25" t="s">
         <v>203</v>
       </c>
       <c r="C40" s="25" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D40" s="25"/>
       <c r="E40" s="25" t="s">
@@ -16278,13 +16319,13 @@
     </row>
     <row r="41" spans="1:12" ht="238.5" x14ac:dyDescent="0.35">
       <c r="A41" s="25" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="B41" s="25" t="s">
         <v>210</v>
       </c>
       <c r="C41" s="25" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="D41" s="25" t="s">
         <v>370</v>
@@ -16316,13 +16357,13 @@
     </row>
     <row r="42" spans="1:12" ht="409.6" x14ac:dyDescent="0.35">
       <c r="A42" s="25" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="B42" s="25" t="s">
         <v>212</v>
       </c>
       <c r="C42" s="25" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="D42" s="25" t="s">
         <v>372</v>
@@ -16354,13 +16395,13 @@
     </row>
     <row r="43" spans="1:12" ht="126" x14ac:dyDescent="0.35">
       <c r="A43" s="25" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="B43" s="25" t="s">
         <v>213</v>
       </c>
       <c r="C43" s="25" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="D43" s="25" t="s">
         <v>373</v>
@@ -16456,13 +16497,13 @@
     </row>
     <row r="48" spans="1:12" ht="76" x14ac:dyDescent="0.35">
       <c r="A48" s="25" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B48" s="25" t="s">
         <v>218</v>
       </c>
       <c r="C48" s="25" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="D48" s="25" t="s">
         <v>374</v>
@@ -16494,13 +16535,13 @@
     </row>
     <row r="49" spans="1:12" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A49" s="25" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="B49" s="25" t="s">
         <v>220</v>
       </c>
       <c r="C49" s="25" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="D49" s="25" t="s">
         <v>375</v>
@@ -16532,13 +16573,13 @@
     </row>
     <row r="50" spans="1:12" ht="138.5" x14ac:dyDescent="0.35">
       <c r="A50" s="25" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="B50" s="25" t="s">
         <v>222</v>
       </c>
       <c r="C50" s="25" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="D50" s="25" t="s">
         <v>376</v>
@@ -16570,13 +16611,13 @@
     </row>
     <row r="51" spans="1:12" ht="51" x14ac:dyDescent="0.35">
       <c r="A51" s="25" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B51" s="25" t="s">
         <v>224</v>
       </c>
       <c r="C51" s="25" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="D51" s="25" t="s">
         <v>364</v>
@@ -16608,13 +16649,13 @@
     </row>
     <row r="52" spans="1:12" ht="51" x14ac:dyDescent="0.35">
       <c r="A52" s="25" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B52" s="25" t="s">
         <v>226</v>
       </c>
       <c r="C52" s="25" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="D52" s="25" t="s">
         <v>364</v>
@@ -16646,13 +16687,13 @@
     </row>
     <row r="53" spans="1:12" ht="51" x14ac:dyDescent="0.35">
       <c r="A53" s="25" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B53" s="25" t="s">
         <v>228</v>
       </c>
       <c r="C53" s="25" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="D53" s="25" t="s">
         <v>364</v>
@@ -16684,13 +16725,13 @@
     </row>
     <row r="54" spans="1:12" ht="126" x14ac:dyDescent="0.35">
       <c r="A54" s="25" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B54" s="25" t="s">
         <v>229</v>
       </c>
       <c r="C54" s="25" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="D54" s="25" t="s">
         <v>373</v>
@@ -16722,13 +16763,13 @@
     </row>
     <row r="55" spans="1:12" ht="409.6" x14ac:dyDescent="0.35">
       <c r="A55" s="25" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B55" s="25" t="s">
         <v>231</v>
       </c>
       <c r="C55" s="25" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="D55" s="25" t="s">
         <v>372</v>
@@ -16760,13 +16801,13 @@
     </row>
     <row r="56" spans="1:12" ht="126" x14ac:dyDescent="0.35">
       <c r="A56" s="25" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B56" s="25" t="s">
         <v>232</v>
       </c>
       <c r="C56" s="25" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="D56" s="25" t="s">
         <v>373</v>
@@ -16830,13 +16871,13 @@
     </row>
     <row r="59" spans="1:12" ht="409.6" x14ac:dyDescent="0.35">
       <c r="A59" s="25" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B59" s="25" t="s">
         <v>236</v>
       </c>
       <c r="C59" s="25" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="D59" s="25" t="s">
         <v>372</v>
@@ -16932,13 +16973,13 @@
     </row>
     <row r="64" spans="1:12" ht="51" x14ac:dyDescent="0.35">
       <c r="A64" s="25" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B64" s="25" t="s">
         <v>241</v>
       </c>
       <c r="C64" s="25" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="D64" s="25" t="s">
         <v>364</v>
@@ -16970,11 +17011,11 @@
     </row>
     <row r="65" spans="1:12" ht="409.6" x14ac:dyDescent="0.35">
       <c r="A65" s="25" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B65" s="25"/>
       <c r="C65" s="25" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="D65" s="25" t="s">
         <v>377</v>
@@ -17006,13 +17047,13 @@
     </row>
     <row r="66" spans="1:12" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A66" s="25" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="B66" s="25" t="s">
         <v>244</v>
       </c>
       <c r="C66" s="25" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="D66" s="25" t="s">
         <v>378</v>
@@ -17044,13 +17085,13 @@
     </row>
     <row r="67" spans="1:12" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A67" s="25" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="B67" s="25" t="s">
         <v>246</v>
       </c>
       <c r="C67" s="25" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D67" s="25" t="s">
         <v>362</v>
@@ -17082,13 +17123,13 @@
     </row>
     <row r="68" spans="1:12" ht="409.6" x14ac:dyDescent="0.35">
       <c r="A68" s="25" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="B68" s="25" t="s">
         <v>248</v>
       </c>
       <c r="C68" s="25" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="D68" s="25" t="s">
         <v>379</v>
@@ -17120,13 +17161,13 @@
     </row>
     <row r="69" spans="1:12" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A69" s="25" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="B69" s="25" t="s">
         <v>250</v>
       </c>
       <c r="C69" s="25" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="D69" s="25" t="s">
         <v>361</v>
@@ -17158,13 +17199,13 @@
     </row>
     <row r="70" spans="1:12" ht="409.6" x14ac:dyDescent="0.35">
       <c r="A70" s="25" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="B70" s="25" t="s">
         <v>252</v>
       </c>
       <c r="C70" s="25" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="D70" s="25" t="s">
         <v>362</v>
@@ -18458,11 +18499,11 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A3F21E7-F613-4F5C-A232-03BE67008ACA}">
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="C1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O2" sqref="O2:R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18476,7 +18517,7 @@
     <col min="12" max="12" width="12.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="14" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" s="14" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>567</v>
       </c>
@@ -18487,7 +18528,7 @@
         <v>569</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="E1" s="11" t="s">
         <v>573</v>
@@ -18514,19 +18555,25 @@
         <v>467</v>
       </c>
       <c r="M1" s="22" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="N1" s="11" t="s">
         <v>479</v>
       </c>
       <c r="O1" s="49" t="s">
+        <v>638</v>
+      </c>
+      <c r="P1" s="49" t="s">
         <v>639</v>
       </c>
-      <c r="P1" s="49" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" s="4" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="Q1" s="22" t="s">
+        <v>801</v>
+      </c>
+      <c r="R1" s="11" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" s="4" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -18540,7 +18587,7 @@
         <v>393</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>401</v>
@@ -18575,8 +18622,14 @@
       <c r="P2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" s="4" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="Q2" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" s="4" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -18625,8 +18678,14 @@
       <c r="P3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" s="4" customFormat="1" ht="145" x14ac:dyDescent="0.35">
+      <c r="Q3" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" s="4" customFormat="1" ht="145" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -18675,8 +18734,14 @@
       <c r="P4" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" s="4" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="Q4" s="1" t="s">
+        <v>851</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" s="4" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -18725,8 +18790,14 @@
       <c r="P5" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" s="4" customFormat="1" ht="87" x14ac:dyDescent="0.35">
+      <c r="Q5" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" s="4" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -18775,8 +18846,14 @@
       <c r="P6" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="Q6" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -18825,8 +18902,14 @@
       <c r="P7" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" s="4" customFormat="1" ht="87" x14ac:dyDescent="0.35">
+      <c r="Q7" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" s="4" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -18875,18 +18958,42 @@
       <c r="P8" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="Q8" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>385</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>386</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>850</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>641</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>849</v>
+      </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="Q9" s="18" t="s">
+        <v>849</v>
+      </c>
+      <c r="R9" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -18896,7 +19003,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -18906,9 +19013,9 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -18917,11 +19024,11 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B5F0622-0CBD-4B06-835F-E38104983047}">
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:R15"/>
   <sheetViews>
     <sheetView zoomScale="77" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18940,7 +19047,7 @@
     <col min="17" max="16384" width="8.7265625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="21" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" s="21" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>567</v>
       </c>
@@ -18984,13 +19091,19 @@
         <v>479</v>
       </c>
       <c r="O1" s="22" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="P1" s="11" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" s="18" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q1" s="22" t="s">
+        <v>801</v>
+      </c>
+      <c r="R1" s="11" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" s="18" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18">
         <v>1</v>
       </c>
@@ -19004,7 +19117,7 @@
         <v>384</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="F2" s="18" t="s">
         <v>388</v>
@@ -19039,8 +19152,14 @@
       <c r="P2" s="18" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" s="18" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="Q2" s="18" t="s">
+        <v>388</v>
+      </c>
+      <c r="R2" s="18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" s="18" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="18">
         <v>2</v>
       </c>
@@ -19054,7 +19173,7 @@
         <v>384</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="F3" s="18" t="s">
         <v>411</v>
@@ -19089,8 +19208,14 @@
       <c r="P3" s="18" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" s="18" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="Q3" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="R3" s="18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" s="18" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A4" s="18">
         <v>3</v>
       </c>
@@ -19104,7 +19229,7 @@
         <v>387</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="F4" s="18" t="s">
         <v>389</v>
@@ -19139,8 +19264,14 @@
       <c r="P4" s="18" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" s="40" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="Q4" s="18" t="s">
+        <v>389</v>
+      </c>
+      <c r="R4" s="18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" s="40" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="40">
         <v>4</v>
       </c>
@@ -19154,7 +19285,7 @@
         <v>387</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="F5" s="40" t="s">
         <v>411</v>
@@ -19189,17 +19320,48 @@
       <c r="P5" s="40" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35"/>
+      <c r="Q5" s="40" t="s">
+        <v>411</v>
+      </c>
+      <c r="R5" s="40" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" s="18" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="18">
+        <v>5</v>
+      </c>
+      <c r="B6" s="40" t="s">
+        <v>385</v>
+      </c>
+      <c r="C6" s="40" t="s">
+        <v>852</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>853</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>641</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>854</v>
+      </c>
+      <c r="Q6" s="18" t="s">
+        <v>854</v>
+      </c>
+      <c r="R6" s="18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="9" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -19209,8 +19371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{038D9871-6BF2-4210-AB19-5595569BDB87}">
   <dimension ref="A1:R16"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
@@ -19271,16 +19433,16 @@
         <v>476</v>
       </c>
       <c r="O1" s="48" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="P1" s="48" t="s">
         <v>559</v>
       </c>
       <c r="Q1" s="22" t="s">
+        <v>801</v>
+      </c>
+      <c r="R1" s="11" t="s">
         <v>802</v>
-      </c>
-      <c r="R1" s="11" t="s">
-        <v>803</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="130.5" x14ac:dyDescent="0.35">
@@ -19501,7 +19663,7 @@
         <v>4</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="R5" s="1" t="s">
         <v>4</v>
@@ -19692,40 +19854,40 @@
         <v>392</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>4</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="J9" s="7" t="s">
         <v>4</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="L9" s="7" t="s">
         <v>4</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="N9" s="7" t="s">
         <v>4</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="P9" s="7" t="s">
         <v>4</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="R9" s="7" t="s">
         <v>4</v>
@@ -19860,40 +20022,40 @@
         <v>392</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>4</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="N12" s="1" t="s">
         <v>4</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="P12" s="1" t="s">
         <v>4</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="R12" s="1" t="s">
         <v>4</v>
@@ -19972,40 +20134,40 @@
         <v>392</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>4</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="N14" s="1" t="s">
         <v>4</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="P14" s="1" t="s">
         <v>4</v>
       </c>
       <c r="Q14" s="4" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="R14" s="1" t="s">
         <v>4</v>
@@ -20028,40 +20190,40 @@
         <v>392</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>4</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="N15" s="1" t="s">
         <v>4</v>
       </c>
       <c r="O15" s="4" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="P15" s="1" t="s">
         <v>4</v>
       </c>
       <c r="Q15" s="4" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="R15" s="1" t="s">
         <v>4</v>
@@ -20081,13 +20243,13 @@
         <v>419</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="Q16" s="4" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="R16" t="s">
         <v>4</v>
@@ -20101,11 +20263,11 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2471C963-B84B-411E-BDA6-79ECD81BD5B2}">
-  <dimension ref="A1:X7"/>
+  <dimension ref="A1:Z9"/>
   <sheetViews>
-    <sheetView zoomScale="72" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S3" sqref="S3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="72" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Y9" sqref="Y9:Z9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20120,7 +20282,7 @@
     <col min="18" max="18" width="12.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="12" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" s="12" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>567</v>
       </c>
@@ -20152,49 +20314,55 @@
         <v>458</v>
       </c>
       <c r="K1" s="11" t="s">
+        <v>631</v>
+      </c>
+      <c r="L1" s="11" t="s">
         <v>632</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="M1" s="11" t="s">
         <v>633</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="N1" s="11" t="s">
         <v>634</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="O1" s="11" t="s">
         <v>635</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="P1" s="11" t="s">
+        <v>628</v>
+      </c>
+      <c r="Q1" s="11" t="s">
         <v>636</v>
-      </c>
-      <c r="P1" s="11" t="s">
-        <v>629</v>
-      </c>
-      <c r="Q1" s="11" t="s">
-        <v>637</v>
       </c>
       <c r="R1" s="11" t="s">
         <v>467</v>
       </c>
       <c r="S1" s="22" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="T1" s="11" t="s">
         <v>474</v>
       </c>
       <c r="U1" s="27" t="s">
+        <v>638</v>
+      </c>
+      <c r="V1" s="11" t="s">
         <v>639</v>
       </c>
-      <c r="V1" s="11" t="s">
-        <v>640</v>
-      </c>
       <c r="W1" s="11" t="s">
+        <v>629</v>
+      </c>
+      <c r="X1" s="11" t="s">
         <v>630</v>
       </c>
-      <c r="X1" s="11" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" ht="116" x14ac:dyDescent="0.35">
+      <c r="Y1" s="22" t="s">
+        <v>801</v>
+      </c>
+      <c r="Z1" s="11" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" ht="116" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -20267,8 +20435,14 @@
       <c r="X2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:24" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="Y2" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -20341,8 +20515,14 @@
       <c r="X3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:24" ht="145" x14ac:dyDescent="0.35">
+      <c r="Y3" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="145" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -20415,8 +20595,14 @@
       <c r="X4" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:24" ht="348" x14ac:dyDescent="0.35">
+      <c r="Y4" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="348" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -20489,8 +20675,14 @@
       <c r="X5" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:24" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="Y5" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -20563,22 +20755,25 @@
       <c r="X6" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:24" ht="87" x14ac:dyDescent="0.35">
+      <c r="Y6" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="87" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>620</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>627</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>628</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>468</v>
@@ -20635,6 +20830,64 @@
         <v>468</v>
       </c>
       <c r="X7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="87" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>856</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>857</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="87" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>858</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>860</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="Z9" t="s">
         <v>4</v>
       </c>
     </row>
@@ -20645,11 +20898,11 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D48F8994-0480-456C-9C73-8DEBC1CF05E8}">
-  <dimension ref="A1:AB26"/>
+  <dimension ref="A1:AB27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="74" zoomScaleNormal="78" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z26" sqref="Y26:Z26"/>
+    <sheetView topLeftCell="G1" zoomScale="74" zoomScaleNormal="78" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AA1" sqref="AA1:AB1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20742,10 +20995,10 @@
         <v>483</v>
       </c>
       <c r="AA1" s="22" t="s">
+        <v>801</v>
+      </c>
+      <c r="AB1" s="11" t="s">
         <v>802</v>
-      </c>
-      <c r="AB1" s="11" t="s">
-        <v>803</v>
       </c>
     </row>
     <row r="2" spans="1:28" ht="101.5" x14ac:dyDescent="0.35">
@@ -21000,7 +21253,7 @@
         <v>4</v>
       </c>
       <c r="AA4" s="1" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="AB4" s="1" t="s">
         <v>4</v>
@@ -22804,24 +23057,29 @@
         <v>589</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>837</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>838</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>839</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>840</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>841</v>
       </c>
       <c r="Y26" s="1"/>
       <c r="Z26" s="1"/>
       <c r="AA26" s="1" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="AB26" s="1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A27" s="1">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -22909,10 +23167,10 @@
         <v>483</v>
       </c>
       <c r="S1" s="22" t="s">
+        <v>801</v>
+      </c>
+      <c r="T1" s="11" t="s">
         <v>802</v>
-      </c>
-      <c r="T1" s="11" t="s">
-        <v>803</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="87" x14ac:dyDescent="0.35">
@@ -23419,13 +23677,13 @@
         <v>581</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>834</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>835</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>836</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>837</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>32</v>
@@ -23465,19 +23723,19 @@
         <v>569</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="F1" s="20" t="s">
         <v>481</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="H1" s="11" t="s">
         <v>543</v>
@@ -23485,25 +23743,25 @@
     </row>
     <row r="2" spans="1:8" ht="50.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
+        <v>779</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>784</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>792</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>780</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>785</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>793</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>781</v>
-      </c>
       <c r="E2" s="4" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>4</v>
@@ -23511,25 +23769,25 @@
     </row>
     <row r="3" spans="1:8" ht="63.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>4</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>4</v>
@@ -23537,25 +23795,25 @@
     </row>
     <row r="4" spans="1:8" ht="50.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>4</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>4</v>
@@ -23563,25 +23821,25 @@
     </row>
     <row r="5" spans="1:8" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="F5" s="44" t="s">
         <v>4</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>4</v>
@@ -23677,16 +23935,16 @@
         <v>483</v>
       </c>
       <c r="S1" s="22" t="s">
+        <v>801</v>
+      </c>
+      <c r="T1" s="11" t="s">
         <v>802</v>
       </c>
-      <c r="T1" s="11" t="s">
-        <v>803</v>
-      </c>
       <c r="U1" s="22" t="s">
+        <v>801</v>
+      </c>
+      <c r="V1" s="11" t="s">
         <v>802</v>
-      </c>
-      <c r="V1" s="11" t="s">
-        <v>803</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="145" x14ac:dyDescent="0.35">
@@ -25635,25 +25893,25 @@
         <v>571</v>
       </c>
       <c r="C31" s="9" t="s">
+        <v>797</v>
+      </c>
+      <c r="D31" s="10" t="s">
         <v>798</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="E31" s="10" t="s">
         <v>799</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="F31" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="S31" s="1" t="s">
         <v>800</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>804</v>
-      </c>
-      <c r="S31" s="1" t="s">
-        <v>801</v>
       </c>
       <c r="T31" s="10" t="s">
         <v>140</v>
       </c>
       <c r="U31" s="1" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="V31" s="10" t="s">
         <v>4</v>
@@ -25667,19 +25925,19 @@
         <v>571</v>
       </c>
       <c r="C32" s="9" t="s">
+        <v>831</v>
+      </c>
+      <c r="D32" s="10" t="s">
         <v>832</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="E32" s="10" t="s">
         <v>833</v>
       </c>
-      <c r="E32" s="10" t="s">
-        <v>834</v>
-      </c>
       <c r="F32" s="4" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="U32" s="4" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="V32" s="10" t="s">
         <v>4</v>
@@ -25710,7 +25968,7 @@
         <v>569</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>3</v>
@@ -25734,10 +25992,10 @@
         <v>473</v>
       </c>
       <c r="K1" s="20" t="s">
+        <v>777</v>
+      </c>
+      <c r="L1" s="20" t="s">
         <v>778</v>
-      </c>
-      <c r="L1" s="20" t="s">
-        <v>779</v>
       </c>
       <c r="M1" s="22" t="s">
         <v>550</v>
@@ -25748,13 +26006,13 @@
     </row>
     <row r="2" spans="1:14" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="30" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="B2" s="30" t="s">
         <v>243</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="D2" s="30" t="s">
         <v>378</v>
@@ -25792,13 +26050,13 @@
     </row>
     <row r="3" spans="1:14" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="30" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="B3" s="30" t="s">
         <v>245</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D3" s="30" t="s">
         <v>362</v>
@@ -25836,13 +26094,13 @@
     </row>
     <row r="4" spans="1:14" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="30" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="B4" s="30" t="s">
         <v>247</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="D4" s="30" t="s">
         <v>379</v>
@@ -25914,13 +26172,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="11" t="s">
+        <v>774</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>775</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="20" t="s">
         <v>776</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>777</v>
       </c>
       <c r="H1" s="20" t="s">
         <v>501</v>
@@ -25932,13 +26190,13 @@
         <v>473</v>
       </c>
       <c r="K1" s="20" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="L1" s="20" t="s">
         <v>512</v>
       </c>
       <c r="M1" s="20" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="N1" s="20" t="s">
         <v>480</v>
@@ -25958,13 +26216,13 @@
     </row>
     <row r="2" spans="1:18" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>507</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>500</v>
@@ -26014,13 +26272,13 @@
     </row>
     <row r="3" spans="1:18" ht="174" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>506</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>502</v>
@@ -26070,13 +26328,13 @@
     </row>
     <row r="4" spans="1:18" ht="145" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>508</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>503</v>
@@ -26126,13 +26384,13 @@
     </row>
     <row r="5" spans="1:18" ht="174" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>509</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>504</v>
@@ -26182,13 +26440,13 @@
     </row>
     <row r="6" spans="1:18" ht="174" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>510</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>505</v>
@@ -26267,7 +26525,7 @@
         <v>569</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>3</v>
@@ -26317,13 +26575,13 @@
     </row>
     <row r="2" spans="1:18" ht="120.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="36" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B2" s="36" t="s">
         <v>202</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="D2" s="36" t="s">
         <v>551</v>
@@ -26373,13 +26631,13 @@
     </row>
     <row r="3" spans="1:18" ht="147.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="36" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="B3" s="36" t="s">
         <v>202</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D3" s="36" t="s">
         <v>560</v>
@@ -26429,13 +26687,13 @@
     </row>
     <row r="4" spans="1:18" ht="80.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="36" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B4" s="36" t="s">
         <v>242</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="D4" s="36" t="s">
         <v>562</v>
@@ -26511,7 +26769,7 @@
         <v>569</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>3</v>
@@ -26555,13 +26813,13 @@
     </row>
     <row r="2" spans="1:25" ht="115.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="30" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="B2" s="30" t="s">
         <v>209</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>566</v>
@@ -26614,13 +26872,13 @@
     </row>
     <row r="3" spans="1:25" ht="110.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="30" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="B3" s="30" t="s">
         <v>249</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="D3" s="30" t="s">
         <v>361</v>
@@ -26704,7 +26962,7 @@
         <v>569</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D1" s="20" t="s">
         <v>2</v>
@@ -26763,13 +27021,13 @@
     </row>
     <row r="2" spans="1:21" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="31" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="B2" s="31" t="s">
         <v>211</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="D2" s="31" t="s">
         <v>371</v>
@@ -26828,13 +27086,13 @@
     </row>
     <row r="3" spans="1:21" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="31" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B3" s="31" t="s">
         <v>230</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="D3" s="31" t="s">
         <v>371</v>
@@ -26893,13 +27151,13 @@
     </row>
     <row r="4" spans="1:21" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="31" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B4" s="31" t="s">
         <v>235</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="D4" s="31" t="s">
         <v>371</v>
@@ -26958,16 +27216,16 @@
     </row>
     <row r="5" spans="1:21" ht="96.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="18" t="s">
+        <v>767</v>
+      </c>
+      <c r="B5" s="29" t="s">
         <v>768</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="C5" s="31" t="s">
         <v>769</v>
       </c>
-      <c r="C5" s="31" t="s">
-        <v>770</v>
-      </c>
       <c r="D5" s="29" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="E5" s="29" t="s">
         <v>362</v>
@@ -27023,13 +27281,13 @@
     </row>
     <row r="6" spans="1:21" ht="94.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="18" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="B6" s="29" t="s">
         <v>251</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="D6" s="29" t="s">
         <v>380</v>
@@ -27309,13 +27567,13 @@
     </row>
     <row r="2" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="30" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B2" s="30" t="s">
         <v>172</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="D2" s="30" t="s">
         <v>174</v>
@@ -27353,13 +27611,13 @@
     </row>
     <row r="3" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="30" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B3" s="30" t="s">
         <v>175</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="D3" s="30" t="s">
         <v>177</v>
@@ -27397,13 +27655,13 @@
     </row>
     <row r="4" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="30" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B4" s="30" t="s">
         <v>178</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="D4" s="30" t="s">
         <v>180</v>
@@ -27441,13 +27699,13 @@
     </row>
     <row r="5" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="30" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B5" s="30" t="s">
         <v>181</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="D5" s="30" t="s">
         <v>357</v>
@@ -27485,13 +27743,13 @@
     </row>
     <row r="6" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="30" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B6" s="34" t="s">
         <v>182</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="D6" s="30" t="s">
         <v>358</v>
@@ -27529,13 +27787,13 @@
     </row>
     <row r="7" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="30" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B7" s="30" t="s">
         <v>184</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="D7" s="30" t="s">
         <v>186</v>
@@ -27573,13 +27831,13 @@
     </row>
     <row r="8" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="30" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B8" s="30" t="s">
         <v>187</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="D8" s="30" t="s">
         <v>188</v>
@@ -27617,13 +27875,13 @@
     </row>
     <row r="9" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="30" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B9" s="30" t="s">
         <v>191</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="D9" s="30" t="s">
         <v>359</v>
@@ -27661,13 +27919,13 @@
     </row>
     <row r="10" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="30" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B10" s="30" t="s">
         <v>193</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="D10" s="30" t="s">
         <v>360</v>
@@ -27705,13 +27963,13 @@
     </row>
     <row r="11" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="30" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="B11" s="30" t="s">
         <v>200</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="D11" s="30" t="s">
         <v>364</v>
@@ -27750,13 +28008,13 @@
     </row>
     <row r="12" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="30" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B12" s="30" t="s">
         <v>206</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D12" s="30" t="s">
         <v>367</v>
@@ -27795,13 +28053,13 @@
     </row>
     <row r="13" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="30" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="B13" s="30" t="s">
         <v>219</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="D13" s="30" t="s">
         <v>375</v>
@@ -27839,13 +28097,13 @@
     </row>
     <row r="14" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="30" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="B14" s="30" t="s">
         <v>221</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="D14" s="30" t="s">
         <v>376</v>
@@ -27883,13 +28141,13 @@
     </row>
     <row r="15" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="30" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B15" s="30" t="s">
         <v>223</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="D15" s="30" t="s">
         <v>364</v>
@@ -27927,13 +28185,13 @@
     </row>
     <row r="16" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="30" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B16" s="30" t="s">
         <v>225</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="D16" s="30" t="s">
         <v>364</v>
@@ -27971,13 +28229,13 @@
     </row>
     <row r="17" spans="1:14" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="30" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B17" s="30" t="s">
         <v>227</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="D17" s="30" t="s">
         <v>364</v>
@@ -28128,7 +28386,7 @@
         <v>569</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>3</v>
@@ -28172,13 +28430,13 @@
     </row>
     <row r="2" spans="1:16" ht="50.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="45" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="B2" s="45" t="s">
         <v>205</v>
       </c>
       <c r="C2" s="45" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="D2" s="45" t="s">
         <v>364</v>
@@ -28222,13 +28480,13 @@
     </row>
     <row r="3" spans="1:16" ht="113" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="45" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="B3" s="45" t="s">
         <v>545</v>
       </c>
       <c r="C3" s="45" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="D3" s="45" t="s">
         <v>547</v>
@@ -28252,13 +28510,13 @@
     </row>
     <row r="4" spans="1:16" ht="50.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="45" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B4" s="45" t="s">
         <v>544</v>
       </c>
       <c r="C4" s="45" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="D4" s="45" t="s">
         <v>364</v>
@@ -28302,13 +28560,13 @@
     </row>
     <row r="5" spans="1:16" ht="145.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="45" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="B5" s="45" t="s">
         <v>546</v>
       </c>
       <c r="C5" s="45" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>547</v>

</xml_diff>